<commit_message>
add new Forms . Implemented adding new values to the table
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71559B2-21A1-47C6-A4AC-91308CAE88AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EF1A40-AEAE-4C11-B5CF-A783E0F2BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32535" yWindow="2940" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -112,13 +112,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;₴&quot;_-;\-* #,##0\ &quot;₴&quot;_-;_-* &quot;-&quot;\ &quot;₴&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;₴&quot;_-;\-* #,##0.00\ &quot;₴&quot;_-;_-* &quot;-&quot;??\ &quot;₴&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;₴&quot;_-;\-* #,##0.00\ &quot;₴&quot;_-;_-* &quot;-&quot;??\ &quot;₴&quot;_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0\ &quot;₴&quot;_-;\-* #,##0\ &quot;₴&quot;_-;_-* &quot;-&quot;\ &quot;₴&quot;_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00&quot;₴&quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00&quot;₴&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +273,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -575,8 +581,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -620,7 +626,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -659,63 +665,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
-    <cellStyle name="20% – колірна тема 1" xfId="24" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 2" xfId="28" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 3" xfId="32" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 4" xfId="36" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 5" xfId="40" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 6" xfId="44" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 1" xfId="25" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 2" xfId="29" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 3" xfId="33" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 4" xfId="37" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 5" xfId="41" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 6" xfId="45" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 1" xfId="26" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 2" xfId="30" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 3" xfId="34" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 4" xfId="38" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 5" xfId="42" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 6" xfId="46" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Ввід" xfId="14" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Відсотковий" xfId="5" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Гарний" xfId="11" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Грошовий" xfId="3" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Грошовий [0]" xfId="4" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="24" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="28" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="32" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="36" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="40" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="44" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="25" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="29" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="33" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="37" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="41" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="45" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="26" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="30" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="34" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="38" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="42" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="46" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="23" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="27" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="31" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="35" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="39" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="43" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="14" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="15" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Денежный" xfId="3" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Денежный [0]" xfId="4" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Заголовок 1" xfId="7" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Заголовок 2" xfId="8" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Заголовок 3" xfId="9" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Заголовок 4" xfId="10" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Звичайний" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Зв'язана клітинка" xfId="17" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 1" xfId="23" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 2" xfId="27" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 3" xfId="31" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 4" xfId="35" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 5" xfId="39" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 6" xfId="43" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Контрольна клітинка" xfId="18" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Назва" xfId="6" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральний" xfId="13" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обчислення" xfId="16" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Підсумок" xfId="22" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Поганий" xfId="12" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Примітка" xfId="20" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Результат" xfId="15" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Текст попередження" xfId="19" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Текст пояснення" xfId="21" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Фінансовий" xfId="1" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Фінансовий [0]" xfId="2" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="22" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="18" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="6" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="13" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Плохой" xfId="12" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="21" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="20" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Процентный" xfId="5" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="17" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="19" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Финансовый" xfId="1" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Финансовый [0]" xfId="2" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="11" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -751,19 +782,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -931,7 +949,7 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="#,##0.00&quot;₴&quot;"/>
+      <numFmt numFmtId="166" formatCode="#,##0.00&quot;₴&quot;"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1000,7 +1018,7 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="168" formatCode="#,##0.00&quot;₴&quot;"/>
+      <numFmt numFmtId="166" formatCode="#,##0.00&quot;₴&quot;"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1397,8 +1415,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M6" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="B3:M6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M36" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="B3:M36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="25" totalsRowDxfId="24">
       <calculatedColumnFormula>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</calculatedColumnFormula>
@@ -1415,7 +1433,7 @@
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Інтервал поповнення в днях" dataDxfId="9" totalsRowDxfId="8"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Кількість для поповнення" dataDxfId="7" totalsRowDxfId="6"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Вилучено?" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{161F85EE-351B-4E90-B245-0F800118DEC0}" name="Група" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{161F85EE-351B-4E90-B245-0F800118DEC0}" name="Група" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Таблиця показників організації" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1624,10 +1642,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M6"/>
+  <dimension ref="B1:M36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" activeCellId="5" sqref="C7 E7 D7 F7 M7 I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1709,7 +1727,7 @@
       <c r="L3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1819,13 +1837,612 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
     </row>
+    <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="19"/>
+    </row>
+    <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="19"/>
+    </row>
+    <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="19"/>
+    </row>
+    <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="19"/>
+    </row>
+    <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="19"/>
+    </row>
+    <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="19"/>
+    </row>
+    <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="19"/>
+    </row>
+    <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="19"/>
+    </row>
+    <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="19"/>
+    </row>
+    <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="19"/>
+    </row>
+    <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="19"/>
+    </row>
+    <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="19"/>
+    </row>
+    <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="16"/>
+      <c r="M34" s="19"/>
+    </row>
+    <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="16"/>
+      <c r="M35" s="19"/>
+    </row>
+    <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="15">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="17">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="16"/>
+      <c r="M36" s="19"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B4:M6">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="B4:M36">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$L4="Так"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$B4=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1875,7 +2492,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B4:B6</xm:sqref>
+          <xm:sqref>B4:B36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1884,12 +2501,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2101,20 +2718,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2140,9 +2755,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix creating a new product in the table
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EF1A40-AEAE-4C11-B5CF-A783E0F2BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E8BCDF-DECF-4E5C-ABE0-E492381993B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32535" yWindow="2940" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -41,22 +41,7 @@
     <t>Ідентифікатор товару</t>
   </si>
   <si>
-    <t>IN0001</t>
-  </si>
-  <si>
-    <t>IN0002</t>
-  </si>
-  <si>
-    <t>IN0003</t>
-  </si>
-  <si>
     <t>Назва</t>
-  </si>
-  <si>
-    <t>Товар 1</t>
-  </si>
-  <si>
-    <t>Товар 3</t>
   </si>
   <si>
     <t>Ціна за одиницю</t>
@@ -92,19 +77,16 @@
     <t>Постачальник</t>
   </si>
   <si>
-    <t>Постачальник1</t>
+    <t>Група</t>
   </si>
   <si>
-    <t>Постачальник2</t>
+    <t>sad</t>
   </si>
   <si>
-    <t>Постачальник3</t>
+    <t>asd</t>
   </si>
   <si>
-    <t>Товар 2</t>
-  </si>
-  <si>
-    <t>Група</t>
+    <t>Item 1</t>
   </si>
 </sst>
 </file>
@@ -626,7 +608,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -654,16 +636,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
@@ -679,9 +655,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1415,8 +1388,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M36" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="B3:M36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M37" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="B3:M37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="25" totalsRowDxfId="24">
       <calculatedColumnFormula>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</calculatedColumnFormula>
@@ -1642,27 +1615,27 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M36"/>
+  <dimension ref="B1:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" activeCellId="5" sqref="C7 E7 D7 F7 M7 I7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="6" customWidth="1"/>
-    <col min="4" max="5" width="16.77734375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="15" style="8" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" style="8" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="1.77734375"/>
+    <col min="2" max="2" customWidth="true" style="3" width="11.5546875"/>
+    <col min="3" max="3" customWidth="true" style="6" width="12.77734375"/>
+    <col min="4" max="5" customWidth="true" style="6" width="16.77734375"/>
+    <col min="6" max="6" customWidth="true" style="8" width="13.109375"/>
+    <col min="7" max="7" customWidth="true" style="8" width="12.33203125"/>
+    <col min="8" max="8" customWidth="true" style="8" width="11.44140625"/>
+    <col min="9" max="9" customWidth="true" style="8" width="15.0"/>
+    <col min="10" max="10" customWidth="true" style="8" width="11.88671875"/>
+    <col min="11" max="11" customWidth="true" style="8" width="14.77734375"/>
+    <col min="12" max="12" customWidth="true" style="6" width="12.77734375"/>
+    <col min="13" max="13" customWidth="true" style="4" width="12.5546875"/>
+    <col min="14" max="16384" style="4" width="8.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1674,23 +1647,19 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="M1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>15</v>
+      <c r="G2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:13" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1701,34 +1670,34 @@
         <v>1</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1736,709 +1705,679 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="14">
-        <v>51</v>
-      </c>
-      <c r="G4" s="8">
-        <v>25</v>
-      </c>
-      <c r="H4" s="14">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>1275</v>
-      </c>
-      <c r="I4" s="8">
-        <v>29</v>
-      </c>
-      <c r="J4" s="8">
-        <v>13</v>
-      </c>
-      <c r="K4" s="8">
-        <v>50</v>
-      </c>
-      <c r="M4" s="6"/>
+      <c r="C4" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="12" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="H4" s="12">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="14">
-        <v>93</v>
-      </c>
-      <c r="G5" s="8">
-        <v>132</v>
-      </c>
-      <c r="H5" s="14">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>12276</v>
-      </c>
-      <c r="I5" s="8">
-        <v>231</v>
-      </c>
-      <c r="J5" s="8">
-        <v>4</v>
-      </c>
-      <c r="K5" s="8">
-        <v>50</v>
-      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="12"/>
+      <c r="H5" s="12">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="8"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="14">
-        <v>57</v>
-      </c>
-      <c r="G6" s="8">
-        <v>151</v>
-      </c>
-      <c r="H6" s="14">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>8607</v>
-      </c>
-      <c r="I6" s="8">
-        <v>114</v>
-      </c>
-      <c r="J6" s="8">
-        <v>11</v>
-      </c>
-      <c r="K6" s="8">
-        <v>150</v>
+        <v>1</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="H6" s="12">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
       </c>
       <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
+      <c r="M6" s="6"/>
     </row>
     <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="8"/>
+      <c r="B7" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="6"/>
     </row>
     <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="8"/>
+      <c r="B8" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="6"/>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="8"/>
+      <c r="B9" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="6"/>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="8"/>
+      <c r="B10" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="8"/>
+      <c r="B11" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="8"/>
+      <c r="B12" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="8"/>
+      <c r="B13" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="8"/>
+      <c r="B14" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="6"/>
     </row>
     <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="8"/>
+      <c r="B15" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="6"/>
     </row>
     <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="8"/>
+      <c r="B16" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="6"/>
     </row>
     <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="16"/>
-      <c r="M17" s="8"/>
+      <c r="B17" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="6"/>
     </row>
     <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="19"/>
+      <c r="B18" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="6"/>
     </row>
     <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="19"/>
+      <c r="B19" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="6"/>
     </row>
     <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="16"/>
-      <c r="M20" s="19"/>
+      <c r="B20" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="6"/>
     </row>
     <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="19"/>
+      <c r="B21" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="6"/>
     </row>
     <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="19"/>
+      <c r="B22" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="6"/>
     </row>
     <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="19"/>
+      <c r="B23" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="6"/>
     </row>
     <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="19"/>
+      <c r="B24" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="6"/>
     </row>
     <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="16"/>
-      <c r="M25" s="19"/>
+      <c r="B25" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="6"/>
     </row>
     <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="19"/>
+      <c r="B26" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="6"/>
     </row>
     <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="19"/>
+      <c r="B27" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="6"/>
     </row>
     <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="19"/>
+      <c r="B28" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="6"/>
     </row>
     <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="19"/>
+      <c r="B29" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="6"/>
     </row>
     <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="19"/>
+      <c r="B30" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="6"/>
     </row>
     <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="19"/>
+      <c r="B31" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="6"/>
     </row>
     <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="19"/>
+      <c r="B32" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="6"/>
     </row>
     <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="17"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="19"/>
+      <c r="B33" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="6"/>
     </row>
     <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="19"/>
+      <c r="B34" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="6"/>
     </row>
     <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="19"/>
+      <c r="B35" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="6"/>
     </row>
     <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="15">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="17">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="19"/>
+      <c r="B36" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="2:13" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="B37" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B4:M36">
+  <conditionalFormatting sqref="B4:M37">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$L4="Так"</formula>
     </cfRule>
@@ -2458,7 +2397,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці кількість кожного товару на складі" sqref="G3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці ціну за одиницю кожного товару" sqref="F3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці опис товару" sqref="E3" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:M5" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L5" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Так"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Щоб почати виділення елементів перевпорядкування, виберіть «Так». Після цього в стовпці B з’являтиметься позначка, а весь відповідний рядок виділятиметься кольором у таблиці «Список запасів». Якщо вибрати «Ні», позначки та виділення повністю прибираються." sqref="L2" xr:uid="{00000000-0002-0000-0000-00000D000000}">
@@ -2492,7 +2431,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B4:B36</xm:sqref>
+          <xm:sqref>B4:B37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
bug fix + add Names + IDs to config.json
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E8BCDF-DECF-4E5C-ABE0-E492381993B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63CCF5A-987D-4F09-AE0A-E2596E70A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -78,15 +78,6 @@
   </si>
   <si>
     <t>Група</t>
-  </si>
-  <si>
-    <t>sad</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>Item 1</t>
   </si>
 </sst>
 </file>
@@ -608,7 +599,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -655,6 +646,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -1365,21 +1359,6 @@
             <a:t>Інвентарний список</a:t>
           </a:r>
         </a:p>
-        <a:p>
-          <a:pPr marL="0" algn="l" rtl="0"/>
-          <a:r>
-            <a:rPr lang="uk" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="tx2">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Franklin Gothic Book" panose="020B0503020102020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Назва компанії</a:t>
-          </a:r>
-        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -1388,8 +1367,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M37" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="B3:M37" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M100" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="B3:M100" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="25" totalsRowDxfId="24">
       <calculatedColumnFormula>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</calculatedColumnFormula>
@@ -1615,27 +1594,27 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M37"/>
+  <dimension ref="B1:M100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="I4" sqref="I4:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="1.77734375"/>
-    <col min="2" max="2" customWidth="true" style="3" width="11.5546875"/>
-    <col min="3" max="3" customWidth="true" style="6" width="12.77734375"/>
-    <col min="4" max="5" customWidth="true" style="6" width="16.77734375"/>
-    <col min="6" max="6" customWidth="true" style="8" width="13.109375"/>
-    <col min="7" max="7" customWidth="true" style="8" width="12.33203125"/>
-    <col min="8" max="8" customWidth="true" style="8" width="11.44140625"/>
-    <col min="9" max="9" customWidth="true" style="8" width="15.0"/>
-    <col min="10" max="10" customWidth="true" style="8" width="11.88671875"/>
-    <col min="11" max="11" customWidth="true" style="8" width="14.77734375"/>
-    <col min="12" max="12" customWidth="true" style="6" width="12.77734375"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.5546875"/>
-    <col min="14" max="16384" style="4" width="8.77734375"/>
+    <col min="1" max="1" width="1.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="6" customWidth="1"/>
+    <col min="4" max="5" width="16.77734375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="15" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,42 +1684,23 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="12" t="n">
-        <v>123.0</v>
-      </c>
+      <c r="F4" s="12"/>
       <c r="H4" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I4" t="n">
-        <v>123.0</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="M4" s="6"/>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
       <c r="F5" s="12"/>
       <c r="H5" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I5" s="8"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1748,15 +1708,18 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
+      <c r="D6"/>
+      <c r="E6"/>
       <c r="F6" s="12"/>
       <c r="H6" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
+      <c r="I6"/>
       <c r="L6" s="8"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
@@ -1774,7 +1737,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="6"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
@@ -1794,13 +1757,14 @@
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="15"/>
@@ -1813,7 +1777,7 @@
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="6"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
@@ -1833,7 +1797,7 @@
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="6"/>
+      <c r="M10" s="17"/>
     </row>
     <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
@@ -1853,7 +1817,7 @@
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="6"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
@@ -1873,7 +1837,7 @@
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
       <c r="L12" s="14"/>
-      <c r="M12" s="6"/>
+      <c r="M12" s="17"/>
     </row>
     <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
@@ -1893,7 +1857,7 @@
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
       <c r="L13" s="14"/>
-      <c r="M13" s="6"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
@@ -1913,7 +1877,7 @@
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
       <c r="L14" s="14"/>
-      <c r="M14" s="6"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
@@ -1933,7 +1897,7 @@
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
       <c r="L15" s="14"/>
-      <c r="M15" s="6"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
@@ -1953,7 +1917,7 @@
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
       <c r="L16" s="14"/>
-      <c r="M16" s="6"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
@@ -1973,7 +1937,7 @@
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="14"/>
-      <c r="M17" s="6"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
@@ -1993,7 +1957,7 @@
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
       <c r="L18" s="14"/>
-      <c r="M18" s="6"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
@@ -2013,7 +1977,7 @@
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
       <c r="L19" s="14"/>
-      <c r="M19" s="6"/>
+      <c r="M19" s="17"/>
     </row>
     <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
@@ -2033,7 +1997,7 @@
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
       <c r="L20" s="14"/>
-      <c r="M20" s="6"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
@@ -2053,7 +2017,7 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
       <c r="L21" s="14"/>
-      <c r="M21" s="6"/>
+      <c r="M21" s="17"/>
     </row>
     <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
@@ -2073,7 +2037,7 @@
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
       <c r="L22" s="14"/>
-      <c r="M22" s="6"/>
+      <c r="M22" s="17"/>
     </row>
     <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
@@ -2093,7 +2057,7 @@
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="6"/>
+      <c r="M23" s="17"/>
     </row>
     <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
@@ -2113,7 +2077,7 @@
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
       <c r="L24" s="14"/>
-      <c r="M24" s="6"/>
+      <c r="M24" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
@@ -2133,7 +2097,7 @@
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
       <c r="L25" s="14"/>
-      <c r="M25" s="6"/>
+      <c r="M25" s="17"/>
     </row>
     <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
@@ -2153,7 +2117,7 @@
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
       <c r="L26" s="14"/>
-      <c r="M26" s="6"/>
+      <c r="M26" s="17"/>
     </row>
     <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
@@ -2173,7 +2137,7 @@
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
       <c r="L27" s="14"/>
-      <c r="M27" s="6"/>
+      <c r="M27" s="17"/>
     </row>
     <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13">
@@ -2193,7 +2157,7 @@
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
       <c r="L28" s="14"/>
-      <c r="M28" s="6"/>
+      <c r="M28" s="17"/>
     </row>
     <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
@@ -2213,7 +2177,7 @@
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
       <c r="L29" s="14"/>
-      <c r="M29" s="6"/>
+      <c r="M29" s="17"/>
     </row>
     <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
@@ -2233,7 +2197,7 @@
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
       <c r="L30" s="14"/>
-      <c r="M30" s="6"/>
+      <c r="M30" s="17"/>
     </row>
     <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="13">
@@ -2253,7 +2217,7 @@
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
       <c r="L31" s="14"/>
-      <c r="M31" s="6"/>
+      <c r="M31" s="17"/>
     </row>
     <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
@@ -2273,7 +2237,7 @@
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
       <c r="L32" s="14"/>
-      <c r="M32" s="6"/>
+      <c r="M32" s="17"/>
     </row>
     <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="13">
@@ -2293,7 +2257,7 @@
       <c r="J33" s="16"/>
       <c r="K33" s="16"/>
       <c r="L33" s="14"/>
-      <c r="M33" s="6"/>
+      <c r="M33" s="17"/>
     </row>
     <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="13">
@@ -2313,7 +2277,7 @@
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
       <c r="L34" s="14"/>
-      <c r="M34" s="6"/>
+      <c r="M34" s="17"/>
     </row>
     <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="13">
@@ -2333,7 +2297,7 @@
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
       <c r="L35" s="14"/>
-      <c r="M35" s="6"/>
+      <c r="M35" s="17"/>
     </row>
     <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="13">
@@ -2353,9 +2317,9 @@
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
       <c r="L36" s="14"/>
-      <c r="M36" s="6"/>
-    </row>
-    <row r="37" spans="2:13" ht="13.5" x14ac:dyDescent="0.3">
+      <c r="M36" s="17"/>
+    </row>
+    <row r="37" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="13">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
@@ -2373,11 +2337,1271 @@
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
       <c r="L37" s="14"/>
-      <c r="M37" s="6"/>
+      <c r="M37" s="17"/>
+    </row>
+    <row r="38" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="14"/>
+      <c r="M38" s="17"/>
+    </row>
+    <row r="39" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="16"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="17"/>
+    </row>
+    <row r="40" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="14"/>
+      <c r="M40" s="17"/>
+    </row>
+    <row r="41" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I41" s="16"/>
+      <c r="J41" s="16"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="17"/>
+    </row>
+    <row r="42" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="16"/>
+      <c r="H42" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+      <c r="K42" s="16"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="17"/>
+    </row>
+    <row r="43" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="17"/>
+    </row>
+    <row r="44" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="16"/>
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="14"/>
+      <c r="M44" s="17"/>
+    </row>
+    <row r="45" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="16"/>
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="17"/>
+    </row>
+    <row r="46" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="14"/>
+      <c r="M46" s="17"/>
+    </row>
+    <row r="47" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="17"/>
+    </row>
+    <row r="48" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="14"/>
+      <c r="M48" s="17"/>
+    </row>
+    <row r="49" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="17"/>
+    </row>
+    <row r="50" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="14"/>
+      <c r="M50" s="17"/>
+    </row>
+    <row r="51" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="17"/>
+    </row>
+    <row r="52" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="17"/>
+    </row>
+    <row r="53" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="17"/>
+    </row>
+    <row r="54" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I54" s="16"/>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="17"/>
+    </row>
+    <row r="55" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="17"/>
+    </row>
+    <row r="56" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="16"/>
+      <c r="L56" s="14"/>
+      <c r="M56" s="17"/>
+    </row>
+    <row r="57" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I57" s="16"/>
+      <c r="J57" s="16"/>
+      <c r="K57" s="16"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="17"/>
+    </row>
+    <row r="58" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I58" s="16"/>
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="14"/>
+      <c r="M58" s="17"/>
+    </row>
+    <row r="59" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="17"/>
+    </row>
+    <row r="60" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="17"/>
+    </row>
+    <row r="61" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I61" s="16"/>
+      <c r="J61" s="16"/>
+      <c r="K61" s="16"/>
+      <c r="L61" s="14"/>
+      <c r="M61" s="17"/>
+    </row>
+    <row r="62" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="16"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="17"/>
+    </row>
+    <row r="63" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="17"/>
+    </row>
+    <row r="64" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="14"/>
+      <c r="M64" s="17"/>
+    </row>
+    <row r="65" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I65" s="16"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="17"/>
+    </row>
+    <row r="66" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="16"/>
+      <c r="J66" s="16"/>
+      <c r="K66" s="16"/>
+      <c r="L66" s="14"/>
+      <c r="M66" s="17"/>
+    </row>
+    <row r="67" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I67" s="16"/>
+      <c r="J67" s="16"/>
+      <c r="K67" s="16"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="17"/>
+    </row>
+    <row r="68" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
+      <c r="K68" s="16"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="17"/>
+    </row>
+    <row r="69" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="16"/>
+      <c r="L69" s="14"/>
+      <c r="M69" s="17"/>
+    </row>
+    <row r="70" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I70" s="16"/>
+      <c r="J70" s="16"/>
+      <c r="K70" s="16"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="17"/>
+    </row>
+    <row r="71" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I71" s="16"/>
+      <c r="J71" s="16"/>
+      <c r="K71" s="16"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="17"/>
+    </row>
+    <row r="72" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="16"/>
+      <c r="H72" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I72" s="16"/>
+      <c r="J72" s="16"/>
+      <c r="K72" s="16"/>
+      <c r="L72" s="14"/>
+      <c r="M72" s="17"/>
+    </row>
+    <row r="73" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="17"/>
+    </row>
+    <row r="74" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
+      <c r="L74" s="14"/>
+      <c r="M74" s="17"/>
+    </row>
+    <row r="75" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I75" s="16"/>
+      <c r="J75" s="16"/>
+      <c r="K75" s="16"/>
+      <c r="L75" s="14"/>
+      <c r="M75" s="17"/>
+    </row>
+    <row r="76" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I76" s="16"/>
+      <c r="J76" s="16"/>
+      <c r="K76" s="16"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="17"/>
+    </row>
+    <row r="77" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C77" s="14"/>
+      <c r="D77" s="14"/>
+      <c r="E77" s="14"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="16"/>
+      <c r="H77" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I77" s="16"/>
+      <c r="J77" s="16"/>
+      <c r="K77" s="16"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="17"/>
+    </row>
+    <row r="78" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I78" s="16"/>
+      <c r="J78" s="16"/>
+      <c r="K78" s="16"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="17"/>
+    </row>
+    <row r="79" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C79" s="14"/>
+      <c r="D79" s="14"/>
+      <c r="E79" s="14"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16"/>
+      <c r="K79" s="16"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="17"/>
+    </row>
+    <row r="80" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C80" s="14"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="14"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I80" s="16"/>
+      <c r="J80" s="16"/>
+      <c r="K80" s="16"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="17"/>
+    </row>
+    <row r="81" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="17"/>
+    </row>
+    <row r="82" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="17"/>
+    </row>
+    <row r="83" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16"/>
+      <c r="K83" s="16"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="17"/>
+    </row>
+    <row r="84" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I84" s="16"/>
+      <c r="J84" s="16"/>
+      <c r="K84" s="16"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="17"/>
+    </row>
+    <row r="85" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16"/>
+      <c r="K85" s="16"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="17"/>
+    </row>
+    <row r="86" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I86" s="16"/>
+      <c r="J86" s="16"/>
+      <c r="K86" s="16"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="17"/>
+    </row>
+    <row r="87" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I87" s="16"/>
+      <c r="J87" s="16"/>
+      <c r="K87" s="16"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="17"/>
+    </row>
+    <row r="88" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I88" s="16"/>
+      <c r="J88" s="16"/>
+      <c r="K88" s="16"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="17"/>
+    </row>
+    <row r="89" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I89" s="16"/>
+      <c r="J89" s="16"/>
+      <c r="K89" s="16"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="17"/>
+    </row>
+    <row r="90" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I90" s="16"/>
+      <c r="J90" s="16"/>
+      <c r="K90" s="16"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="17"/>
+    </row>
+    <row r="91" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I91" s="16"/>
+      <c r="J91" s="16"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="17"/>
+    </row>
+    <row r="92" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B92" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="16"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="17"/>
+    </row>
+    <row r="93" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I93" s="16"/>
+      <c r="J93" s="16"/>
+      <c r="K93" s="16"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="17"/>
+    </row>
+    <row r="94" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="16"/>
+      <c r="H94" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I94" s="16"/>
+      <c r="J94" s="16"/>
+      <c r="K94" s="16"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="17"/>
+    </row>
+    <row r="95" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B95" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I95" s="16"/>
+      <c r="J95" s="16"/>
+      <c r="K95" s="16"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="17"/>
+    </row>
+    <row r="96" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B96" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="16"/>
+      <c r="L96" s="14"/>
+      <c r="M96" s="17"/>
+    </row>
+    <row r="97" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I97" s="16"/>
+      <c r="J97" s="16"/>
+      <c r="K97" s="16"/>
+      <c r="L97" s="14"/>
+      <c r="M97" s="17"/>
+    </row>
+    <row r="98" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I98" s="16"/>
+      <c r="J98" s="16"/>
+      <c r="K98" s="16"/>
+      <c r="L98" s="14"/>
+      <c r="M98" s="17"/>
+    </row>
+    <row r="99" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B99" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I99" s="16"/>
+      <c r="J99" s="16"/>
+      <c r="K99" s="16"/>
+      <c r="L99" s="14"/>
+      <c r="M99" s="17"/>
+    </row>
+    <row r="100" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B100" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="16"/>
+      <c r="H100" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I100" s="16"/>
+      <c r="J100" s="16"/>
+      <c r="K100" s="16"/>
+      <c r="L100" s="14"/>
+      <c r="M100" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B4:M37">
+  <conditionalFormatting sqref="B4:M100">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$L4="Так"</formula>
     </cfRule>
@@ -2431,7 +3655,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B4:B37</xm:sqref>
+          <xm:sqref>B4:B100</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2440,12 +3664,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2657,18 +3881,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2694,11 +3920,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
small fix + add JDateChooser
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -78,6 +78,30 @@
   </si>
   <si>
     <t>Група</t>
+  </si>
+  <si>
+    <t>In0001</t>
+  </si>
+  <si>
+    <t>Tovar</t>
+  </si>
+  <si>
+    <t>Item 1</t>
+  </si>
+  <si>
+    <t>Item 2</t>
+  </si>
+  <si>
+    <t>In0002</t>
+  </si>
+  <si>
+    <t>Tovar1</t>
+  </si>
+  <si>
+    <t>In0003</t>
+  </si>
+  <si>
+    <t>Tovar2</t>
   </si>
 </sst>
 </file>
@@ -1602,19 +1626,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="6" customWidth="1"/>
-    <col min="4" max="5" width="16.77734375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="15" style="8" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" style="8" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="1.77734375"/>
+    <col min="2" max="2" customWidth="true" style="3" width="11.5546875"/>
+    <col min="3" max="3" customWidth="true" style="6" width="12.77734375"/>
+    <col min="4" max="5" customWidth="true" style="6" width="16.77734375"/>
+    <col min="6" max="6" customWidth="true" style="8" width="13.109375"/>
+    <col min="7" max="7" customWidth="true" style="8" width="12.33203125"/>
+    <col min="8" max="8" customWidth="true" style="8" width="11.44140625"/>
+    <col min="9" max="9" customWidth="true" style="8" width="15.0"/>
+    <col min="10" max="10" customWidth="true" style="8" width="11.88671875"/>
+    <col min="11" max="11" customWidth="true" style="8" width="14.77734375"/>
+    <col min="12" max="12" customWidth="true" style="6" width="12.77734375"/>
+    <col min="13" max="13" customWidth="true" style="4" width="12.5546875"/>
+    <col min="14" max="16384" style="4" width="8.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1684,40 +1708,85 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="12"/>
+      <c r="C4" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s" s="6">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s" s="6">
+        <v>17</v>
+      </c>
+      <c r="F4" s="12" t="n">
+        <v>33.0</v>
+      </c>
       <c r="H4" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="M4" s="6"/>
+      <c r="I4" t="n" s="8">
+        <v>200.0</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="C5" t="s" s="6">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>18</v>
+      </c>
+      <c r="F5" s="12" t="n">
+        <v>34.0</v>
+      </c>
       <c r="H5" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="I5" t="n" s="8">
+        <v>20.0</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6" s="12"/>
+      <c r="C6" t="s" s="6">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="12" t="n">
+        <v>123.0</v>
+      </c>
       <c r="H6" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I6"/>
+      <c r="I6" s="8" t="n">
+        <v>132.0</v>
+      </c>
       <c r="L6" s="8"/>
-      <c r="M6" s="6"/>
+      <c r="M6" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13">

</xml_diff>

<commit_message>
Add supplier / Group logic
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63CCF5A-987D-4F09-AE0A-E2596E70A9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310D0C06-A8C0-44CB-944B-15474718D0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30570" yWindow="1125" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -80,28 +80,34 @@
     <t>Група</t>
   </si>
   <si>
-    <t>In0001</t>
+    <t>Id01</t>
   </si>
   <si>
-    <t>Tovar</t>
+    <t>Tovar01</t>
   </si>
   <si>
-    <t>Item 1</t>
+    <t>Sup1</t>
   </si>
   <si>
-    <t>Item 2</t>
+    <t>Group2</t>
   </si>
   <si>
-    <t>In0002</t>
+    <t>Id02</t>
   </si>
   <si>
-    <t>Tovar1</t>
+    <t>Tovar02</t>
   </si>
   <si>
-    <t>In0003</t>
+    <t>Sup2</t>
   </si>
   <si>
-    <t>Tovar2</t>
+    <t>Group1</t>
+  </si>
+  <si>
+    <t>Id03</t>
+  </si>
+  <si>
+    <t>Tovar03</t>
   </si>
 </sst>
 </file>
@@ -1621,7 +1627,7 @@
   <dimension ref="B1:M100"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:M6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1718,14 +1724,17 @@
         <v>17</v>
       </c>
       <c r="F4" s="12" t="n">
-        <v>33.0</v>
+        <v>40.0</v>
       </c>
       <c r="H4" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
       <c r="I4" t="n" s="8">
-        <v>200.0</v>
+        <v>32.0</v>
+      </c>
+      <c r="J4" t="n" s="8">
+        <v>20.0</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>18</v>
@@ -1743,20 +1752,23 @@
         <v>20</v>
       </c>
       <c r="E5" t="s" s="6">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F5" s="12" t="n">
-        <v>34.0</v>
+        <v>22.0</v>
       </c>
       <c r="H5" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
       <c r="I5" t="n" s="8">
-        <v>20.0</v>
+        <v>32.0</v>
+      </c>
+      <c r="J5" t="n" s="8">
+        <v>14.0</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1765,27 +1777,30 @@
         <v>1</v>
       </c>
       <c r="C6" t="s" s="6">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>17</v>
-      </c>
       <c r="F6" s="12" t="n">
-        <v>123.0</v>
+        <v>43.0</v>
       </c>
       <c r="H6" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I6" s="8" t="n">
-        <v>132.0</v>
+      <c r="I6" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>55.0</v>
       </c>
       <c r="L6" s="8"/>
       <c r="M6" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3733,12 +3748,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3950,20 +3965,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3989,9 +4002,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding the product to the warehouse + small fix
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43B65FB-46A0-4EDE-9601-75B52F42F987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490C0C39-3828-4E35-B6C7-ABE7DC26635B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30570" yWindow="1125" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -80,46 +80,40 @@
     <t>Група</t>
   </si>
   <si>
-    <t>Id01</t>
-  </si>
-  <si>
-    <t>tov1</t>
-  </si>
-  <si>
     <t>Sup1</t>
   </si>
   <si>
     <t>Group1</t>
   </si>
   <si>
-    <t>Id02</t>
+    <t>a</t>
   </si>
   <si>
-    <t>tov2</t>
+    <t>b</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>bb</t>
   </si>
   <si>
     <t>Sup2</t>
   </si>
   <si>
-    <t>Id03</t>
+    <t>aaa</t>
   </si>
   <si>
-    <t>tov3</t>
-  </si>
-  <si>
-    <t>Id04</t>
-  </si>
-  <si>
-    <t>tov4</t>
+    <t>bbb</t>
   </si>
   <si>
     <t>Group2</t>
   </si>
   <si>
-    <t>tov01</t>
+    <t>aaaa</t>
   </si>
   <si>
-    <t>tov02</t>
+    <t>bbbb</t>
   </si>
 </sst>
 </file>
@@ -641,7 +635,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -691,6 +685,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -993,6 +990,7 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1409,8 +1407,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M100" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="B3:M100" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M99" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="B3:M99" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="25" totalsRowDxfId="24">
       <calculatedColumnFormula>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</calculatedColumnFormula>
@@ -1636,27 +1634,27 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M100"/>
+  <dimension ref="B1:M101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="1.77734375"/>
-    <col min="2" max="2" customWidth="true" style="3" width="11.5546875"/>
-    <col min="3" max="3" customWidth="true" style="6" width="12.77734375"/>
-    <col min="4" max="5" customWidth="true" style="6" width="16.77734375"/>
-    <col min="6" max="6" customWidth="true" style="8" width="13.109375"/>
-    <col min="7" max="7" customWidth="true" style="8" width="12.33203125"/>
-    <col min="8" max="8" customWidth="true" style="8" width="11.44140625"/>
-    <col min="9" max="9" customWidth="true" style="8" width="15.0"/>
-    <col min="10" max="10" customWidth="true" style="8" width="11.88671875"/>
-    <col min="11" max="11" customWidth="true" style="8" width="14.77734375"/>
-    <col min="12" max="12" customWidth="true" style="6" width="12.77734375"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.5546875"/>
-    <col min="14" max="16384" style="4" width="8.77734375"/>
+    <col min="1" max="1" width="1.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" style="6" customWidth="1"/>
+    <col min="4" max="5" width="16.77734375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="15" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" style="8" customWidth="1"/>
+    <col min="11" max="11" width="14.77734375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1726,30 +1724,33 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C4" t="s" s="6">
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="6">
+      <c r="F4" s="12">
+        <v>12</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="8">
+        <v>32</v>
+      </c>
+      <c r="J4" s="8">
+        <v>21</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="F4" s="12" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="H4" s="12">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I4" t="n" s="8">
-        <v>34.0</v>
-      </c>
-      <c r="J4" t="n" s="8">
-        <v>20.0</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1757,62 +1758,70 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C5" t="s" s="6">
+      <c r="C5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s" s="6">
+      <c r="D5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s" s="6">
+      <c r="E5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="12" t="n">
-        <v>22.0</v>
+      <c r="F5" s="12">
+        <v>132</v>
+      </c>
+      <c r="G5" s="18">
+        <v>0</v>
       </c>
       <c r="H5" s="12">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I5" t="n" s="8">
-        <v>43.0</v>
-      </c>
-      <c r="J5" t="n" s="8">
-        <v>25.0</v>
-      </c>
+      <c r="I5" s="8">
+        <v>132</v>
+      </c>
+      <c r="J5" s="8">
+        <v>33</v>
+      </c>
+      <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="3">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" t="s" s="6">
+      <c r="B6" s="13">
+        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="12" t="n">
-        <v>312.0</v>
-      </c>
-      <c r="H6" s="12">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="J6" s="8" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="6" t="s">
-        <v>18</v>
+      <c r="E6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="15">
+        <v>32</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15">
+        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="16">
+        <v>42</v>
+      </c>
+      <c r="J6" s="16">
+        <v>12</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="17" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1821,32 +1830,34 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="15" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="G7" s="16"/>
+        <v>15</v>
+      </c>
+      <c r="F7" s="15">
+        <v>312</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0</v>
+      </c>
       <c r="H7" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I7" s="16" t="n">
-        <v>43.0</v>
-      </c>
-      <c r="J7" s="16" t="n">
-        <v>25.0</v>
+      <c r="I7" s="16">
+        <v>231</v>
+      </c>
+      <c r="J7" s="16">
+        <v>321</v>
       </c>
       <c r="K7" s="16"/>
       <c r="L7" s="14"/>
       <c r="M7" s="17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1854,136 +1865,88 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="15" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="G8" s="16"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="18">
+        <v>0</v>
+      </c>
       <c r="H8" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I8" s="16" t="n">
-        <v>312.0</v>
-      </c>
-      <c r="J8" s="16" t="n">
-        <v>33.0</v>
-      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
       <c r="K8" s="16"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="17" t="s">
-        <v>18</v>
-      </c>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="15" t="n">
-        <v>61.0</v>
-      </c>
-      <c r="G9" s="16"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="18">
+        <v>0</v>
+      </c>
       <c r="H9" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I9" s="16" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="J9" s="16" t="n">
-        <v>10.0</v>
-      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="17" t="s">
-        <v>18</v>
-      </c>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="15" t="n">
-        <v>55.0</v>
-      </c>
-      <c r="G10" s="16"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="18">
+        <v>0</v>
+      </c>
       <c r="H10" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I10" s="16" t="n">
-        <v>132.0</v>
-      </c>
-      <c r="J10" s="16" t="n">
-        <v>7.0</v>
-      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="16"/>
       <c r="L10" s="14"/>
-      <c r="M10" s="17" t="s">
-        <v>18</v>
-      </c>
+      <c r="M10" s="17"/>
     </row>
     <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="15" t="n">
-        <v>32.0</v>
-      </c>
-      <c r="G11" s="16"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="18">
+        <v>0</v>
+      </c>
       <c r="H11" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I11" s="16" t="n">
-        <v>88.0</v>
-      </c>
-      <c r="J11" s="16" t="n">
-        <v>8.0</v>
-      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
       <c r="K11" s="16"/>
       <c r="L11" s="14"/>
-      <c r="M11" s="17" t="s">
-        <v>26</v>
-      </c>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
@@ -1994,7 +1957,9 @@
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
+      <c r="G12" s="18">
+        <v>0</v>
+      </c>
       <c r="H12" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2014,7 +1979,9 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="G13" s="18">
+        <v>0</v>
+      </c>
       <c r="H13" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2034,7 +2001,9 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
+      <c r="G14" s="18">
+        <v>0</v>
+      </c>
       <c r="H14" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2054,7 +2023,9 @@
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="18">
+        <v>0</v>
+      </c>
       <c r="H15" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2074,7 +2045,9 @@
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
+      <c r="G16" s="18">
+        <v>0</v>
+      </c>
       <c r="H16" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2094,7 +2067,9 @@
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="18">
+        <v>0</v>
+      </c>
       <c r="H17" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2114,7 +2089,9 @@
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
+      <c r="G18" s="18">
+        <v>0</v>
+      </c>
       <c r="H18" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2134,7 +2111,9 @@
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
       <c r="H19" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2154,7 +2133,9 @@
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
+      <c r="G20" s="18">
+        <v>0</v>
+      </c>
       <c r="H20" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2174,7 +2155,9 @@
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
+      <c r="G21" s="18">
+        <v>0</v>
+      </c>
       <c r="H21" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2194,7 +2177,9 @@
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
       <c r="H22" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2214,7 +2199,9 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
+      <c r="G23" s="18">
+        <v>0</v>
+      </c>
       <c r="H23" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2234,7 +2221,9 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
+      <c r="G24" s="18">
+        <v>0</v>
+      </c>
       <c r="H24" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2254,7 +2243,9 @@
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
+      <c r="G25" s="18">
+        <v>0</v>
+      </c>
       <c r="H25" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2274,7 +2265,9 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
+      <c r="G26" s="18">
+        <v>0</v>
+      </c>
       <c r="H26" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2294,7 +2287,9 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
+      <c r="G27" s="18">
+        <v>0</v>
+      </c>
       <c r="H27" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2314,7 +2309,9 @@
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
+      <c r="G28" s="18">
+        <v>0</v>
+      </c>
       <c r="H28" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2334,7 +2331,9 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
+      <c r="G29" s="18">
+        <v>0</v>
+      </c>
       <c r="H29" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2354,7 +2353,9 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="16"/>
+      <c r="G30" s="18">
+        <v>0</v>
+      </c>
       <c r="H30" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2374,7 +2375,9 @@
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
+      <c r="G31" s="18">
+        <v>0</v>
+      </c>
       <c r="H31" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2394,7 +2397,9 @@
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
+      <c r="G32" s="18">
+        <v>0</v>
+      </c>
       <c r="H32" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2414,7 +2419,9 @@
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
+      <c r="G33" s="18">
+        <v>0</v>
+      </c>
       <c r="H33" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2434,7 +2441,9 @@
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
+      <c r="G34" s="18">
+        <v>0</v>
+      </c>
       <c r="H34" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2454,7 +2463,9 @@
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
+      <c r="G35" s="18">
+        <v>0</v>
+      </c>
       <c r="H35" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2474,7 +2485,9 @@
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
+      <c r="G36" s="18">
+        <v>0</v>
+      </c>
       <c r="H36" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2494,7 +2507,9 @@
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
+      <c r="G37" s="18">
+        <v>0</v>
+      </c>
       <c r="H37" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2514,7 +2529,9 @@
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
+      <c r="G38" s="18">
+        <v>0</v>
+      </c>
       <c r="H38" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2534,7 +2551,9 @@
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="15"/>
-      <c r="G39" s="16"/>
+      <c r="G39" s="18">
+        <v>0</v>
+      </c>
       <c r="H39" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2554,7 +2573,9 @@
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="15"/>
-      <c r="G40" s="16"/>
+      <c r="G40" s="18">
+        <v>0</v>
+      </c>
       <c r="H40" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2574,7 +2595,9 @@
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="15"/>
-      <c r="G41" s="16"/>
+      <c r="G41" s="18">
+        <v>0</v>
+      </c>
       <c r="H41" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2594,7 +2617,9 @@
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="15"/>
-      <c r="G42" s="16"/>
+      <c r="G42" s="18">
+        <v>0</v>
+      </c>
       <c r="H42" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2614,7 +2639,9 @@
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="16"/>
+      <c r="G43" s="18">
+        <v>0</v>
+      </c>
       <c r="H43" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2634,7 +2661,9 @@
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="15"/>
-      <c r="G44" s="16"/>
+      <c r="G44" s="18">
+        <v>0</v>
+      </c>
       <c r="H44" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2654,7 +2683,9 @@
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="15"/>
-      <c r="G45" s="16"/>
+      <c r="G45" s="18">
+        <v>0</v>
+      </c>
       <c r="H45" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2674,7 +2705,9 @@
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="15"/>
-      <c r="G46" s="16"/>
+      <c r="G46" s="18">
+        <v>0</v>
+      </c>
       <c r="H46" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2694,7 +2727,9 @@
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="15"/>
-      <c r="G47" s="16"/>
+      <c r="G47" s="18">
+        <v>0</v>
+      </c>
       <c r="H47" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2714,7 +2749,9 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="15"/>
-      <c r="G48" s="16"/>
+      <c r="G48" s="18">
+        <v>0</v>
+      </c>
       <c r="H48" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2734,7 +2771,9 @@
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="15"/>
-      <c r="G49" s="16"/>
+      <c r="G49" s="18">
+        <v>0</v>
+      </c>
       <c r="H49" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2754,7 +2793,9 @@
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="15"/>
-      <c r="G50" s="16"/>
+      <c r="G50" s="18">
+        <v>0</v>
+      </c>
       <c r="H50" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2774,7 +2815,9 @@
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="15"/>
-      <c r="G51" s="16"/>
+      <c r="G51" s="18">
+        <v>0</v>
+      </c>
       <c r="H51" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2794,7 +2837,9 @@
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="15"/>
-      <c r="G52" s="16"/>
+      <c r="G52" s="18">
+        <v>0</v>
+      </c>
       <c r="H52" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2814,7 +2859,9 @@
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="15"/>
-      <c r="G53" s="16"/>
+      <c r="G53" s="18">
+        <v>0</v>
+      </c>
       <c r="H53" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2834,7 +2881,9 @@
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
+      <c r="G54" s="18">
+        <v>0</v>
+      </c>
       <c r="H54" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2854,7 +2903,9 @@
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="15"/>
-      <c r="G55" s="16"/>
+      <c r="G55" s="18">
+        <v>0</v>
+      </c>
       <c r="H55" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2874,7 +2925,9 @@
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="15"/>
-      <c r="G56" s="16"/>
+      <c r="G56" s="18">
+        <v>0</v>
+      </c>
       <c r="H56" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2894,7 +2947,9 @@
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="15"/>
-      <c r="G57" s="16"/>
+      <c r="G57" s="18">
+        <v>0</v>
+      </c>
       <c r="H57" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2914,7 +2969,9 @@
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="15"/>
-      <c r="G58" s="16"/>
+      <c r="G58" s="18">
+        <v>0</v>
+      </c>
       <c r="H58" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2934,7 +2991,9 @@
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="15"/>
-      <c r="G59" s="16"/>
+      <c r="G59" s="18">
+        <v>0</v>
+      </c>
       <c r="H59" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2954,7 +3013,9 @@
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="15"/>
-      <c r="G60" s="16"/>
+      <c r="G60" s="18">
+        <v>0</v>
+      </c>
       <c r="H60" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2974,7 +3035,9 @@
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="15"/>
-      <c r="G61" s="16"/>
+      <c r="G61" s="18">
+        <v>0</v>
+      </c>
       <c r="H61" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -2994,7 +3057,9 @@
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="15"/>
-      <c r="G62" s="16"/>
+      <c r="G62" s="18">
+        <v>0</v>
+      </c>
       <c r="H62" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3014,7 +3079,9 @@
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="15"/>
-      <c r="G63" s="16"/>
+      <c r="G63" s="18">
+        <v>0</v>
+      </c>
       <c r="H63" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3034,7 +3101,9 @@
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="15"/>
-      <c r="G64" s="16"/>
+      <c r="G64" s="18">
+        <v>0</v>
+      </c>
       <c r="H64" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3054,7 +3123,9 @@
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
       <c r="F65" s="15"/>
-      <c r="G65" s="16"/>
+      <c r="G65" s="18">
+        <v>0</v>
+      </c>
       <c r="H65" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3074,7 +3145,9 @@
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="15"/>
-      <c r="G66" s="16"/>
+      <c r="G66" s="18">
+        <v>0</v>
+      </c>
       <c r="H66" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3094,7 +3167,9 @@
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="15"/>
-      <c r="G67" s="16"/>
+      <c r="G67" s="18">
+        <v>0</v>
+      </c>
       <c r="H67" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3114,7 +3189,9 @@
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="15"/>
-      <c r="G68" s="16"/>
+      <c r="G68" s="18">
+        <v>0</v>
+      </c>
       <c r="H68" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3134,7 +3211,9 @@
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="15"/>
-      <c r="G69" s="16"/>
+      <c r="G69" s="18">
+        <v>0</v>
+      </c>
       <c r="H69" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3154,7 +3233,9 @@
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="15"/>
-      <c r="G70" s="16"/>
+      <c r="G70" s="18">
+        <v>0</v>
+      </c>
       <c r="H70" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3174,7 +3255,9 @@
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="15"/>
-      <c r="G71" s="16"/>
+      <c r="G71" s="18">
+        <v>0</v>
+      </c>
       <c r="H71" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3194,7 +3277,9 @@
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="15"/>
-      <c r="G72" s="16"/>
+      <c r="G72" s="18">
+        <v>0</v>
+      </c>
       <c r="H72" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3214,7 +3299,9 @@
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="15"/>
-      <c r="G73" s="16"/>
+      <c r="G73" s="18">
+        <v>0</v>
+      </c>
       <c r="H73" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3234,7 +3321,9 @@
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="15"/>
-      <c r="G74" s="16"/>
+      <c r="G74" s="18">
+        <v>0</v>
+      </c>
       <c r="H74" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3254,7 +3343,9 @@
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="15"/>
-      <c r="G75" s="16"/>
+      <c r="G75" s="18">
+        <v>0</v>
+      </c>
       <c r="H75" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3274,7 +3365,9 @@
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="15"/>
-      <c r="G76" s="16"/>
+      <c r="G76" s="18">
+        <v>0</v>
+      </c>
       <c r="H76" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3294,7 +3387,9 @@
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="15"/>
-      <c r="G77" s="16"/>
+      <c r="G77" s="18">
+        <v>0</v>
+      </c>
       <c r="H77" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3314,7 +3409,9 @@
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="15"/>
-      <c r="G78" s="16"/>
+      <c r="G78" s="18">
+        <v>0</v>
+      </c>
       <c r="H78" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3334,7 +3431,9 @@
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="15"/>
-      <c r="G79" s="16"/>
+      <c r="G79" s="18">
+        <v>0</v>
+      </c>
       <c r="H79" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3354,7 +3453,9 @@
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="15"/>
-      <c r="G80" s="16"/>
+      <c r="G80" s="18">
+        <v>0</v>
+      </c>
       <c r="H80" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3374,7 +3475,9 @@
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
       <c r="F81" s="15"/>
-      <c r="G81" s="16"/>
+      <c r="G81" s="18">
+        <v>0</v>
+      </c>
       <c r="H81" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3394,7 +3497,9 @@
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="15"/>
-      <c r="G82" s="16"/>
+      <c r="G82" s="18">
+        <v>0</v>
+      </c>
       <c r="H82" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3414,7 +3519,9 @@
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
       <c r="F83" s="15"/>
-      <c r="G83" s="16"/>
+      <c r="G83" s="18">
+        <v>0</v>
+      </c>
       <c r="H83" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3434,7 +3541,9 @@
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
       <c r="F84" s="15"/>
-      <c r="G84" s="16"/>
+      <c r="G84" s="18">
+        <v>0</v>
+      </c>
       <c r="H84" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3454,7 +3563,9 @@
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="15"/>
-      <c r="G85" s="16"/>
+      <c r="G85" s="18">
+        <v>0</v>
+      </c>
       <c r="H85" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3474,7 +3585,9 @@
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="15"/>
-      <c r="G86" s="16"/>
+      <c r="G86" s="18">
+        <v>0</v>
+      </c>
       <c r="H86" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3494,7 +3607,9 @@
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
       <c r="F87" s="15"/>
-      <c r="G87" s="16"/>
+      <c r="G87" s="18">
+        <v>0</v>
+      </c>
       <c r="H87" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3514,7 +3629,9 @@
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="15"/>
-      <c r="G88" s="16"/>
+      <c r="G88" s="18">
+        <v>0</v>
+      </c>
       <c r="H88" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3534,7 +3651,9 @@
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="15"/>
-      <c r="G89" s="16"/>
+      <c r="G89" s="18">
+        <v>0</v>
+      </c>
       <c r="H89" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3554,7 +3673,9 @@
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
       <c r="F90" s="15"/>
-      <c r="G90" s="16"/>
+      <c r="G90" s="18">
+        <v>0</v>
+      </c>
       <c r="H90" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3574,7 +3695,9 @@
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="15"/>
-      <c r="G91" s="16"/>
+      <c r="G91" s="18">
+        <v>0</v>
+      </c>
       <c r="H91" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3594,7 +3717,9 @@
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
       <c r="F92" s="15"/>
-      <c r="G92" s="16"/>
+      <c r="G92" s="18">
+        <v>0</v>
+      </c>
       <c r="H92" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3614,7 +3739,9 @@
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="15"/>
-      <c r="G93" s="16"/>
+      <c r="G93" s="18">
+        <v>0</v>
+      </c>
       <c r="H93" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3634,7 +3761,9 @@
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="15"/>
-      <c r="G94" s="16"/>
+      <c r="G94" s="18">
+        <v>0</v>
+      </c>
       <c r="H94" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3654,7 +3783,9 @@
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
       <c r="F95" s="15"/>
-      <c r="G95" s="16"/>
+      <c r="G95" s="18">
+        <v>0</v>
+      </c>
       <c r="H95" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3674,7 +3805,9 @@
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="15"/>
-      <c r="G96" s="16"/>
+      <c r="G96" s="18">
+        <v>0</v>
+      </c>
       <c r="H96" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3694,7 +3827,9 @@
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="15"/>
-      <c r="G97" s="16"/>
+      <c r="G97" s="18">
+        <v>0</v>
+      </c>
       <c r="H97" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3714,7 +3849,9 @@
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="15"/>
-      <c r="G98" s="16"/>
+      <c r="G98" s="18">
+        <v>0</v>
+      </c>
       <c r="H98" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3734,7 +3871,9 @@
       <c r="D99" s="14"/>
       <c r="E99" s="14"/>
       <c r="F99" s="15"/>
-      <c r="G99" s="16"/>
+      <c r="G99" s="18">
+        <v>0</v>
+      </c>
       <c r="H99" s="15">
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
@@ -3746,28 +3885,34 @@
       <c r="M99" s="17"/>
     </row>
     <row r="100" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="13">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
+      <c r="B100" s="13"/>
       <c r="C100" s="14"/>
       <c r="D100" s="14"/>
       <c r="E100" s="14"/>
       <c r="F100" s="15"/>
-      <c r="G100" s="16"/>
-      <c r="H100" s="15">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
-        <v>0</v>
-      </c>
+      <c r="H100" s="15"/>
       <c r="I100" s="16"/>
       <c r="J100" s="16"/>
       <c r="K100" s="16"/>
       <c r="L100" s="14"/>
       <c r="M100" s="17"/>
     </row>
+    <row r="101" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="13"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="15"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="16"/>
+      <c r="J101" s="16"/>
+      <c r="K101" s="16"/>
+      <c r="L101" s="14"/>
+      <c r="M101" s="17"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B4:M100">
+  <conditionalFormatting sqref="B4:M99 G100:G101">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$L4="Так"</formula>
     </cfRule>
@@ -3787,13 +3932,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці кількість кожного товару на складі" sqref="G3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці ціну за одиницю кожного товару" sqref="F3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці опис товару" sqref="E3" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L5" xr:uid="{00000000-0002-0000-0000-00000C000000}">
-      <formula1>"Так"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Щоб почати виділення елементів перевпорядкування, виберіть «Так». Після цього в стовпці B з’являтиметься позначка, а весь відповідний рядок виділятиметься кольором у таблиці «Список запасів». Якщо вибрати «Ні», позначки та виділення повністю прибираються." sqref="L2" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"Так, Ні"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Інвентарний список" prompt="Цей аркуш відстежує запаси товарів у таблиці та дає можливість виділити й позначити товари, чиї запаси слід поповнити. Якщо товар вилучено, текст у його рядку закреслюється, а в стовпці &quot;Вилучено&quot; з’являється напис &quot;Так&quot;." sqref="A1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+      <formula1>"Так"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -3805,7 +3950,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{22614FA3-6814-43BC-85E4-CF5B29361B41}">
+          <x14:cfRule type="iconSet" priority="7" id="{22614FA3-6814-43BC-85E4-CF5B29361B41}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3821,7 +3966,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B4:B100</xm:sqref>
+          <xm:sqref>B4:B99</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3830,12 +3975,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4047,20 +4192,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4086,9 +4229,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adding completed, + small fix
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -17,7 +17,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>bbbb</t>
+  </si>
+  <si>
+    <t>In0005</t>
+  </si>
+  <si>
+    <t>Tov5</t>
+  </si>
+  <si>
+    <t>Sup3</t>
+  </si>
+  <si>
+    <t>Group3</t>
+  </si>
+  <si>
+    <t>In0006</t>
+  </si>
+  <si>
+    <t>Tov6</t>
   </si>
 </sst>
 </file>
@@ -1642,19 +1660,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="6" customWidth="1"/>
-    <col min="4" max="5" width="16.77734375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="15" style="8" customWidth="1"/>
-    <col min="10" max="10" width="11.88671875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" style="8" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="8.77734375" style="4"/>
+    <col min="1" max="1" customWidth="true" style="4" width="1.77734375"/>
+    <col min="2" max="2" customWidth="true" style="3" width="11.5546875"/>
+    <col min="3" max="3" customWidth="true" style="6" width="12.77734375"/>
+    <col min="4" max="5" customWidth="true" style="6" width="16.77734375"/>
+    <col min="6" max="6" customWidth="true" style="8" width="13.109375"/>
+    <col min="7" max="7" customWidth="true" style="8" width="12.33203125"/>
+    <col min="8" max="8" customWidth="true" style="8" width="11.44140625"/>
+    <col min="9" max="9" customWidth="true" style="8" width="15.0"/>
+    <col min="10" max="10" customWidth="true" style="8" width="11.88671875"/>
+    <col min="11" max="11" customWidth="true" style="8" width="14.77734375"/>
+    <col min="12" max="12" customWidth="true" style="6" width="12.77734375"/>
+    <col min="13" max="13" customWidth="true" style="4" width="12.5546875"/>
+    <col min="14" max="16384" style="4" width="8.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1865,10 +1883,18 @@
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
+      <c r="C8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="15" t="n">
+        <v>33.0</v>
+      </c>
       <c r="G8" s="18">
         <v>0</v>
       </c>
@@ -1876,21 +1902,35 @@
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
+      <c r="I8" s="16" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="J8" s="16" t="n">
+        <v>2.0</v>
+      </c>
       <c r="K8" s="16"/>
       <c r="L8" s="14"/>
-      <c r="M8" s="17"/>
+      <c r="M8" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
         <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
+      <c r="C9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="15" t="n">
+        <v>33.0</v>
+      </c>
       <c r="G9" s="18">
         <v>0</v>
       </c>
@@ -1898,11 +1938,17 @@
         <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
         <v>0</v>
       </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
+      <c r="I9" s="16" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="J9" s="16" t="n">
+        <v>44.0</v>
+      </c>
       <c r="K9" s="16"/>
       <c r="L9" s="14"/>
-      <c r="M9" s="17"/>
+      <c r="M9" s="17" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13">

</xml_diff>

<commit_message>
add Delete Group,DeleteItemForm fix
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6ECDDE-CEB0-455C-B35E-58345D07FB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D540E2-E876-4EE4-969E-390B9FEEC88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="555" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30480" yWindow="1785" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -80,10 +80,10 @@
     <t>Група</t>
   </si>
   <si>
-    <t>a</t>
+    <t>q1</t>
   </si>
   <si>
-    <t>b</t>
+    <t>t1</t>
   </si>
   <si>
     <t>Sup1</t>
@@ -92,22 +92,25 @@
     <t>Group1</t>
   </si>
   <si>
-    <t>aa</t>
+    <t>q2</t>
   </si>
   <si>
-    <t>bb</t>
+    <t>t2</t>
   </si>
   <si>
-    <t>aaa</t>
+    <t>Group2</t>
   </si>
   <si>
-    <t>bbb</t>
+    <t>q3</t>
   </si>
   <si>
-    <t>aaaaa</t>
+    <t>Group3</t>
   </si>
   <si>
-    <t>bbbbb</t>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>t4</t>
   </si>
 </sst>
 </file>
@@ -629,7 +632,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -679,9 +682,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -984,7 +984,6 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1401,8 +1400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M99" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="B3:M99" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M100" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="B3:M100" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="25" totalsRowDxfId="24">
       <calculatedColumnFormula>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</calculatedColumnFormula>
@@ -1628,10 +1627,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M97"/>
+  <dimension ref="B1:M98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:M6"/>
+      <selection activeCell="C4" sqref="C4:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1715,123 +1714,99 @@
     </row>
     <row r="4" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G4:G4&lt;=InventoryList!I4:I4)*(InventoryList!L4:L4="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="12" t="n">
-        <v>132.0</v>
-      </c>
-      <c r="G4" s="18">
-        <v>0</v>
+        <v>1.0</v>
       </c>
       <c r="H4" s="12">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <f>(InventoryList!F4:F4*InventoryList!G4:G4)</f>
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>132.0</v>
+        <v>1.0</v>
       </c>
       <c r="J4" t="n">
-        <v>132.0</v>
+        <v>1.0</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
-        <f>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G5:G5&lt;=InventoryList!I5:I5)*(InventoryList!L5:L5="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="12" t="n">
-        <v>132.0</v>
-      </c>
-      <c r="G5" s="18">
-        <v>0</v>
+        <v>1.0</v>
       </c>
       <c r="H5" s="12">
-        <f>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</f>
+        <f>(InventoryList!F5:F5*InventoryList!G5:G5)</f>
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>132.0</v>
+        <v>1.0</v>
       </c>
       <c r="J5" t="n">
-        <v>312.0</v>
+        <v>1.0</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
-        <f>IFERROR((InventoryList!#REF!&lt;=InventoryList!#REF!)*(InventoryList!#REF!="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="15" t="n">
-        <v>312.0</v>
-      </c>
-      <c r="G6" s="18">
-        <v>0</v>
-      </c>
+        <f>ЕСЛИОШИБКА((InventoryList!G6:G6&lt;=InventoryList!I6:I6)*(InventoryList!L6:L6="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="15">
-        <f>InventoryList!#REF!*InventoryList!#REF!</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="16" t="n">
-        <v>6516.0</v>
-      </c>
-      <c r="J6" s="16" t="n">
-        <v>561.0</v>
-      </c>
+        <f>(InventoryList!F6:F6*InventoryList!G6:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
       <c r="K6" s="16"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="17" t="s">
-        <v>18</v>
-      </c>
+      <c r="M6" s="17"/>
     </row>
     <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
-        <f>IFERROR((InventoryList!G6:G6&lt;=InventoryList!I6:I6)*(InventoryList!L6:L6="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G7:G7&lt;=InventoryList!I7:I7)*(InventoryList!L7:L7="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
+      <c r="G7" s="16"/>
       <c r="H7" s="15">
-        <f>InventoryList!F6:F6*InventoryList!G6:G6</f>
+        <f>(InventoryList!F7:F7*InventoryList!G7:G7)</f>
         <v>0</v>
       </c>
       <c r="I7" s="16"/>
@@ -1842,18 +1817,16 @@
     </row>
     <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
-        <f>IFERROR((InventoryList!G7:G7&lt;=InventoryList!I7:I7)*(InventoryList!L7:L7="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G8:G8&lt;=InventoryList!I8:I8)*(InventoryList!L8:L8="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="18">
-        <v>0</v>
-      </c>
+      <c r="G8" s="16"/>
       <c r="H8" s="15">
-        <f>InventoryList!F7:F7*InventoryList!G7:G7</f>
+        <f>(InventoryList!F8:F8*InventoryList!G8:G8)</f>
         <v>0</v>
       </c>
       <c r="I8" s="16"/>
@@ -1864,18 +1837,16 @@
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
-        <f>IFERROR((InventoryList!G8:G8&lt;=InventoryList!I8:I8)*(InventoryList!L8:L8="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G9:G9&lt;=InventoryList!I9:I9)*(InventoryList!L9:L9="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="18">
-        <v>0</v>
-      </c>
+      <c r="G9" s="16"/>
       <c r="H9" s="15">
-        <f>InventoryList!F8:F8*InventoryList!G8:G8</f>
+        <f>(InventoryList!F9:F9*InventoryList!G9:G9)</f>
         <v>0</v>
       </c>
       <c r="I9" s="16"/>
@@ -1886,18 +1857,16 @@
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
-        <f>IFERROR((InventoryList!G9:G9&lt;=InventoryList!I9:I9)*(InventoryList!L9:L9="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G10:G10&lt;=InventoryList!I10:I10)*(InventoryList!L10:L10="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
+      <c r="G10" s="16"/>
       <c r="H10" s="15">
-        <f>InventoryList!F9:F9*InventoryList!G9:G9</f>
+        <f>(InventoryList!F10:F10*InventoryList!G10:G10)</f>
         <v>0</v>
       </c>
       <c r="I10" s="16"/>
@@ -1908,18 +1877,16 @@
     </row>
     <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
-        <f>IFERROR((InventoryList!G10:G10&lt;=InventoryList!I10:I10)*(InventoryList!L10:L10="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G11:G11&lt;=InventoryList!I11:I11)*(InventoryList!L11:L11="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
+      <c r="G11" s="16"/>
       <c r="H11" s="15">
-        <f>InventoryList!F10:F10*InventoryList!G10:G10</f>
+        <f>(InventoryList!F11:F11*InventoryList!G11:G11)</f>
         <v>0</v>
       </c>
       <c r="I11" s="16"/>
@@ -1930,18 +1897,16 @@
     </row>
     <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
-        <f>IFERROR((InventoryList!G11:G11&lt;=InventoryList!I11:I11)*(InventoryList!L11:L11="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G12:G12&lt;=InventoryList!I12:I12)*(InventoryList!L12:L12="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
+      <c r="G12" s="16"/>
       <c r="H12" s="15">
-        <f>InventoryList!F11:F11*InventoryList!G11:G11</f>
+        <f>(InventoryList!F12:F12*InventoryList!G12:G12)</f>
         <v>0</v>
       </c>
       <c r="I12" s="16"/>
@@ -1952,18 +1917,16 @@
     </row>
     <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
-        <f>IFERROR((InventoryList!G12:G12&lt;=InventoryList!I12:I12)*(InventoryList!L12:L12="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G13:G13&lt;=InventoryList!I13:I13)*(InventoryList!L13:L13="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="18">
-        <v>0</v>
-      </c>
+      <c r="G13" s="16"/>
       <c r="H13" s="15">
-        <f>InventoryList!F12:F12*InventoryList!G12:G12</f>
+        <f>(InventoryList!F13:F13*InventoryList!G13:G13)</f>
         <v>0</v>
       </c>
       <c r="I13" s="16"/>
@@ -1974,18 +1937,16 @@
     </row>
     <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
-        <f>IFERROR((InventoryList!G13:G13&lt;=InventoryList!I13:I13)*(InventoryList!L13:L13="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G14:G14&lt;=InventoryList!I14:I14)*(InventoryList!L14:L14="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="18">
-        <v>0</v>
-      </c>
+      <c r="G14" s="16"/>
       <c r="H14" s="15">
-        <f>InventoryList!F13:F13*InventoryList!G13:G13</f>
+        <f>(InventoryList!F14:F14*InventoryList!G14:G14)</f>
         <v>0</v>
       </c>
       <c r="I14" s="16"/>
@@ -1996,18 +1957,16 @@
     </row>
     <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
-        <f>IFERROR((InventoryList!G14:G14&lt;=InventoryList!I14:I14)*(InventoryList!L14:L14="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G15:G15&lt;=InventoryList!I15:I15)*(InventoryList!L15:L15="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
+      <c r="G15" s="16"/>
       <c r="H15" s="15">
-        <f>InventoryList!F14:F14*InventoryList!G14:G14</f>
+        <f>(InventoryList!F15:F15*InventoryList!G15:G15)</f>
         <v>0</v>
       </c>
       <c r="I15" s="16"/>
@@ -2018,18 +1977,16 @@
     </row>
     <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
-        <f>IFERROR((InventoryList!G15:G15&lt;=InventoryList!I15:I15)*(InventoryList!L15:L15="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G16:G16&lt;=InventoryList!I16:I16)*(InventoryList!L16:L16="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
+      <c r="G16" s="16"/>
       <c r="H16" s="15">
-        <f>InventoryList!F15:F15*InventoryList!G15:G15</f>
+        <f>(InventoryList!F16:F16*InventoryList!G16:G16)</f>
         <v>0</v>
       </c>
       <c r="I16" s="16"/>
@@ -2040,18 +1997,16 @@
     </row>
     <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
-        <f>IFERROR((InventoryList!G16:G16&lt;=InventoryList!I16:I16)*(InventoryList!L16:L16="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G17:G17&lt;=InventoryList!I17:I17)*(InventoryList!L17:L17="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="18">
-        <v>0</v>
-      </c>
+      <c r="G17" s="16"/>
       <c r="H17" s="15">
-        <f>InventoryList!F16:F16*InventoryList!G16:G16</f>
+        <f>(InventoryList!F17:F17*InventoryList!G17:G17)</f>
         <v>0</v>
       </c>
       <c r="I17" s="16"/>
@@ -2062,18 +2017,16 @@
     </row>
     <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
-        <f>IFERROR((InventoryList!G17:G17&lt;=InventoryList!I17:I17)*(InventoryList!L17:L17="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G18:G18&lt;=InventoryList!I18:I18)*(InventoryList!L18:L18="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="18">
-        <v>0</v>
-      </c>
+      <c r="G18" s="16"/>
       <c r="H18" s="15">
-        <f>InventoryList!F17:F17*InventoryList!G17:G17</f>
+        <f>(InventoryList!F18:F18*InventoryList!G18:G18)</f>
         <v>0</v>
       </c>
       <c r="I18" s="16"/>
@@ -2084,18 +2037,16 @@
     </row>
     <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
-        <f>IFERROR((InventoryList!G18:G18&lt;=InventoryList!I18:I18)*(InventoryList!L18:L18="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G19:G19&lt;=InventoryList!I19:I19)*(InventoryList!L19:L19="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
+      <c r="G19" s="16"/>
       <c r="H19" s="15">
-        <f>InventoryList!F18:F18*InventoryList!G18:G18</f>
+        <f>(InventoryList!F19:F19*InventoryList!G19:G19)</f>
         <v>0</v>
       </c>
       <c r="I19" s="16"/>
@@ -2106,18 +2057,16 @@
     </row>
     <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
-        <f>IFERROR((InventoryList!G19:G19&lt;=InventoryList!I19:I19)*(InventoryList!L19:L19="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G20:G20&lt;=InventoryList!I20:I20)*(InventoryList!L20:L20="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="18">
-        <v>0</v>
-      </c>
+      <c r="G20" s="16"/>
       <c r="H20" s="15">
-        <f>InventoryList!F19:F19*InventoryList!G19:G19</f>
+        <f>(InventoryList!F20:F20*InventoryList!G20:G20)</f>
         <v>0</v>
       </c>
       <c r="I20" s="16"/>
@@ -2128,18 +2077,16 @@
     </row>
     <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
-        <f>IFERROR((InventoryList!G20:G20&lt;=InventoryList!I20:I20)*(InventoryList!L20:L20="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G21:G21&lt;=InventoryList!I21:I21)*(InventoryList!L21:L21="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="18">
-        <v>0</v>
-      </c>
+      <c r="G21" s="16"/>
       <c r="H21" s="15">
-        <f>InventoryList!F20:F20*InventoryList!G20:G20</f>
+        <f>(InventoryList!F21:F21*InventoryList!G21:G21)</f>
         <v>0</v>
       </c>
       <c r="I21" s="16"/>
@@ -2150,18 +2097,16 @@
     </row>
     <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
-        <f>IFERROR((InventoryList!G21:G21&lt;=InventoryList!I21:I21)*(InventoryList!L21:L21="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G22:G22&lt;=InventoryList!I22:I22)*(InventoryList!L22:L22="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="18">
-        <v>0</v>
-      </c>
+      <c r="G22" s="16"/>
       <c r="H22" s="15">
-        <f>InventoryList!F21:F21*InventoryList!G21:G21</f>
+        <f>(InventoryList!F22:F22*InventoryList!G22:G22)</f>
         <v>0</v>
       </c>
       <c r="I22" s="16"/>
@@ -2172,18 +2117,16 @@
     </row>
     <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
-        <f>IFERROR((InventoryList!G22:G22&lt;=InventoryList!I22:I22)*(InventoryList!L22:L22="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G23:G23&lt;=InventoryList!I23:I23)*(InventoryList!L23:L23="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="18">
-        <v>0</v>
-      </c>
+      <c r="G23" s="16"/>
       <c r="H23" s="15">
-        <f>InventoryList!F22:F22*InventoryList!G22:G22</f>
+        <f>(InventoryList!F23:F23*InventoryList!G23:G23)</f>
         <v>0</v>
       </c>
       <c r="I23" s="16"/>
@@ -2194,18 +2137,16 @@
     </row>
     <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
-        <f>IFERROR((InventoryList!G23:G23&lt;=InventoryList!I23:I23)*(InventoryList!L23:L23="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G24:G24&lt;=InventoryList!I24:I24)*(InventoryList!L24:L24="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="18">
-        <v>0</v>
-      </c>
+      <c r="G24" s="16"/>
       <c r="H24" s="15">
-        <f>InventoryList!F23:F23*InventoryList!G23:G23</f>
+        <f>(InventoryList!F24:F24*InventoryList!G24:G24)</f>
         <v>0</v>
       </c>
       <c r="I24" s="16"/>
@@ -2216,18 +2157,16 @@
     </row>
     <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
-        <f>IFERROR((InventoryList!G24:G24&lt;=InventoryList!I24:I24)*(InventoryList!L24:L24="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G25:G25&lt;=InventoryList!I25:I25)*(InventoryList!L25:L25="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="18">
-        <v>0</v>
-      </c>
+      <c r="G25" s="16"/>
       <c r="H25" s="15">
-        <f>InventoryList!F24:F24*InventoryList!G24:G24</f>
+        <f>(InventoryList!F25:F25*InventoryList!G25:G25)</f>
         <v>0</v>
       </c>
       <c r="I25" s="16"/>
@@ -2238,18 +2177,16 @@
     </row>
     <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
-        <f>IFERROR((InventoryList!G25:G25&lt;=InventoryList!I25:I25)*(InventoryList!L25:L25="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G26:G26&lt;=InventoryList!I26:I26)*(InventoryList!L26:L26="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C26" s="14"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
+      <c r="G26" s="16"/>
       <c r="H26" s="15">
-        <f>InventoryList!F25:F25*InventoryList!G25:G25</f>
+        <f>(InventoryList!F26:F26*InventoryList!G26:G26)</f>
         <v>0</v>
       </c>
       <c r="I26" s="16"/>
@@ -2260,18 +2197,16 @@
     </row>
     <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
-        <f>IFERROR((InventoryList!G26:G26&lt;=InventoryList!I26:I26)*(InventoryList!L26:L26="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G27:G27&lt;=InventoryList!I27:I27)*(InventoryList!L27:L27="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="18">
-        <v>0</v>
-      </c>
+      <c r="G27" s="16"/>
       <c r="H27" s="15">
-        <f>InventoryList!F26:F26*InventoryList!G26:G26</f>
+        <f>(InventoryList!F27:F27*InventoryList!G27:G27)</f>
         <v>0</v>
       </c>
       <c r="I27" s="16"/>
@@ -2282,18 +2217,16 @@
     </row>
     <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13">
-        <f>IFERROR((InventoryList!G27:G27&lt;=InventoryList!I27:I27)*(InventoryList!L27:L27="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G28:G28&lt;=InventoryList!I28:I28)*(InventoryList!L28:L28="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="18">
-        <v>0</v>
-      </c>
+      <c r="G28" s="16"/>
       <c r="H28" s="15">
-        <f>InventoryList!F27:F27*InventoryList!G27:G27</f>
+        <f>(InventoryList!F28:F28*InventoryList!G28:G28)</f>
         <v>0</v>
       </c>
       <c r="I28" s="16"/>
@@ -2304,18 +2237,16 @@
     </row>
     <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
-        <f>IFERROR((InventoryList!G28:G28&lt;=InventoryList!I28:I28)*(InventoryList!L28:L28="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G29:G29&lt;=InventoryList!I29:I29)*(InventoryList!L29:L29="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C29" s="14"/>
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="18">
-        <v>0</v>
-      </c>
+      <c r="G29" s="16"/>
       <c r="H29" s="15">
-        <f>InventoryList!F28:F28*InventoryList!G28:G28</f>
+        <f>(InventoryList!F29:F29*InventoryList!G29:G29)</f>
         <v>0</v>
       </c>
       <c r="I29" s="16"/>
@@ -2326,18 +2257,16 @@
     </row>
     <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
-        <f>IFERROR((InventoryList!G29:G29&lt;=InventoryList!I29:I29)*(InventoryList!L29:L29="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G30:G30&lt;=InventoryList!I30:I30)*(InventoryList!L30:L30="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="18">
-        <v>0</v>
-      </c>
+      <c r="G30" s="16"/>
       <c r="H30" s="15">
-        <f>InventoryList!F29:F29*InventoryList!G29:G29</f>
+        <f>(InventoryList!F30:F30*InventoryList!G30:G30)</f>
         <v>0</v>
       </c>
       <c r="I30" s="16"/>
@@ -2348,18 +2277,16 @@
     </row>
     <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="13">
-        <f>IFERROR((InventoryList!G30:G30&lt;=InventoryList!I30:I30)*(InventoryList!L30:L30="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G31:G31&lt;=InventoryList!I31:I31)*(InventoryList!L31:L31="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="18">
-        <v>0</v>
-      </c>
+      <c r="G31" s="16"/>
       <c r="H31" s="15">
-        <f>InventoryList!F30:F30*InventoryList!G30:G30</f>
+        <f>(InventoryList!F31:F31*InventoryList!G31:G31)</f>
         <v>0</v>
       </c>
       <c r="I31" s="16"/>
@@ -2370,18 +2297,16 @@
     </row>
     <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
-        <f>IFERROR((InventoryList!G31:G31&lt;=InventoryList!I31:I31)*(InventoryList!L31:L31="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G32:G32&lt;=InventoryList!I32:I32)*(InventoryList!L32:L32="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="15"/>
-      <c r="G32" s="18">
-        <v>0</v>
-      </c>
+      <c r="G32" s="16"/>
       <c r="H32" s="15">
-        <f>InventoryList!F31:F31*InventoryList!G31:G31</f>
+        <f>(InventoryList!F32:F32*InventoryList!G32:G32)</f>
         <v>0</v>
       </c>
       <c r="I32" s="16"/>
@@ -2392,18 +2317,16 @@
     </row>
     <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="13">
-        <f>IFERROR((InventoryList!G32:G32&lt;=InventoryList!I32:I32)*(InventoryList!L32:L32="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G33:G33&lt;=InventoryList!I33:I33)*(InventoryList!L33:L33="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="15"/>
-      <c r="G33" s="18">
-        <v>0</v>
-      </c>
+      <c r="G33" s="16"/>
       <c r="H33" s="15">
-        <f>InventoryList!F32:F32*InventoryList!G32:G32</f>
+        <f>(InventoryList!F33:F33*InventoryList!G33:G33)</f>
         <v>0</v>
       </c>
       <c r="I33" s="16"/>
@@ -2414,18 +2337,16 @@
     </row>
     <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="13">
-        <f>IFERROR((InventoryList!G33:G33&lt;=InventoryList!I33:I33)*(InventoryList!L33:L33="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G34:G34&lt;=InventoryList!I34:I34)*(InventoryList!L34:L34="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C34" s="14"/>
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="18">
-        <v>0</v>
-      </c>
+      <c r="G34" s="16"/>
       <c r="H34" s="15">
-        <f>InventoryList!F33:F33*InventoryList!G33:G33</f>
+        <f>(InventoryList!F34:F34*InventoryList!G34:G34)</f>
         <v>0</v>
       </c>
       <c r="I34" s="16"/>
@@ -2436,18 +2357,16 @@
     </row>
     <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="13">
-        <f>IFERROR((InventoryList!G34:G34&lt;=InventoryList!I34:I34)*(InventoryList!L34:L34="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G35:G35&lt;=InventoryList!I35:I35)*(InventoryList!L35:L35="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="15"/>
-      <c r="G35" s="18">
-        <v>0</v>
-      </c>
+      <c r="G35" s="16"/>
       <c r="H35" s="15">
-        <f>InventoryList!F34:F34*InventoryList!G34:G34</f>
+        <f>(InventoryList!F35:F35*InventoryList!G35:G35)</f>
         <v>0</v>
       </c>
       <c r="I35" s="16"/>
@@ -2458,18 +2377,16 @@
     </row>
     <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="13">
-        <f>IFERROR((InventoryList!G35:G35&lt;=InventoryList!I35:I35)*(InventoryList!L35:L35="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G36:G36&lt;=InventoryList!I36:I36)*(InventoryList!L36:L36="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="15"/>
-      <c r="G36" s="18">
-        <v>0</v>
-      </c>
+      <c r="G36" s="16"/>
       <c r="H36" s="15">
-        <f>InventoryList!F35:F35*InventoryList!G35:G35</f>
+        <f>(InventoryList!F36:F36*InventoryList!G36:G36)</f>
         <v>0</v>
       </c>
       <c r="I36" s="16"/>
@@ -2480,18 +2397,16 @@
     </row>
     <row r="37" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="13">
-        <f>IFERROR((InventoryList!G36:G36&lt;=InventoryList!I36:I36)*(InventoryList!L36:L36="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G37:G37&lt;=InventoryList!I37:I37)*(InventoryList!L37:L37="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C37" s="14"/>
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="18">
-        <v>0</v>
-      </c>
+      <c r="G37" s="16"/>
       <c r="H37" s="15">
-        <f>InventoryList!F36:F36*InventoryList!G36:G36</f>
+        <f>(InventoryList!F37:F37*InventoryList!G37:G37)</f>
         <v>0</v>
       </c>
       <c r="I37" s="16"/>
@@ -2502,18 +2417,16 @@
     </row>
     <row r="38" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="13">
-        <f>IFERROR((InventoryList!G37:G37&lt;=InventoryList!I37:I37)*(InventoryList!L37:L37="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G38:G38&lt;=InventoryList!I38:I38)*(InventoryList!L38:L38="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="18">
-        <v>0</v>
-      </c>
+      <c r="G38" s="16"/>
       <c r="H38" s="15">
-        <f>InventoryList!F37:F37*InventoryList!G37:G37</f>
+        <f>(InventoryList!F38:F38*InventoryList!G38:G38)</f>
         <v>0</v>
       </c>
       <c r="I38" s="16"/>
@@ -2524,18 +2437,16 @@
     </row>
     <row r="39" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="13">
-        <f>IFERROR((InventoryList!G38:G38&lt;=InventoryList!I38:I38)*(InventoryList!L38:L38="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G39:G39&lt;=InventoryList!I39:I39)*(InventoryList!L39:L39="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C39" s="14"/>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="15"/>
-      <c r="G39" s="18">
-        <v>0</v>
-      </c>
+      <c r="G39" s="16"/>
       <c r="H39" s="15">
-        <f>InventoryList!F38:F38*InventoryList!G38:G38</f>
+        <f>(InventoryList!F39:F39*InventoryList!G39:G39)</f>
         <v>0</v>
       </c>
       <c r="I39" s="16"/>
@@ -2546,18 +2457,16 @@
     </row>
     <row r="40" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="13">
-        <f>IFERROR((InventoryList!G39:G39&lt;=InventoryList!I39:I39)*(InventoryList!L39:L39="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G40:G40&lt;=InventoryList!I40:I40)*(InventoryList!L40:L40="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="15"/>
-      <c r="G40" s="18">
-        <v>0</v>
-      </c>
+      <c r="G40" s="16"/>
       <c r="H40" s="15">
-        <f>InventoryList!F39:F39*InventoryList!G39:G39</f>
+        <f>(InventoryList!F40:F40*InventoryList!G40:G40)</f>
         <v>0</v>
       </c>
       <c r="I40" s="16"/>
@@ -2568,18 +2477,16 @@
     </row>
     <row r="41" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="13">
-        <f>IFERROR((InventoryList!G40:G40&lt;=InventoryList!I40:I40)*(InventoryList!L40:L40="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G41:G41&lt;=InventoryList!I41:I41)*(InventoryList!L41:L41="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C41" s="14"/>
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="15"/>
-      <c r="G41" s="18">
-        <v>0</v>
-      </c>
+      <c r="G41" s="16"/>
       <c r="H41" s="15">
-        <f>InventoryList!F40:F40*InventoryList!G40:G40</f>
+        <f>(InventoryList!F41:F41*InventoryList!G41:G41)</f>
         <v>0</v>
       </c>
       <c r="I41" s="16"/>
@@ -2590,18 +2497,16 @@
     </row>
     <row r="42" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="13">
-        <f>IFERROR((InventoryList!G41:G41&lt;=InventoryList!I41:I41)*(InventoryList!L41:L41="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G42:G42&lt;=InventoryList!I42:I42)*(InventoryList!L42:L42="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="15"/>
-      <c r="G42" s="18">
-        <v>0</v>
-      </c>
+      <c r="G42" s="16"/>
       <c r="H42" s="15">
-        <f>InventoryList!F41:F41*InventoryList!G41:G41</f>
+        <f>(InventoryList!F42:F42*InventoryList!G42:G42)</f>
         <v>0</v>
       </c>
       <c r="I42" s="16"/>
@@ -2612,18 +2517,16 @@
     </row>
     <row r="43" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="13">
-        <f>IFERROR((InventoryList!G42:G42&lt;=InventoryList!I42:I42)*(InventoryList!L42:L42="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G43:G43&lt;=InventoryList!I43:I43)*(InventoryList!L43:L43="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="18">
-        <v>0</v>
-      </c>
+      <c r="G43" s="16"/>
       <c r="H43" s="15">
-        <f>InventoryList!F42:F42*InventoryList!G42:G42</f>
+        <f>(InventoryList!F43:F43*InventoryList!G43:G43)</f>
         <v>0</v>
       </c>
       <c r="I43" s="16"/>
@@ -2634,18 +2537,16 @@
     </row>
     <row r="44" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="13">
-        <f>IFERROR((InventoryList!G43:G43&lt;=InventoryList!I43:I43)*(InventoryList!L43:L43="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G44:G44&lt;=InventoryList!I44:I44)*(InventoryList!L44:L44="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="15"/>
-      <c r="G44" s="18">
-        <v>0</v>
-      </c>
+      <c r="G44" s="16"/>
       <c r="H44" s="15">
-        <f>InventoryList!F43:F43*InventoryList!G43:G43</f>
+        <f>(InventoryList!F44:F44*InventoryList!G44:G44)</f>
         <v>0</v>
       </c>
       <c r="I44" s="16"/>
@@ -2656,18 +2557,16 @@
     </row>
     <row r="45" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="13">
-        <f>IFERROR((InventoryList!G44:G44&lt;=InventoryList!I44:I44)*(InventoryList!L44:L44="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G45:G45&lt;=InventoryList!I45:I45)*(InventoryList!L45:L45="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="15"/>
-      <c r="G45" s="18">
-        <v>0</v>
-      </c>
+      <c r="G45" s="16"/>
       <c r="H45" s="15">
-        <f>InventoryList!F44:F44*InventoryList!G44:G44</f>
+        <f>(InventoryList!F45:F45*InventoryList!G45:G45)</f>
         <v>0</v>
       </c>
       <c r="I45" s="16"/>
@@ -2678,18 +2577,16 @@
     </row>
     <row r="46" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="13">
-        <f>IFERROR((InventoryList!G45:G45&lt;=InventoryList!I45:I45)*(InventoryList!L45:L45="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G46:G46&lt;=InventoryList!I46:I46)*(InventoryList!L46:L46="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="15"/>
-      <c r="G46" s="18">
-        <v>0</v>
-      </c>
+      <c r="G46" s="16"/>
       <c r="H46" s="15">
-        <f>InventoryList!F45:F45*InventoryList!G45:G45</f>
+        <f>(InventoryList!F46:F46*InventoryList!G46:G46)</f>
         <v>0</v>
       </c>
       <c r="I46" s="16"/>
@@ -2700,18 +2597,16 @@
     </row>
     <row r="47" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="13">
-        <f>IFERROR((InventoryList!G46:G46&lt;=InventoryList!I46:I46)*(InventoryList!L46:L46="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G47:G47&lt;=InventoryList!I47:I47)*(InventoryList!L47:L47="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="15"/>
-      <c r="G47" s="18">
-        <v>0</v>
-      </c>
+      <c r="G47" s="16"/>
       <c r="H47" s="15">
-        <f>InventoryList!F46:F46*InventoryList!G46:G46</f>
+        <f>(InventoryList!F47:F47*InventoryList!G47:G47)</f>
         <v>0</v>
       </c>
       <c r="I47" s="16"/>
@@ -2722,18 +2617,16 @@
     </row>
     <row r="48" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="13">
-        <f>IFERROR((InventoryList!G47:G47&lt;=InventoryList!I47:I47)*(InventoryList!L47:L47="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G48:G48&lt;=InventoryList!I48:I48)*(InventoryList!L48:L48="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="15"/>
-      <c r="G48" s="18">
-        <v>0</v>
-      </c>
+      <c r="G48" s="16"/>
       <c r="H48" s="15">
-        <f>InventoryList!F47:F47*InventoryList!G47:G47</f>
+        <f>(InventoryList!F48:F48*InventoryList!G48:G48)</f>
         <v>0</v>
       </c>
       <c r="I48" s="16"/>
@@ -2744,18 +2637,16 @@
     </row>
     <row r="49" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="13">
-        <f>IFERROR((InventoryList!G48:G48&lt;=InventoryList!I48:I48)*(InventoryList!L48:L48="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G49:G49&lt;=InventoryList!I49:I49)*(InventoryList!L49:L49="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="15"/>
-      <c r="G49" s="18">
-        <v>0</v>
-      </c>
+      <c r="G49" s="16"/>
       <c r="H49" s="15">
-        <f>InventoryList!F48:F48*InventoryList!G48:G48</f>
+        <f>(InventoryList!F49:F49*InventoryList!G49:G49)</f>
         <v>0</v>
       </c>
       <c r="I49" s="16"/>
@@ -2766,18 +2657,16 @@
     </row>
     <row r="50" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="13">
-        <f>IFERROR((InventoryList!G49:G49&lt;=InventoryList!I49:I49)*(InventoryList!L49:L49="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G50:G50&lt;=InventoryList!I50:I50)*(InventoryList!L50:L50="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="15"/>
-      <c r="G50" s="18">
-        <v>0</v>
-      </c>
+      <c r="G50" s="16"/>
       <c r="H50" s="15">
-        <f>InventoryList!F49:F49*InventoryList!G49:G49</f>
+        <f>(InventoryList!F50:F50*InventoryList!G50:G50)</f>
         <v>0</v>
       </c>
       <c r="I50" s="16"/>
@@ -2788,18 +2677,16 @@
     </row>
     <row r="51" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="13">
-        <f>IFERROR((InventoryList!G50:G50&lt;=InventoryList!I50:I50)*(InventoryList!L50:L50="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G51:G51&lt;=InventoryList!I51:I51)*(InventoryList!L51:L51="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="15"/>
-      <c r="G51" s="18">
-        <v>0</v>
-      </c>
+      <c r="G51" s="16"/>
       <c r="H51" s="15">
-        <f>InventoryList!F50:F50*InventoryList!G50:G50</f>
+        <f>(InventoryList!F51:F51*InventoryList!G51:G51)</f>
         <v>0</v>
       </c>
       <c r="I51" s="16"/>
@@ -2810,18 +2697,16 @@
     </row>
     <row r="52" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="13">
-        <f>IFERROR((InventoryList!G51:G51&lt;=InventoryList!I51:I51)*(InventoryList!L51:L51="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G52:G52&lt;=InventoryList!I52:I52)*(InventoryList!L52:L52="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="15"/>
-      <c r="G52" s="18">
-        <v>0</v>
-      </c>
+      <c r="G52" s="16"/>
       <c r="H52" s="15">
-        <f>InventoryList!F51:F51*InventoryList!G51:G51</f>
+        <f>(InventoryList!F52:F52*InventoryList!G52:G52)</f>
         <v>0</v>
       </c>
       <c r="I52" s="16"/>
@@ -2832,18 +2717,16 @@
     </row>
     <row r="53" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="13">
-        <f>IFERROR((InventoryList!G52:G52&lt;=InventoryList!I52:I52)*(InventoryList!L52:L52="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G53:G53&lt;=InventoryList!I53:I53)*(InventoryList!L53:L53="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="15"/>
-      <c r="G53" s="18">
-        <v>0</v>
-      </c>
+      <c r="G53" s="16"/>
       <c r="H53" s="15">
-        <f>InventoryList!F52:F52*InventoryList!G52:G52</f>
+        <f>(InventoryList!F53:F53*InventoryList!G53:G53)</f>
         <v>0</v>
       </c>
       <c r="I53" s="16"/>
@@ -2854,18 +2737,16 @@
     </row>
     <row r="54" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="13">
-        <f>IFERROR((InventoryList!G53:G53&lt;=InventoryList!I53:I53)*(InventoryList!L53:L53="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G54:G54&lt;=InventoryList!I54:I54)*(InventoryList!L54:L54="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="15"/>
-      <c r="G54" s="18">
-        <v>0</v>
-      </c>
+      <c r="G54" s="16"/>
       <c r="H54" s="15">
-        <f>InventoryList!F53:F53*InventoryList!G53:G53</f>
+        <f>(InventoryList!F54:F54*InventoryList!G54:G54)</f>
         <v>0</v>
       </c>
       <c r="I54" s="16"/>
@@ -2876,18 +2757,16 @@
     </row>
     <row r="55" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="13">
-        <f>IFERROR((InventoryList!G54:G54&lt;=InventoryList!I54:I54)*(InventoryList!L54:L54="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G55:G55&lt;=InventoryList!I55:I55)*(InventoryList!L55:L55="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="15"/>
-      <c r="G55" s="18">
-        <v>0</v>
-      </c>
+      <c r="G55" s="16"/>
       <c r="H55" s="15">
-        <f>InventoryList!F54:F54*InventoryList!G54:G54</f>
+        <f>(InventoryList!F55:F55*InventoryList!G55:G55)</f>
         <v>0</v>
       </c>
       <c r="I55" s="16"/>
@@ -2898,18 +2777,16 @@
     </row>
     <row r="56" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="13">
-        <f>IFERROR((InventoryList!G55:G55&lt;=InventoryList!I55:I55)*(InventoryList!L55:L55="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G56:G56&lt;=InventoryList!I56:I56)*(InventoryList!L56:L56="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="15"/>
-      <c r="G56" s="18">
-        <v>0</v>
-      </c>
+      <c r="G56" s="16"/>
       <c r="H56" s="15">
-        <f>InventoryList!F55:F55*InventoryList!G55:G55</f>
+        <f>(InventoryList!F56:F56*InventoryList!G56:G56)</f>
         <v>0</v>
       </c>
       <c r="I56" s="16"/>
@@ -2920,18 +2797,16 @@
     </row>
     <row r="57" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="13">
-        <f>IFERROR((InventoryList!G56:G56&lt;=InventoryList!I56:I56)*(InventoryList!L56:L56="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G57:G57&lt;=InventoryList!I57:I57)*(InventoryList!L57:L57="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="15"/>
-      <c r="G57" s="18">
-        <v>0</v>
-      </c>
+      <c r="G57" s="16"/>
       <c r="H57" s="15">
-        <f>InventoryList!F56:F56*InventoryList!G56:G56</f>
+        <f>(InventoryList!F57:F57*InventoryList!G57:G57)</f>
         <v>0</v>
       </c>
       <c r="I57" s="16"/>
@@ -2942,18 +2817,16 @@
     </row>
     <row r="58" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="13">
-        <f>IFERROR((InventoryList!G57:G57&lt;=InventoryList!I57:I57)*(InventoryList!L57:L57="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G58:G58&lt;=InventoryList!I58:I58)*(InventoryList!L58:L58="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="15"/>
-      <c r="G58" s="18">
-        <v>0</v>
-      </c>
+      <c r="G58" s="16"/>
       <c r="H58" s="15">
-        <f>InventoryList!F57:F57*InventoryList!G57:G57</f>
+        <f>(InventoryList!F58:F58*InventoryList!G58:G58)</f>
         <v>0</v>
       </c>
       <c r="I58" s="16"/>
@@ -2964,18 +2837,16 @@
     </row>
     <row r="59" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="13">
-        <f>IFERROR((InventoryList!G58:G58&lt;=InventoryList!I58:I58)*(InventoryList!L58:L58="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G59:G59&lt;=InventoryList!I59:I59)*(InventoryList!L59:L59="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="15"/>
-      <c r="G59" s="18">
-        <v>0</v>
-      </c>
+      <c r="G59" s="16"/>
       <c r="H59" s="15">
-        <f>InventoryList!F58:F58*InventoryList!G58:G58</f>
+        <f>(InventoryList!F59:F59*InventoryList!G59:G59)</f>
         <v>0</v>
       </c>
       <c r="I59" s="16"/>
@@ -2986,18 +2857,16 @@
     </row>
     <row r="60" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="13">
-        <f>IFERROR((InventoryList!G59:G59&lt;=InventoryList!I59:I59)*(InventoryList!L59:L59="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G60:G60&lt;=InventoryList!I60:I60)*(InventoryList!L60:L60="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="15"/>
-      <c r="G60" s="18">
-        <v>0</v>
-      </c>
+      <c r="G60" s="16"/>
       <c r="H60" s="15">
-        <f>InventoryList!F59:F59*InventoryList!G59:G59</f>
+        <f>(InventoryList!F60:F60*InventoryList!G60:G60)</f>
         <v>0</v>
       </c>
       <c r="I60" s="16"/>
@@ -3008,18 +2877,16 @@
     </row>
     <row r="61" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="13">
-        <f>IFERROR((InventoryList!G60:G60&lt;=InventoryList!I60:I60)*(InventoryList!L60:L60="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G61:G61&lt;=InventoryList!I61:I61)*(InventoryList!L61:L61="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="15"/>
-      <c r="G61" s="18">
-        <v>0</v>
-      </c>
+      <c r="G61" s="16"/>
       <c r="H61" s="15">
-        <f>InventoryList!F60:F60*InventoryList!G60:G60</f>
+        <f>(InventoryList!F61:F61*InventoryList!G61:G61)</f>
         <v>0</v>
       </c>
       <c r="I61" s="16"/>
@@ -3030,18 +2897,16 @@
     </row>
     <row r="62" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="13">
-        <f>IFERROR((InventoryList!G61:G61&lt;=InventoryList!I61:I61)*(InventoryList!L61:L61="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G62:G62&lt;=InventoryList!I62:I62)*(InventoryList!L62:L62="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="15"/>
-      <c r="G62" s="18">
-        <v>0</v>
-      </c>
+      <c r="G62" s="16"/>
       <c r="H62" s="15">
-        <f>InventoryList!F61:F61*InventoryList!G61:G61</f>
+        <f>(InventoryList!F62:F62*InventoryList!G62:G62)</f>
         <v>0</v>
       </c>
       <c r="I62" s="16"/>
@@ -3052,18 +2917,16 @@
     </row>
     <row r="63" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="13">
-        <f>IFERROR((InventoryList!G62:G62&lt;=InventoryList!I62:I62)*(InventoryList!L62:L62="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G63:G63&lt;=InventoryList!I63:I63)*(InventoryList!L63:L63="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="15"/>
-      <c r="G63" s="18">
-        <v>0</v>
-      </c>
+      <c r="G63" s="16"/>
       <c r="H63" s="15">
-        <f>InventoryList!F62:F62*InventoryList!G62:G62</f>
+        <f>(InventoryList!F63:F63*InventoryList!G63:G63)</f>
         <v>0</v>
       </c>
       <c r="I63" s="16"/>
@@ -3074,18 +2937,16 @@
     </row>
     <row r="64" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="13">
-        <f>IFERROR((InventoryList!G63:G63&lt;=InventoryList!I63:I63)*(InventoryList!L63:L63="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G64:G64&lt;=InventoryList!I64:I64)*(InventoryList!L64:L64="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="15"/>
-      <c r="G64" s="18">
-        <v>0</v>
-      </c>
+      <c r="G64" s="16"/>
       <c r="H64" s="15">
-        <f>InventoryList!F63:F63*InventoryList!G63:G63</f>
+        <f>(InventoryList!F64:F64*InventoryList!G64:G64)</f>
         <v>0</v>
       </c>
       <c r="I64" s="16"/>
@@ -3096,18 +2957,16 @@
     </row>
     <row r="65" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="13">
-        <f>IFERROR((InventoryList!G64:G64&lt;=InventoryList!I64:I64)*(InventoryList!L64:L64="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G65:G65&lt;=InventoryList!I65:I65)*(InventoryList!L65:L65="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C65" s="14"/>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
       <c r="F65" s="15"/>
-      <c r="G65" s="18">
-        <v>0</v>
-      </c>
+      <c r="G65" s="16"/>
       <c r="H65" s="15">
-        <f>InventoryList!F64:F64*InventoryList!G64:G64</f>
+        <f>(InventoryList!F65:F65*InventoryList!G65:G65)</f>
         <v>0</v>
       </c>
       <c r="I65" s="16"/>
@@ -3118,18 +2977,16 @@
     </row>
     <row r="66" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="13">
-        <f>IFERROR((InventoryList!G65:G65&lt;=InventoryList!I65:I65)*(InventoryList!L65:L65="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G66:G66&lt;=InventoryList!I66:I66)*(InventoryList!L66:L66="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C66" s="14"/>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="15"/>
-      <c r="G66" s="18">
-        <v>0</v>
-      </c>
+      <c r="G66" s="16"/>
       <c r="H66" s="15">
-        <f>InventoryList!F65:F65*InventoryList!G65:G65</f>
+        <f>(InventoryList!F66:F66*InventoryList!G66:G66)</f>
         <v>0</v>
       </c>
       <c r="I66" s="16"/>
@@ -3140,18 +2997,16 @@
     </row>
     <row r="67" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="13">
-        <f>IFERROR((InventoryList!G66:G66&lt;=InventoryList!I66:I66)*(InventoryList!L66:L66="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G67:G67&lt;=InventoryList!I67:I67)*(InventoryList!L67:L67="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="15"/>
-      <c r="G67" s="18">
-        <v>0</v>
-      </c>
+      <c r="G67" s="16"/>
       <c r="H67" s="15">
-        <f>InventoryList!F66:F66*InventoryList!G66:G66</f>
+        <f>(InventoryList!F67:F67*InventoryList!G67:G67)</f>
         <v>0</v>
       </c>
       <c r="I67" s="16"/>
@@ -3162,18 +3017,16 @@
     </row>
     <row r="68" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="13">
-        <f>IFERROR((InventoryList!G67:G67&lt;=InventoryList!I67:I67)*(InventoryList!L67:L67="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G68:G68&lt;=InventoryList!I68:I68)*(InventoryList!L68:L68="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="15"/>
-      <c r="G68" s="18">
-        <v>0</v>
-      </c>
+      <c r="G68" s="16"/>
       <c r="H68" s="15">
-        <f>InventoryList!F67:F67*InventoryList!G67:G67</f>
+        <f>(InventoryList!F68:F68*InventoryList!G68:G68)</f>
         <v>0</v>
       </c>
       <c r="I68" s="16"/>
@@ -3184,18 +3037,16 @@
     </row>
     <row r="69" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="13">
-        <f>IFERROR((InventoryList!G68:G68&lt;=InventoryList!I68:I68)*(InventoryList!L68:L68="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G69:G69&lt;=InventoryList!I69:I69)*(InventoryList!L69:L69="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="15"/>
-      <c r="G69" s="18">
-        <v>0</v>
-      </c>
+      <c r="G69" s="16"/>
       <c r="H69" s="15">
-        <f>InventoryList!F68:F68*InventoryList!G68:G68</f>
+        <f>(InventoryList!F69:F69*InventoryList!G69:G69)</f>
         <v>0</v>
       </c>
       <c r="I69" s="16"/>
@@ -3206,18 +3057,16 @@
     </row>
     <row r="70" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="13">
-        <f>IFERROR((InventoryList!G69:G69&lt;=InventoryList!I69:I69)*(InventoryList!L69:L69="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G70:G70&lt;=InventoryList!I70:I70)*(InventoryList!L70:L70="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="15"/>
-      <c r="G70" s="18">
-        <v>0</v>
-      </c>
+      <c r="G70" s="16"/>
       <c r="H70" s="15">
-        <f>InventoryList!F69:F69*InventoryList!G69:G69</f>
+        <f>(InventoryList!F70:F70*InventoryList!G70:G70)</f>
         <v>0</v>
       </c>
       <c r="I70" s="16"/>
@@ -3228,18 +3077,16 @@
     </row>
     <row r="71" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="13">
-        <f>IFERROR((InventoryList!G70:G70&lt;=InventoryList!I70:I70)*(InventoryList!L70:L70="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G71:G71&lt;=InventoryList!I71:I71)*(InventoryList!L71:L71="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="15"/>
-      <c r="G71" s="18">
-        <v>0</v>
-      </c>
+      <c r="G71" s="16"/>
       <c r="H71" s="15">
-        <f>InventoryList!F70:F70*InventoryList!G70:G70</f>
+        <f>(InventoryList!F71:F71*InventoryList!G71:G71)</f>
         <v>0</v>
       </c>
       <c r="I71" s="16"/>
@@ -3250,18 +3097,16 @@
     </row>
     <row r="72" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="13">
-        <f>IFERROR((InventoryList!G71:G71&lt;=InventoryList!I71:I71)*(InventoryList!L71:L71="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G72:G72&lt;=InventoryList!I72:I72)*(InventoryList!L72:L72="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C72" s="14"/>
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="15"/>
-      <c r="G72" s="18">
-        <v>0</v>
-      </c>
+      <c r="G72" s="16"/>
       <c r="H72" s="15">
-        <f>InventoryList!F71:F71*InventoryList!G71:G71</f>
+        <f>(InventoryList!F72:F72*InventoryList!G72:G72)</f>
         <v>0</v>
       </c>
       <c r="I72" s="16"/>
@@ -3272,18 +3117,16 @@
     </row>
     <row r="73" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="13">
-        <f>IFERROR((InventoryList!G72:G72&lt;=InventoryList!I72:I72)*(InventoryList!L72:L72="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G73:G73&lt;=InventoryList!I73:I73)*(InventoryList!L73:L73="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C73" s="14"/>
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="15"/>
-      <c r="G73" s="18">
-        <v>0</v>
-      </c>
+      <c r="G73" s="16"/>
       <c r="H73" s="15">
-        <f>InventoryList!F72:F72*InventoryList!G72:G72</f>
+        <f>(InventoryList!F73:F73*InventoryList!G73:G73)</f>
         <v>0</v>
       </c>
       <c r="I73" s="16"/>
@@ -3294,18 +3137,16 @@
     </row>
     <row r="74" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="13">
-        <f>IFERROR((InventoryList!G73:G73&lt;=InventoryList!I73:I73)*(InventoryList!L73:L73="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G74:G74&lt;=InventoryList!I74:I74)*(InventoryList!L74:L74="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="15"/>
-      <c r="G74" s="18">
-        <v>0</v>
-      </c>
+      <c r="G74" s="16"/>
       <c r="H74" s="15">
-        <f>InventoryList!F73:F73*InventoryList!G73:G73</f>
+        <f>(InventoryList!F74:F74*InventoryList!G74:G74)</f>
         <v>0</v>
       </c>
       <c r="I74" s="16"/>
@@ -3316,18 +3157,16 @@
     </row>
     <row r="75" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="13">
-        <f>IFERROR((InventoryList!G74:G74&lt;=InventoryList!I74:I74)*(InventoryList!L74:L74="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G75:G75&lt;=InventoryList!I75:I75)*(InventoryList!L75:L75="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C75" s="14"/>
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="15"/>
-      <c r="G75" s="18">
-        <v>0</v>
-      </c>
+      <c r="G75" s="16"/>
       <c r="H75" s="15">
-        <f>InventoryList!F74:F74*InventoryList!G74:G74</f>
+        <f>(InventoryList!F75:F75*InventoryList!G75:G75)</f>
         <v>0</v>
       </c>
       <c r="I75" s="16"/>
@@ -3338,18 +3177,16 @@
     </row>
     <row r="76" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="13">
-        <f>IFERROR((InventoryList!G75:G75&lt;=InventoryList!I75:I75)*(InventoryList!L75:L75="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G76:G76&lt;=InventoryList!I76:I76)*(InventoryList!L76:L76="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C76" s="14"/>
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="15"/>
-      <c r="G76" s="18">
-        <v>0</v>
-      </c>
+      <c r="G76" s="16"/>
       <c r="H76" s="15">
-        <f>InventoryList!F75:F75*InventoryList!G75:G75</f>
+        <f>(InventoryList!F76:F76*InventoryList!G76:G76)</f>
         <v>0</v>
       </c>
       <c r="I76" s="16"/>
@@ -3360,18 +3197,16 @@
     </row>
     <row r="77" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="13">
-        <f>IFERROR((InventoryList!G76:G76&lt;=InventoryList!I76:I76)*(InventoryList!L76:L76="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G77:G77&lt;=InventoryList!I77:I77)*(InventoryList!L77:L77="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C77" s="14"/>
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="15"/>
-      <c r="G77" s="18">
-        <v>0</v>
-      </c>
+      <c r="G77" s="16"/>
       <c r="H77" s="15">
-        <f>InventoryList!F76:F76*InventoryList!G76:G76</f>
+        <f>(InventoryList!F77:F77*InventoryList!G77:G77)</f>
         <v>0</v>
       </c>
       <c r="I77" s="16"/>
@@ -3382,18 +3217,16 @@
     </row>
     <row r="78" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="13">
-        <f>IFERROR((InventoryList!G77:G77&lt;=InventoryList!I77:I77)*(InventoryList!L77:L77="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G78:G78&lt;=InventoryList!I78:I78)*(InventoryList!L78:L78="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C78" s="14"/>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="15"/>
-      <c r="G78" s="18">
-        <v>0</v>
-      </c>
+      <c r="G78" s="16"/>
       <c r="H78" s="15">
-        <f>InventoryList!F77:F77*InventoryList!G77:G77</f>
+        <f>(InventoryList!F78:F78*InventoryList!G78:G78)</f>
         <v>0</v>
       </c>
       <c r="I78" s="16"/>
@@ -3404,18 +3237,16 @@
     </row>
     <row r="79" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="13">
-        <f>IFERROR((InventoryList!G78:G78&lt;=InventoryList!I78:I78)*(InventoryList!L78:L78="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G79:G79&lt;=InventoryList!I79:I79)*(InventoryList!L79:L79="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C79" s="14"/>
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="15"/>
-      <c r="G79" s="18">
-        <v>0</v>
-      </c>
+      <c r="G79" s="16"/>
       <c r="H79" s="15">
-        <f>InventoryList!F78:F78*InventoryList!G78:G78</f>
+        <f>(InventoryList!F79:F79*InventoryList!G79:G79)</f>
         <v>0</v>
       </c>
       <c r="I79" s="16"/>
@@ -3426,18 +3257,16 @@
     </row>
     <row r="80" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="13">
-        <f>IFERROR((InventoryList!G79:G79&lt;=InventoryList!I79:I79)*(InventoryList!L79:L79="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G80:G80&lt;=InventoryList!I80:I80)*(InventoryList!L80:L80="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C80" s="14"/>
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="15"/>
-      <c r="G80" s="18">
-        <v>0</v>
-      </c>
+      <c r="G80" s="16"/>
       <c r="H80" s="15">
-        <f>InventoryList!F79:F79*InventoryList!G79:G79</f>
+        <f>(InventoryList!F80:F80*InventoryList!G80:G80)</f>
         <v>0</v>
       </c>
       <c r="I80" s="16"/>
@@ -3448,18 +3277,16 @@
     </row>
     <row r="81" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="13">
-        <f>IFERROR((InventoryList!G80:G80&lt;=InventoryList!I80:I80)*(InventoryList!L80:L80="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G81:G81&lt;=InventoryList!I81:I81)*(InventoryList!L81:L81="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C81" s="14"/>
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
       <c r="F81" s="15"/>
-      <c r="G81" s="18">
-        <v>0</v>
-      </c>
+      <c r="G81" s="16"/>
       <c r="H81" s="15">
-        <f>InventoryList!F80:F80*InventoryList!G80:G80</f>
+        <f>(InventoryList!F81:F81*InventoryList!G81:G81)</f>
         <v>0</v>
       </c>
       <c r="I81" s="16"/>
@@ -3470,18 +3297,16 @@
     </row>
     <row r="82" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="13">
-        <f>IFERROR((InventoryList!G81:G81&lt;=InventoryList!I81:I81)*(InventoryList!L81:L81="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G82:G82&lt;=InventoryList!I82:I82)*(InventoryList!L82:L82="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C82" s="14"/>
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="15"/>
-      <c r="G82" s="18">
-        <v>0</v>
-      </c>
+      <c r="G82" s="16"/>
       <c r="H82" s="15">
-        <f>InventoryList!F81:F81*InventoryList!G81:G81</f>
+        <f>(InventoryList!F82:F82*InventoryList!G82:G82)</f>
         <v>0</v>
       </c>
       <c r="I82" s="16"/>
@@ -3492,18 +3317,16 @@
     </row>
     <row r="83" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="13">
-        <f>IFERROR((InventoryList!G82:G82&lt;=InventoryList!I82:I82)*(InventoryList!L82:L82="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G83:G83&lt;=InventoryList!I83:I83)*(InventoryList!L83:L83="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C83" s="14"/>
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
       <c r="F83" s="15"/>
-      <c r="G83" s="18">
-        <v>0</v>
-      </c>
+      <c r="G83" s="16"/>
       <c r="H83" s="15">
-        <f>InventoryList!F82:F82*InventoryList!G82:G82</f>
+        <f>(InventoryList!F83:F83*InventoryList!G83:G83)</f>
         <v>0</v>
       </c>
       <c r="I83" s="16"/>
@@ -3514,18 +3337,16 @@
     </row>
     <row r="84" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="13">
-        <f>IFERROR((InventoryList!G83:G83&lt;=InventoryList!I83:I83)*(InventoryList!L83:L83="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G84:G84&lt;=InventoryList!I84:I84)*(InventoryList!L84:L84="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C84" s="14"/>
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
       <c r="F84" s="15"/>
-      <c r="G84" s="18">
-        <v>0</v>
-      </c>
+      <c r="G84" s="16"/>
       <c r="H84" s="15">
-        <f>InventoryList!F83:F83*InventoryList!G83:G83</f>
+        <f>(InventoryList!F84:F84*InventoryList!G84:G84)</f>
         <v>0</v>
       </c>
       <c r="I84" s="16"/>
@@ -3536,18 +3357,16 @@
     </row>
     <row r="85" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="13">
-        <f>IFERROR((InventoryList!G84:G84&lt;=InventoryList!I84:I84)*(InventoryList!L84:L84="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G85:G85&lt;=InventoryList!I85:I85)*(InventoryList!L85:L85="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C85" s="14"/>
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="15"/>
-      <c r="G85" s="18">
-        <v>0</v>
-      </c>
+      <c r="G85" s="16"/>
       <c r="H85" s="15">
-        <f>InventoryList!F84:F84*InventoryList!G84:G84</f>
+        <f>(InventoryList!F85:F85*InventoryList!G85:G85)</f>
         <v>0</v>
       </c>
       <c r="I85" s="16"/>
@@ -3558,18 +3377,16 @@
     </row>
     <row r="86" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="13">
-        <f>IFERROR((InventoryList!G85:G85&lt;=InventoryList!I85:I85)*(InventoryList!L85:L85="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G86:G86&lt;=InventoryList!I86:I86)*(InventoryList!L86:L86="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C86" s="14"/>
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="15"/>
-      <c r="G86" s="18">
-        <v>0</v>
-      </c>
+      <c r="G86" s="16"/>
       <c r="H86" s="15">
-        <f>InventoryList!F85:F85*InventoryList!G85:G85</f>
+        <f>(InventoryList!F86:F86*InventoryList!G86:G86)</f>
         <v>0</v>
       </c>
       <c r="I86" s="16"/>
@@ -3580,18 +3397,16 @@
     </row>
     <row r="87" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="13">
-        <f>IFERROR((InventoryList!G86:G86&lt;=InventoryList!I86:I86)*(InventoryList!L86:L86="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G87:G87&lt;=InventoryList!I87:I87)*(InventoryList!L87:L87="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C87" s="14"/>
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
       <c r="F87" s="15"/>
-      <c r="G87" s="18">
-        <v>0</v>
-      </c>
+      <c r="G87" s="16"/>
       <c r="H87" s="15">
-        <f>InventoryList!F86:F86*InventoryList!G86:G86</f>
+        <f>(InventoryList!F87:F87*InventoryList!G87:G87)</f>
         <v>0</v>
       </c>
       <c r="I87" s="16"/>
@@ -3602,18 +3417,16 @@
     </row>
     <row r="88" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="13">
-        <f>IFERROR((InventoryList!G87:G87&lt;=InventoryList!I87:I87)*(InventoryList!L87:L87="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G88:G88&lt;=InventoryList!I88:I88)*(InventoryList!L88:L88="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C88" s="14"/>
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="15"/>
-      <c r="G88" s="18">
-        <v>0</v>
-      </c>
+      <c r="G88" s="16"/>
       <c r="H88" s="15">
-        <f>InventoryList!F87:F87*InventoryList!G87:G87</f>
+        <f>(InventoryList!F88:F88*InventoryList!G88:G88)</f>
         <v>0</v>
       </c>
       <c r="I88" s="16"/>
@@ -3624,18 +3437,16 @@
     </row>
     <row r="89" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="13">
-        <f>IFERROR((InventoryList!G88:G88&lt;=InventoryList!I88:I88)*(InventoryList!L88:L88="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G89:G89&lt;=InventoryList!I89:I89)*(InventoryList!L89:L89="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C89" s="14"/>
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="15"/>
-      <c r="G89" s="18">
-        <v>0</v>
-      </c>
+      <c r="G89" s="16"/>
       <c r="H89" s="15">
-        <f>InventoryList!F88:F88*InventoryList!G88:G88</f>
+        <f>(InventoryList!F89:F89*InventoryList!G89:G89)</f>
         <v>0</v>
       </c>
       <c r="I89" s="16"/>
@@ -3646,18 +3457,16 @@
     </row>
     <row r="90" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="13">
-        <f>IFERROR((InventoryList!G89:G89&lt;=InventoryList!I89:I89)*(InventoryList!L89:L89="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G90:G90&lt;=InventoryList!I90:I90)*(InventoryList!L90:L90="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C90" s="14"/>
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
       <c r="F90" s="15"/>
-      <c r="G90" s="18">
-        <v>0</v>
-      </c>
+      <c r="G90" s="16"/>
       <c r="H90" s="15">
-        <f>InventoryList!F89:F89*InventoryList!G89:G89</f>
+        <f>(InventoryList!F90:F90*InventoryList!G90:G90)</f>
         <v>0</v>
       </c>
       <c r="I90" s="16"/>
@@ -3668,18 +3477,16 @@
     </row>
     <row r="91" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="13">
-        <f>IFERROR((InventoryList!G90:G90&lt;=InventoryList!I90:I90)*(InventoryList!L90:L90="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G91:G91&lt;=InventoryList!I91:I91)*(InventoryList!L91:L91="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C91" s="14"/>
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="15"/>
-      <c r="G91" s="18">
-        <v>0</v>
-      </c>
+      <c r="G91" s="16"/>
       <c r="H91" s="15">
-        <f>InventoryList!F90:F90*InventoryList!G90:G90</f>
+        <f>(InventoryList!F91:F91*InventoryList!G91:G91)</f>
         <v>0</v>
       </c>
       <c r="I91" s="16"/>
@@ -3690,18 +3497,16 @@
     </row>
     <row r="92" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="13">
-        <f>IFERROR((InventoryList!G91:G91&lt;=InventoryList!I91:I91)*(InventoryList!L91:L91="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G92:G92&lt;=InventoryList!I92:I92)*(InventoryList!L92:L92="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C92" s="14"/>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
       <c r="F92" s="15"/>
-      <c r="G92" s="18">
-        <v>0</v>
-      </c>
+      <c r="G92" s="16"/>
       <c r="H92" s="15">
-        <f>InventoryList!F91:F91*InventoryList!G91:G91</f>
+        <f>(InventoryList!F92:F92*InventoryList!G92:G92)</f>
         <v>0</v>
       </c>
       <c r="I92" s="16"/>
@@ -3712,18 +3517,16 @@
     </row>
     <row r="93" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="13">
-        <f>IFERROR((InventoryList!G92:G92&lt;=InventoryList!I92:I92)*(InventoryList!L92:L92="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G93:G93&lt;=InventoryList!I93:I93)*(InventoryList!L93:L93="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C93" s="14"/>
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="15"/>
-      <c r="G93" s="18">
-        <v>0</v>
-      </c>
+      <c r="G93" s="16"/>
       <c r="H93" s="15">
-        <f>InventoryList!F92:F92*InventoryList!G92:G92</f>
+        <f>(InventoryList!F93:F93*InventoryList!G93:G93)</f>
         <v>0</v>
       </c>
       <c r="I93" s="16"/>
@@ -3734,18 +3537,16 @@
     </row>
     <row r="94" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="13">
-        <f>IFERROR((InventoryList!G93:G93&lt;=InventoryList!I93:I93)*(InventoryList!L93:L93="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G94:G94&lt;=InventoryList!I94:I94)*(InventoryList!L94:L94="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C94" s="14"/>
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="15"/>
-      <c r="G94" s="18">
-        <v>0</v>
-      </c>
+      <c r="G94" s="16"/>
       <c r="H94" s="15">
-        <f>InventoryList!F93:F93*InventoryList!G93:G93</f>
+        <f>(InventoryList!F94:F94*InventoryList!G94:G94)</f>
         <v>0</v>
       </c>
       <c r="I94" s="16"/>
@@ -3756,18 +3557,16 @@
     </row>
     <row r="95" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="13">
-        <f>IFERROR((InventoryList!G94:G94&lt;=InventoryList!I94:I94)*(InventoryList!L94:L94="")*valHighlight,0)</f>
+        <f>ЕСЛИОШИБКА((InventoryList!G95:G95&lt;=InventoryList!I95:I95)*(InventoryList!L95:L95="")*valHighlight,0)</f>
         <v>1</v>
       </c>
       <c r="C95" s="14"/>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
       <c r="F95" s="15"/>
-      <c r="G95" s="18">
-        <v>0</v>
-      </c>
+      <c r="G95" s="16"/>
       <c r="H95" s="15">
-        <f>InventoryList!F94:F94*InventoryList!G94:G94</f>
+        <f>(InventoryList!F95:F95*InventoryList!G95:G95)</f>
         <v>0</v>
       </c>
       <c r="I95" s="16"/>
@@ -3777,12 +3576,19 @@
       <c r="M95" s="17"/>
     </row>
     <row r="96" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="13"/>
+      <c r="B96" s="13">
+        <f>ЕСЛИОШИБКА((InventoryList!G96:G96&lt;=InventoryList!I96:I96)*(InventoryList!L96:L96="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
       <c r="C96" s="14"/>
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="15"/>
-      <c r="H96" s="15"/>
+      <c r="G96" s="16"/>
+      <c r="H96" s="15">
+        <f>(InventoryList!F96:F96*InventoryList!G96:G96)</f>
+        <v>0</v>
+      </c>
       <c r="I96" s="16"/>
       <c r="J96" s="16"/>
       <c r="K96" s="16"/>
@@ -3790,26 +3596,53 @@
       <c r="M96" s="17"/>
     </row>
     <row r="97" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="13"/>
+      <c r="B97" s="13">
+        <f>ЕСЛИОШИБКА((InventoryList!G97:G97&lt;=InventoryList!I97:I97)*(InventoryList!L97:L97="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
       <c r="C97" s="14"/>
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="15"/>
-      <c r="H97" s="15"/>
+      <c r="G97" s="16"/>
+      <c r="H97" s="15">
+        <f>(InventoryList!F97:F97*InventoryList!G97:G97)</f>
+        <v>0</v>
+      </c>
       <c r="I97" s="16"/>
       <c r="J97" s="16"/>
       <c r="K97" s="16"/>
       <c r="L97" s="14"/>
       <c r="M97" s="17"/>
     </row>
+    <row r="98" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="13">
+        <f>ЕСЛИОШИБКА((InventoryList!G98:G98&lt;=InventoryList!I98:I98)*(InventoryList!L98:L98="")*valHighlight,0)</f>
+        <v>1</v>
+      </c>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="15">
+        <f>(InventoryList!F98:F98*InventoryList!G98:G98)</f>
+        <v>0</v>
+      </c>
+      <c r="I98" s="16"/>
+      <c r="J98" s="16"/>
+      <c r="K98" s="16"/>
+      <c r="L98" s="14"/>
+      <c r="M98" s="17"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B4:M95 G96:G97">
+  <conditionalFormatting sqref="B4:M98">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$L4="Так"</formula>
+      <formula>#REF!="Так"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$B4=1</formula>
+      <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="67" yWindow="628" count="14">
@@ -3824,13 +3657,13 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці кількість кожного товару на складі" sqref="G3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці ціну за одиницю кожного товару" sqref="F3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці опис товару" sqref="E3" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L5" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+      <formula1>"Так"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Щоб почати виділення елементів перевпорядкування, виберіть «Так». Після цього в стовпці B з’являтиметься позначка, а весь відповідний рядок виділятиметься кольором у таблиці «Список запасів». Якщо вибрати «Ні», позначки та виділення повністю прибираються." sqref="L2" xr:uid="{00000000-0002-0000-0000-00000D000000}">
       <formula1>"Так, Ні"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Інвентарний список" prompt="Цей аркуш відстежує запаси товарів у таблиці та дає можливість виділити й позначити товари, чиї запаси слід поповнити. Якщо товар вилучено, текст у його рядку закреслюється, а в стовпці &quot;Вилучено&quot; з’являється напис &quot;Так&quot;." sqref="A1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4" xr:uid="{00000000-0002-0000-0000-00000C000000}">
-      <formula1>"Так"</formula1>
-    </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="62" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -3842,7 +3675,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{22614FA3-6814-43BC-85E4-CF5B29361B41}">
+          <x14:cfRule type="iconSet" priority="6" id="{22614FA3-6814-43BC-85E4-CF5B29361B41}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -3858,7 +3691,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B4:B99</xm:sqref>
+          <xm:sqref>B4:B100</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3867,12 +3700,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4084,20 +3917,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4123,9 +3954,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Delete complete ? mb fix
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D540E2-E876-4EE4-969E-390B9FEEC88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4658B34A-33AF-4069-8387-C001E4CDAC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30480" yWindow="1785" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="1350" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <definedName name="valHighlight">IFERROR(IF(InventoryList!$L$2="Так", TRUE, FALSE),FALSE)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">InventoryList!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Для нижньої межі</t>
   </si>
@@ -80,10 +83,7 @@
     <t>Група</t>
   </si>
   <si>
-    <t>q1</t>
-  </si>
-  <si>
-    <t>t1</t>
+    <t>a1</t>
   </si>
   <si>
     <t>Sup1</t>
@@ -92,25 +92,28 @@
     <t>Group1</t>
   </si>
   <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>t2</t>
+    <t>a2</t>
   </si>
   <si>
     <t>Group2</t>
   </si>
   <si>
-    <t>q3</t>
+    <t>a3</t>
   </si>
   <si>
     <t>Group3</t>
   </si>
   <si>
-    <t>q4</t>
+    <t>b1</t>
   </si>
   <si>
-    <t>t4</t>
+    <t>Sup2</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>Sup3</t>
   </si>
 </sst>
 </file>
@@ -1630,7 +1633,7 @@
   <dimension ref="B1:M98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:G7"/>
+      <selection activeCell="B10" sqref="B10:B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1713,131 +1716,181 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3">
-        <f>ЕСЛИОШИБКА((InventoryList!G4:G4&lt;=InventoryList!I4:I4)*(InventoryList!L4:L4="")*valHighlight,0)</f>
+      <c r="B4" s="13">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G4:G4)&lt;=_xlfn.SINGLE(InventoryList!I4:I4))*(_xlfn.SINGLE(InventoryList!L4:L4)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="12" t="n">
-        <v>1.0</v>
+        <v>16</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
       </c>
       <c r="H4" s="12">
         <f>(InventoryList!F4:F4*InventoryList!G4:G4)</f>
         <v>0</v>
       </c>
-      <c r="I4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1.0</v>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="3">
-        <f>ЕСЛИОШИБКА((InventoryList!G5:G5&lt;=InventoryList!I5:I5)*(InventoryList!L5:L5="")*valHighlight,0)</f>
+      <c r="B5" s="13">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G5:G5)&lt;=_xlfn.SINGLE(InventoryList!I5:I5))*(_xlfn.SINGLE(InventoryList!L5:L5)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="12" t="n">
-        <v>1.0</v>
+        <v>16</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
       </c>
       <c r="H5" s="12">
         <f>(InventoryList!F5:F5*InventoryList!G5:G5)</f>
         <v>0</v>
       </c>
-      <c r="I5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>1.0</v>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G6:G6&lt;=InventoryList!I6:I6)*(InventoryList!L6:L6="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G6:G6)&lt;=_xlfn.SINGLE(InventoryList!I6:I6))*(_xlfn.SINGLE(InventoryList!L6:L6)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="15">
+        <v>1</v>
+      </c>
       <c r="G6" s="16"/>
       <c r="H6" s="15">
         <f>(InventoryList!F6:F6*InventoryList!G6:G6)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
+      <c r="I6" s="16">
+        <v>1</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1</v>
+      </c>
       <c r="K6" s="16"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="17"/>
+      <c r="M6" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G7:G7&lt;=InventoryList!I7:I7)*(InventoryList!L7:L7="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="16"/>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G7:G7)&lt;=_xlfn.SINGLE(InventoryList!I7:I7))*(_xlfn.SINGLE(InventoryList!L7:L7)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="15">
+        <v>1</v>
+      </c>
+      <c r="G7" s="16">
+        <v>45</v>
+      </c>
       <c r="H7" s="15">
         <f>(InventoryList!F7:F7*InventoryList!G7:G7)</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+        <v>45</v>
+      </c>
+      <c r="I7" s="16">
+        <v>1</v>
+      </c>
+      <c r="J7" s="16">
+        <v>1</v>
+      </c>
+      <c r="K7" s="16">
+        <v>12</v>
+      </c>
       <c r="L7" s="14"/>
-      <c r="M7" s="17"/>
+      <c r="M7" s="17" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G8:G8&lt;=InventoryList!I8:I8)*(InventoryList!L8:L8="")*valHighlight,0)</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G8:G8)&lt;=_xlfn.SINGLE(InventoryList!I8:I8))*(_xlfn.SINGLE(InventoryList!L8:L8)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="15">
+        <v>3</v>
+      </c>
+      <c r="G8" s="16" t="n">
+        <v>157.0</v>
+      </c>
       <c r="H8" s="15">
         <f>(InventoryList!F8:F8*InventoryList!G8:G8)</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
+        <v>468</v>
+      </c>
+      <c r="I8" s="16">
+        <v>3</v>
+      </c>
+      <c r="J8" s="16">
+        <v>3</v>
+      </c>
+      <c r="K8" s="16" t="n">
+        <v>1.0</v>
+      </c>
       <c r="L8" s="14"/>
-      <c r="M8" s="17"/>
+      <c r="M8" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G9:G9&lt;=InventoryList!I9:I9)*(InventoryList!L9:L9="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G9:G9)&lt;=_xlfn.SINGLE(InventoryList!I9:I9))*(_xlfn.SINGLE(InventoryList!L9:L9)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C9" s="14"/>
@@ -1857,7 +1910,7 @@
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G10:G10&lt;=InventoryList!I10:I10)*(InventoryList!L10:L10="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G10:G10)&lt;=_xlfn.SINGLE(InventoryList!I10:I10))*(_xlfn.SINGLE(InventoryList!L10:L10)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C10" s="14"/>
@@ -1877,7 +1930,7 @@
     </row>
     <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G11:G11&lt;=InventoryList!I11:I11)*(InventoryList!L11:L11="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G11:G11)&lt;=_xlfn.SINGLE(InventoryList!I11:I11))*(_xlfn.SINGLE(InventoryList!L11:L11)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C11" s="14"/>
@@ -1897,7 +1950,7 @@
     </row>
     <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G12:G12&lt;=InventoryList!I12:I12)*(InventoryList!L12:L12="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G12:G12)&lt;=_xlfn.SINGLE(InventoryList!I12:I12))*(_xlfn.SINGLE(InventoryList!L12:L12)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C12" s="14"/>
@@ -1917,7 +1970,7 @@
     </row>
     <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G13:G13&lt;=InventoryList!I13:I13)*(InventoryList!L13:L13="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G13:G13)&lt;=_xlfn.SINGLE(InventoryList!I13:I13))*(_xlfn.SINGLE(InventoryList!L13:L13)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C13" s="14"/>
@@ -1937,7 +1990,7 @@
     </row>
     <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G14:G14&lt;=InventoryList!I14:I14)*(InventoryList!L14:L14="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G14:G14)&lt;=_xlfn.SINGLE(InventoryList!I14:I14))*(_xlfn.SINGLE(InventoryList!L14:L14)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C14" s="14"/>
@@ -1957,7 +2010,7 @@
     </row>
     <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G15:G15&lt;=InventoryList!I15:I15)*(InventoryList!L15:L15="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G15:G15)&lt;=_xlfn.SINGLE(InventoryList!I15:I15))*(_xlfn.SINGLE(InventoryList!L15:L15)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C15" s="14"/>
@@ -1977,7 +2030,7 @@
     </row>
     <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G16:G16&lt;=InventoryList!I16:I16)*(InventoryList!L16:L16="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G16:G16)&lt;=_xlfn.SINGLE(InventoryList!I16:I16))*(_xlfn.SINGLE(InventoryList!L16:L16)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C16" s="14"/>
@@ -1997,7 +2050,7 @@
     </row>
     <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G17:G17&lt;=InventoryList!I17:I17)*(InventoryList!L17:L17="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G17:G17)&lt;=_xlfn.SINGLE(InventoryList!I17:I17))*(_xlfn.SINGLE(InventoryList!L17:L17)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C17" s="14"/>
@@ -2017,7 +2070,7 @@
     </row>
     <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G18:G18&lt;=InventoryList!I18:I18)*(InventoryList!L18:L18="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G18:G18)&lt;=_xlfn.SINGLE(InventoryList!I18:I18))*(_xlfn.SINGLE(InventoryList!L18:L18)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C18" s="14"/>
@@ -2037,7 +2090,7 @@
     </row>
     <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G19:G19&lt;=InventoryList!I19:I19)*(InventoryList!L19:L19="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G19:G19)&lt;=_xlfn.SINGLE(InventoryList!I19:I19))*(_xlfn.SINGLE(InventoryList!L19:L19)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C19" s="14"/>
@@ -2057,7 +2110,7 @@
     </row>
     <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G20:G20&lt;=InventoryList!I20:I20)*(InventoryList!L20:L20="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G20:G20)&lt;=_xlfn.SINGLE(InventoryList!I20:I20))*(_xlfn.SINGLE(InventoryList!L20:L20)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C20" s="14"/>
@@ -2077,7 +2130,7 @@
     </row>
     <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G21:G21&lt;=InventoryList!I21:I21)*(InventoryList!L21:L21="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G21:G21)&lt;=_xlfn.SINGLE(InventoryList!I21:I21))*(_xlfn.SINGLE(InventoryList!L21:L21)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C21" s="14"/>
@@ -2097,7 +2150,7 @@
     </row>
     <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G22:G22&lt;=InventoryList!I22:I22)*(InventoryList!L22:L22="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G22:G22)&lt;=_xlfn.SINGLE(InventoryList!I22:I22))*(_xlfn.SINGLE(InventoryList!L22:L22)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C22" s="14"/>
@@ -2117,7 +2170,7 @@
     </row>
     <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G23:G23&lt;=InventoryList!I23:I23)*(InventoryList!L23:L23="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G23:G23)&lt;=_xlfn.SINGLE(InventoryList!I23:I23))*(_xlfn.SINGLE(InventoryList!L23:L23)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C23" s="14"/>
@@ -2137,7 +2190,7 @@
     </row>
     <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G24:G24&lt;=InventoryList!I24:I24)*(InventoryList!L24:L24="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G24:G24)&lt;=_xlfn.SINGLE(InventoryList!I24:I24))*(_xlfn.SINGLE(InventoryList!L24:L24)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C24" s="14"/>
@@ -2157,7 +2210,7 @@
     </row>
     <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G25:G25&lt;=InventoryList!I25:I25)*(InventoryList!L25:L25="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G25:G25)&lt;=_xlfn.SINGLE(InventoryList!I25:I25))*(_xlfn.SINGLE(InventoryList!L25:L25)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C25" s="14"/>
@@ -2177,7 +2230,7 @@
     </row>
     <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G26:G26&lt;=InventoryList!I26:I26)*(InventoryList!L26:L26="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G26:G26)&lt;=_xlfn.SINGLE(InventoryList!I26:I26))*(_xlfn.SINGLE(InventoryList!L26:L26)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C26" s="14"/>
@@ -2197,7 +2250,7 @@
     </row>
     <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G27:G27&lt;=InventoryList!I27:I27)*(InventoryList!L27:L27="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G27:G27)&lt;=_xlfn.SINGLE(InventoryList!I27:I27))*(_xlfn.SINGLE(InventoryList!L27:L27)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C27" s="14"/>
@@ -2217,7 +2270,7 @@
     </row>
     <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G28:G28&lt;=InventoryList!I28:I28)*(InventoryList!L28:L28="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G28:G28)&lt;=_xlfn.SINGLE(InventoryList!I28:I28))*(_xlfn.SINGLE(InventoryList!L28:L28)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C28" s="14"/>
@@ -2237,7 +2290,7 @@
     </row>
     <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G29:G29&lt;=InventoryList!I29:I29)*(InventoryList!L29:L29="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G29:G29)&lt;=_xlfn.SINGLE(InventoryList!I29:I29))*(_xlfn.SINGLE(InventoryList!L29:L29)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C29" s="14"/>
@@ -2257,7 +2310,7 @@
     </row>
     <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G30:G30&lt;=InventoryList!I30:I30)*(InventoryList!L30:L30="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G30:G30)&lt;=_xlfn.SINGLE(InventoryList!I30:I30))*(_xlfn.SINGLE(InventoryList!L30:L30)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C30" s="14"/>
@@ -2277,7 +2330,7 @@
     </row>
     <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G31:G31&lt;=InventoryList!I31:I31)*(InventoryList!L31:L31="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G31:G31)&lt;=_xlfn.SINGLE(InventoryList!I31:I31))*(_xlfn.SINGLE(InventoryList!L31:L31)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C31" s="14"/>
@@ -2297,7 +2350,7 @@
     </row>
     <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G32:G32&lt;=InventoryList!I32:I32)*(InventoryList!L32:L32="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G32:G32)&lt;=_xlfn.SINGLE(InventoryList!I32:I32))*(_xlfn.SINGLE(InventoryList!L32:L32)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C32" s="14"/>
@@ -2317,7 +2370,7 @@
     </row>
     <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G33:G33&lt;=InventoryList!I33:I33)*(InventoryList!L33:L33="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G33:G33)&lt;=_xlfn.SINGLE(InventoryList!I33:I33))*(_xlfn.SINGLE(InventoryList!L33:L33)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C33" s="14"/>
@@ -2337,7 +2390,7 @@
     </row>
     <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G34:G34&lt;=InventoryList!I34:I34)*(InventoryList!L34:L34="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G34:G34)&lt;=_xlfn.SINGLE(InventoryList!I34:I34))*(_xlfn.SINGLE(InventoryList!L34:L34)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C34" s="14"/>
@@ -2357,7 +2410,7 @@
     </row>
     <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G35:G35&lt;=InventoryList!I35:I35)*(InventoryList!L35:L35="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G35:G35)&lt;=_xlfn.SINGLE(InventoryList!I35:I35))*(_xlfn.SINGLE(InventoryList!L35:L35)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C35" s="14"/>
@@ -2377,7 +2430,7 @@
     </row>
     <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G36:G36&lt;=InventoryList!I36:I36)*(InventoryList!L36:L36="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G36:G36)&lt;=_xlfn.SINGLE(InventoryList!I36:I36))*(_xlfn.SINGLE(InventoryList!L36:L36)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C36" s="14"/>
@@ -2397,7 +2450,7 @@
     </row>
     <row r="37" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G37:G37&lt;=InventoryList!I37:I37)*(InventoryList!L37:L37="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G37:G37)&lt;=_xlfn.SINGLE(InventoryList!I37:I37))*(_xlfn.SINGLE(InventoryList!L37:L37)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C37" s="14"/>
@@ -2417,7 +2470,7 @@
     </row>
     <row r="38" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G38:G38&lt;=InventoryList!I38:I38)*(InventoryList!L38:L38="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G38:G38)&lt;=_xlfn.SINGLE(InventoryList!I38:I38))*(_xlfn.SINGLE(InventoryList!L38:L38)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C38" s="14"/>
@@ -2437,7 +2490,7 @@
     </row>
     <row r="39" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G39:G39&lt;=InventoryList!I39:I39)*(InventoryList!L39:L39="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G39:G39)&lt;=_xlfn.SINGLE(InventoryList!I39:I39))*(_xlfn.SINGLE(InventoryList!L39:L39)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C39" s="14"/>
@@ -2457,7 +2510,7 @@
     </row>
     <row r="40" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G40:G40&lt;=InventoryList!I40:I40)*(InventoryList!L40:L40="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G40:G40)&lt;=_xlfn.SINGLE(InventoryList!I40:I40))*(_xlfn.SINGLE(InventoryList!L40:L40)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C40" s="14"/>
@@ -2477,7 +2530,7 @@
     </row>
     <row r="41" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G41:G41&lt;=InventoryList!I41:I41)*(InventoryList!L41:L41="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G41:G41)&lt;=_xlfn.SINGLE(InventoryList!I41:I41))*(_xlfn.SINGLE(InventoryList!L41:L41)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C41" s="14"/>
@@ -2497,7 +2550,7 @@
     </row>
     <row r="42" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G42:G42&lt;=InventoryList!I42:I42)*(InventoryList!L42:L42="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G42:G42)&lt;=_xlfn.SINGLE(InventoryList!I42:I42))*(_xlfn.SINGLE(InventoryList!L42:L42)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C42" s="14"/>
@@ -2517,7 +2570,7 @@
     </row>
     <row r="43" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G43:G43&lt;=InventoryList!I43:I43)*(InventoryList!L43:L43="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G43:G43)&lt;=_xlfn.SINGLE(InventoryList!I43:I43))*(_xlfn.SINGLE(InventoryList!L43:L43)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C43" s="14"/>
@@ -2537,7 +2590,7 @@
     </row>
     <row r="44" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G44:G44&lt;=InventoryList!I44:I44)*(InventoryList!L44:L44="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G44:G44)&lt;=_xlfn.SINGLE(InventoryList!I44:I44))*(_xlfn.SINGLE(InventoryList!L44:L44)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C44" s="14"/>
@@ -2557,7 +2610,7 @@
     </row>
     <row r="45" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G45:G45&lt;=InventoryList!I45:I45)*(InventoryList!L45:L45="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G45:G45)&lt;=_xlfn.SINGLE(InventoryList!I45:I45))*(_xlfn.SINGLE(InventoryList!L45:L45)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C45" s="14"/>
@@ -2577,7 +2630,7 @@
     </row>
     <row r="46" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G46:G46&lt;=InventoryList!I46:I46)*(InventoryList!L46:L46="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G46:G46)&lt;=_xlfn.SINGLE(InventoryList!I46:I46))*(_xlfn.SINGLE(InventoryList!L46:L46)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C46" s="14"/>
@@ -2597,7 +2650,7 @@
     </row>
     <row r="47" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G47:G47&lt;=InventoryList!I47:I47)*(InventoryList!L47:L47="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G47:G47)&lt;=_xlfn.SINGLE(InventoryList!I47:I47))*(_xlfn.SINGLE(InventoryList!L47:L47)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C47" s="14"/>
@@ -2617,7 +2670,7 @@
     </row>
     <row r="48" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G48:G48&lt;=InventoryList!I48:I48)*(InventoryList!L48:L48="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G48:G48)&lt;=_xlfn.SINGLE(InventoryList!I48:I48))*(_xlfn.SINGLE(InventoryList!L48:L48)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C48" s="14"/>
@@ -2637,7 +2690,7 @@
     </row>
     <row r="49" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G49:G49&lt;=InventoryList!I49:I49)*(InventoryList!L49:L49="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G49:G49)&lt;=_xlfn.SINGLE(InventoryList!I49:I49))*(_xlfn.SINGLE(InventoryList!L49:L49)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C49" s="14"/>
@@ -2657,7 +2710,7 @@
     </row>
     <row r="50" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G50:G50&lt;=InventoryList!I50:I50)*(InventoryList!L50:L50="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G50:G50)&lt;=_xlfn.SINGLE(InventoryList!I50:I50))*(_xlfn.SINGLE(InventoryList!L50:L50)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C50" s="14"/>
@@ -2677,7 +2730,7 @@
     </row>
     <row r="51" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G51:G51&lt;=InventoryList!I51:I51)*(InventoryList!L51:L51="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G51:G51)&lt;=_xlfn.SINGLE(InventoryList!I51:I51))*(_xlfn.SINGLE(InventoryList!L51:L51)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C51" s="14"/>
@@ -2697,7 +2750,7 @@
     </row>
     <row r="52" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G52:G52&lt;=InventoryList!I52:I52)*(InventoryList!L52:L52="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G52:G52)&lt;=_xlfn.SINGLE(InventoryList!I52:I52))*(_xlfn.SINGLE(InventoryList!L52:L52)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C52" s="14"/>
@@ -2717,7 +2770,7 @@
     </row>
     <row r="53" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G53:G53&lt;=InventoryList!I53:I53)*(InventoryList!L53:L53="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G53:G53)&lt;=_xlfn.SINGLE(InventoryList!I53:I53))*(_xlfn.SINGLE(InventoryList!L53:L53)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C53" s="14"/>
@@ -2737,7 +2790,7 @@
     </row>
     <row r="54" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G54:G54&lt;=InventoryList!I54:I54)*(InventoryList!L54:L54="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G54:G54)&lt;=_xlfn.SINGLE(InventoryList!I54:I54))*(_xlfn.SINGLE(InventoryList!L54:L54)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C54" s="14"/>
@@ -2757,7 +2810,7 @@
     </row>
     <row r="55" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G55:G55&lt;=InventoryList!I55:I55)*(InventoryList!L55:L55="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G55:G55)&lt;=_xlfn.SINGLE(InventoryList!I55:I55))*(_xlfn.SINGLE(InventoryList!L55:L55)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C55" s="14"/>
@@ -2777,7 +2830,7 @@
     </row>
     <row r="56" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G56:G56&lt;=InventoryList!I56:I56)*(InventoryList!L56:L56="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G56:G56)&lt;=_xlfn.SINGLE(InventoryList!I56:I56))*(_xlfn.SINGLE(InventoryList!L56:L56)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C56" s="14"/>
@@ -2797,7 +2850,7 @@
     </row>
     <row r="57" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G57:G57&lt;=InventoryList!I57:I57)*(InventoryList!L57:L57="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G57:G57)&lt;=_xlfn.SINGLE(InventoryList!I57:I57))*(_xlfn.SINGLE(InventoryList!L57:L57)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C57" s="14"/>
@@ -2817,7 +2870,7 @@
     </row>
     <row r="58" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G58:G58&lt;=InventoryList!I58:I58)*(InventoryList!L58:L58="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G58:G58)&lt;=_xlfn.SINGLE(InventoryList!I58:I58))*(_xlfn.SINGLE(InventoryList!L58:L58)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C58" s="14"/>
@@ -2837,7 +2890,7 @@
     </row>
     <row r="59" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G59:G59&lt;=InventoryList!I59:I59)*(InventoryList!L59:L59="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G59:G59)&lt;=_xlfn.SINGLE(InventoryList!I59:I59))*(_xlfn.SINGLE(InventoryList!L59:L59)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C59" s="14"/>
@@ -2857,7 +2910,7 @@
     </row>
     <row r="60" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G60:G60&lt;=InventoryList!I60:I60)*(InventoryList!L60:L60="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G60:G60)&lt;=_xlfn.SINGLE(InventoryList!I60:I60))*(_xlfn.SINGLE(InventoryList!L60:L60)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C60" s="14"/>
@@ -2877,7 +2930,7 @@
     </row>
     <row r="61" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G61:G61&lt;=InventoryList!I61:I61)*(InventoryList!L61:L61="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G61:G61)&lt;=_xlfn.SINGLE(InventoryList!I61:I61))*(_xlfn.SINGLE(InventoryList!L61:L61)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C61" s="14"/>
@@ -2897,7 +2950,7 @@
     </row>
     <row r="62" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G62:G62&lt;=InventoryList!I62:I62)*(InventoryList!L62:L62="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G62:G62)&lt;=_xlfn.SINGLE(InventoryList!I62:I62))*(_xlfn.SINGLE(InventoryList!L62:L62)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C62" s="14"/>
@@ -2917,7 +2970,7 @@
     </row>
     <row r="63" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G63:G63&lt;=InventoryList!I63:I63)*(InventoryList!L63:L63="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G63:G63)&lt;=_xlfn.SINGLE(InventoryList!I63:I63))*(_xlfn.SINGLE(InventoryList!L63:L63)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C63" s="14"/>
@@ -2937,7 +2990,7 @@
     </row>
     <row r="64" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G64:G64&lt;=InventoryList!I64:I64)*(InventoryList!L64:L64="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G64:G64)&lt;=_xlfn.SINGLE(InventoryList!I64:I64))*(_xlfn.SINGLE(InventoryList!L64:L64)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C64" s="14"/>
@@ -2957,7 +3010,7 @@
     </row>
     <row r="65" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G65:G65&lt;=InventoryList!I65:I65)*(InventoryList!L65:L65="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G65:G65)&lt;=_xlfn.SINGLE(InventoryList!I65:I65))*(_xlfn.SINGLE(InventoryList!L65:L65)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C65" s="14"/>
@@ -2977,7 +3030,7 @@
     </row>
     <row r="66" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G66:G66&lt;=InventoryList!I66:I66)*(InventoryList!L66:L66="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G66:G66)&lt;=_xlfn.SINGLE(InventoryList!I66:I66))*(_xlfn.SINGLE(InventoryList!L66:L66)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C66" s="14"/>
@@ -2997,7 +3050,7 @@
     </row>
     <row r="67" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G67:G67&lt;=InventoryList!I67:I67)*(InventoryList!L67:L67="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G67:G67)&lt;=_xlfn.SINGLE(InventoryList!I67:I67))*(_xlfn.SINGLE(InventoryList!L67:L67)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C67" s="14"/>
@@ -3017,7 +3070,7 @@
     </row>
     <row r="68" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G68:G68&lt;=InventoryList!I68:I68)*(InventoryList!L68:L68="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G68:G68)&lt;=_xlfn.SINGLE(InventoryList!I68:I68))*(_xlfn.SINGLE(InventoryList!L68:L68)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C68" s="14"/>
@@ -3037,7 +3090,7 @@
     </row>
     <row r="69" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G69:G69&lt;=InventoryList!I69:I69)*(InventoryList!L69:L69="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G69:G69)&lt;=_xlfn.SINGLE(InventoryList!I69:I69))*(_xlfn.SINGLE(InventoryList!L69:L69)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C69" s="14"/>
@@ -3057,7 +3110,7 @@
     </row>
     <row r="70" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G70:G70&lt;=InventoryList!I70:I70)*(InventoryList!L70:L70="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G70:G70)&lt;=_xlfn.SINGLE(InventoryList!I70:I70))*(_xlfn.SINGLE(InventoryList!L70:L70)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C70" s="14"/>
@@ -3077,7 +3130,7 @@
     </row>
     <row r="71" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G71:G71&lt;=InventoryList!I71:I71)*(InventoryList!L71:L71="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G71:G71)&lt;=_xlfn.SINGLE(InventoryList!I71:I71))*(_xlfn.SINGLE(InventoryList!L71:L71)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C71" s="14"/>
@@ -3097,7 +3150,7 @@
     </row>
     <row r="72" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G72:G72&lt;=InventoryList!I72:I72)*(InventoryList!L72:L72="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G72:G72)&lt;=_xlfn.SINGLE(InventoryList!I72:I72))*(_xlfn.SINGLE(InventoryList!L72:L72)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C72" s="14"/>
@@ -3117,7 +3170,7 @@
     </row>
     <row r="73" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G73:G73&lt;=InventoryList!I73:I73)*(InventoryList!L73:L73="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G73:G73)&lt;=_xlfn.SINGLE(InventoryList!I73:I73))*(_xlfn.SINGLE(InventoryList!L73:L73)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C73" s="14"/>
@@ -3137,7 +3190,7 @@
     </row>
     <row r="74" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G74:G74&lt;=InventoryList!I74:I74)*(InventoryList!L74:L74="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G74:G74)&lt;=_xlfn.SINGLE(InventoryList!I74:I74))*(_xlfn.SINGLE(InventoryList!L74:L74)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C74" s="14"/>
@@ -3157,7 +3210,7 @@
     </row>
     <row r="75" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G75:G75&lt;=InventoryList!I75:I75)*(InventoryList!L75:L75="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G75:G75)&lt;=_xlfn.SINGLE(InventoryList!I75:I75))*(_xlfn.SINGLE(InventoryList!L75:L75)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C75" s="14"/>
@@ -3177,7 +3230,7 @@
     </row>
     <row r="76" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G76:G76&lt;=InventoryList!I76:I76)*(InventoryList!L76:L76="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G76:G76)&lt;=_xlfn.SINGLE(InventoryList!I76:I76))*(_xlfn.SINGLE(InventoryList!L76:L76)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C76" s="14"/>
@@ -3197,7 +3250,7 @@
     </row>
     <row r="77" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G77:G77&lt;=InventoryList!I77:I77)*(InventoryList!L77:L77="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G77:G77)&lt;=_xlfn.SINGLE(InventoryList!I77:I77))*(_xlfn.SINGLE(InventoryList!L77:L77)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C77" s="14"/>
@@ -3217,7 +3270,7 @@
     </row>
     <row r="78" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G78:G78&lt;=InventoryList!I78:I78)*(InventoryList!L78:L78="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G78:G78)&lt;=_xlfn.SINGLE(InventoryList!I78:I78))*(_xlfn.SINGLE(InventoryList!L78:L78)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C78" s="14"/>
@@ -3237,7 +3290,7 @@
     </row>
     <row r="79" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G79:G79&lt;=InventoryList!I79:I79)*(InventoryList!L79:L79="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G79:G79)&lt;=_xlfn.SINGLE(InventoryList!I79:I79))*(_xlfn.SINGLE(InventoryList!L79:L79)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C79" s="14"/>
@@ -3257,7 +3310,7 @@
     </row>
     <row r="80" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G80:G80&lt;=InventoryList!I80:I80)*(InventoryList!L80:L80="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G80:G80)&lt;=_xlfn.SINGLE(InventoryList!I80:I80))*(_xlfn.SINGLE(InventoryList!L80:L80)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C80" s="14"/>
@@ -3277,7 +3330,7 @@
     </row>
     <row r="81" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G81:G81&lt;=InventoryList!I81:I81)*(InventoryList!L81:L81="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G81:G81)&lt;=_xlfn.SINGLE(InventoryList!I81:I81))*(_xlfn.SINGLE(InventoryList!L81:L81)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C81" s="14"/>
@@ -3297,7 +3350,7 @@
     </row>
     <row r="82" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G82:G82&lt;=InventoryList!I82:I82)*(InventoryList!L82:L82="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G82:G82)&lt;=_xlfn.SINGLE(InventoryList!I82:I82))*(_xlfn.SINGLE(InventoryList!L82:L82)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C82" s="14"/>
@@ -3317,7 +3370,7 @@
     </row>
     <row r="83" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G83:G83&lt;=InventoryList!I83:I83)*(InventoryList!L83:L83="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G83:G83)&lt;=_xlfn.SINGLE(InventoryList!I83:I83))*(_xlfn.SINGLE(InventoryList!L83:L83)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C83" s="14"/>
@@ -3337,7 +3390,7 @@
     </row>
     <row r="84" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G84:G84&lt;=InventoryList!I84:I84)*(InventoryList!L84:L84="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G84:G84)&lt;=_xlfn.SINGLE(InventoryList!I84:I84))*(_xlfn.SINGLE(InventoryList!L84:L84)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C84" s="14"/>
@@ -3357,7 +3410,7 @@
     </row>
     <row r="85" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G85:G85&lt;=InventoryList!I85:I85)*(InventoryList!L85:L85="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G85:G85)&lt;=_xlfn.SINGLE(InventoryList!I85:I85))*(_xlfn.SINGLE(InventoryList!L85:L85)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C85" s="14"/>
@@ -3377,7 +3430,7 @@
     </row>
     <row r="86" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G86:G86&lt;=InventoryList!I86:I86)*(InventoryList!L86:L86="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G86:G86)&lt;=_xlfn.SINGLE(InventoryList!I86:I86))*(_xlfn.SINGLE(InventoryList!L86:L86)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C86" s="14"/>
@@ -3397,7 +3450,7 @@
     </row>
     <row r="87" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G87:G87&lt;=InventoryList!I87:I87)*(InventoryList!L87:L87="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G87:G87)&lt;=_xlfn.SINGLE(InventoryList!I87:I87))*(_xlfn.SINGLE(InventoryList!L87:L87)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C87" s="14"/>
@@ -3417,7 +3470,7 @@
     </row>
     <row r="88" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G88:G88&lt;=InventoryList!I88:I88)*(InventoryList!L88:L88="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G88:G88)&lt;=_xlfn.SINGLE(InventoryList!I88:I88))*(_xlfn.SINGLE(InventoryList!L88:L88)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C88" s="14"/>
@@ -3437,7 +3490,7 @@
     </row>
     <row r="89" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G89:G89&lt;=InventoryList!I89:I89)*(InventoryList!L89:L89="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G89:G89)&lt;=_xlfn.SINGLE(InventoryList!I89:I89))*(_xlfn.SINGLE(InventoryList!L89:L89)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C89" s="14"/>
@@ -3457,7 +3510,7 @@
     </row>
     <row r="90" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G90:G90&lt;=InventoryList!I90:I90)*(InventoryList!L90:L90="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G90:G90)&lt;=_xlfn.SINGLE(InventoryList!I90:I90))*(_xlfn.SINGLE(InventoryList!L90:L90)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C90" s="14"/>
@@ -3477,7 +3530,7 @@
     </row>
     <row r="91" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G91:G91&lt;=InventoryList!I91:I91)*(InventoryList!L91:L91="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G91:G91)&lt;=_xlfn.SINGLE(InventoryList!I91:I91))*(_xlfn.SINGLE(InventoryList!L91:L91)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C91" s="14"/>
@@ -3497,7 +3550,7 @@
     </row>
     <row r="92" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G92:G92&lt;=InventoryList!I92:I92)*(InventoryList!L92:L92="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G92:G92)&lt;=_xlfn.SINGLE(InventoryList!I92:I92))*(_xlfn.SINGLE(InventoryList!L92:L92)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C92" s="14"/>
@@ -3517,7 +3570,7 @@
     </row>
     <row r="93" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G93:G93&lt;=InventoryList!I93:I93)*(InventoryList!L93:L93="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G93:G93)&lt;=_xlfn.SINGLE(InventoryList!I93:I93))*(_xlfn.SINGLE(InventoryList!L93:L93)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C93" s="14"/>
@@ -3537,7 +3590,7 @@
     </row>
     <row r="94" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G94:G94&lt;=InventoryList!I94:I94)*(InventoryList!L94:L94="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G94:G94)&lt;=_xlfn.SINGLE(InventoryList!I94:I94))*(_xlfn.SINGLE(InventoryList!L94:L94)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C94" s="14"/>
@@ -3557,7 +3610,7 @@
     </row>
     <row r="95" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G95:G95&lt;=InventoryList!I95:I95)*(InventoryList!L95:L95="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G95:G95)&lt;=_xlfn.SINGLE(InventoryList!I95:I95))*(_xlfn.SINGLE(InventoryList!L95:L95)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C95" s="14"/>
@@ -3577,7 +3630,7 @@
     </row>
     <row r="96" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G96:G96&lt;=InventoryList!I96:I96)*(InventoryList!L96:L96="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G96:G96)&lt;=_xlfn.SINGLE(InventoryList!I96:I96))*(_xlfn.SINGLE(InventoryList!L96:L96)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C96" s="14"/>
@@ -3597,7 +3650,7 @@
     </row>
     <row r="97" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G97:G97&lt;=InventoryList!I97:I97)*(InventoryList!L97:L97="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G97:G97)&lt;=_xlfn.SINGLE(InventoryList!I97:I97))*(_xlfn.SINGLE(InventoryList!L97:L97)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C97" s="14"/>
@@ -3617,7 +3670,7 @@
     </row>
     <row r="98" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="13">
-        <f>ЕСЛИОШИБКА((InventoryList!G98:G98&lt;=InventoryList!I98:I98)*(InventoryList!L98:L98="")*valHighlight,0)</f>
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G98:G98)&lt;=_xlfn.SINGLE(InventoryList!I98:I98))*(_xlfn.SINGLE(InventoryList!L98:L98)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
       <c r="C98" s="14"/>
@@ -3700,12 +3753,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3917,18 +3970,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3954,11 +4009,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Nomenclature complete ? maybe need fix
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4658B34A-33AF-4069-8387-C001E4CDAC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2959278-3C4A-44FD-9CB4-1947A6287A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="1350" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -738,19 +738,6 @@
   </cellStyles>
   <dxfs count="31">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-        <color theme="1" tint="0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1197,6 +1184,19 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1403,25 +1403,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M100" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M100" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="B3:M100" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ідентифікатор товару" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Назва" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Постачальник" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Ціна за одиницю" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Кількість на складі" dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Вартість запасів" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ідентифікатор товару" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Назва" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Постачальник" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Ціна за одиницю" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Кількість на складі" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Вартість запасів" dataDxfId="11" totalsRowDxfId="10">
       <calculatedColumnFormula>Таблиця_Інвентарного_Списку[[#This Row],[Ціна за одиницю]]*Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Нижня межа поповнення" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Інтервал поповнення в днях" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Кількість для поповнення" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Вилучено?" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{161F85EE-351B-4E90-B245-0F800118DEC0}" name="Група" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Нижня межа поповнення" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Інтервал поповнення в днях" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Кількість для поповнення" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Вилучено?" totalsRowFunction="count" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{161F85EE-351B-4E90-B245-0F800118DEC0}" name="Група" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Таблиця показників організації" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1633,7 +1633,7 @@
   <dimension ref="B1:M98"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B98"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1868,11 +1868,11 @@
         <v>3</v>
       </c>
       <c r="G8" s="16" t="n">
-        <v>157.0</v>
+        <v>130.0</v>
       </c>
       <c r="H8" s="15">
         <f>(InventoryList!F8:F8*InventoryList!G8:G8)</f>
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="I8" s="16">
         <v>3</v>
@@ -1880,8 +1880,8 @@
       <c r="J8" s="16">
         <v>3</v>
       </c>
-      <c r="K8" s="16" t="n">
-        <v>1.0</v>
+      <c r="K8" s="16">
+        <v>1</v>
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="17" t="s">
@@ -3691,10 +3691,10 @@
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="B4:M98">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="27" priority="1">
       <formula>#REF!="Так"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="26" priority="2">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3753,12 +3753,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3970,20 +3970,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4009,9 +4007,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
+ Find by name
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2959278-3C4A-44FD-9CB4-1947A6287A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBBC284-205A-48B4-9585-544FDF853413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="1350" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32610" yWindow="2235" windowWidth="24990" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,9 @@
     <definedName name="valHighlight">IFERROR(IF(InventoryList!$L$2="Так", TRUE, FALSE),FALSE)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">InventoryList!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="true"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,9 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
-  <si>
-    <t>Для нижньої межі</t>
-  </si>
   <si>
     <t>Ідентифікатор товару</t>
   </si>
@@ -115,6 +112,9 @@
   <si>
     <t>Sup3</t>
   </si>
+  <si>
+    <t>Менше нижньої межі</t>
+  </si>
 </sst>
 </file>
 
@@ -127,7 +127,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0.00&quot;₴&quot;"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +286,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Franklin Gothic Book"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -635,7 +643,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -686,6 +694,25 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% — акцент1" xfId="24" builtinId="30" customBuiltin="1"/>
@@ -1403,10 +1430,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M100" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="B3:M100" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Таблиця_Інвентарного_Списку" displayName="Таблиця_Інвентарного_Списку" ref="B3:M98" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="B3:M98" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Для нижньої межі" totalsRowLabel="Підсумок" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Менше нижньої межі" totalsRowLabel="Підсумок" dataDxfId="23" totalsRowDxfId="22">
       <calculatedColumnFormula>IFERROR((Таблиця_Інвентарного_Списку[[#This Row],[Кількість на складі]]&lt;=Таблиця_Інвентарного_Списку[[#This Row],[Нижня межа поповнення]])*(Таблиця_Інвентарного_Списку[[#This Row],[Вилучено?]]="")*valHighlight,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Ідентифікатор товару" dataDxfId="21" totalsRowDxfId="20"/>
@@ -1630,27 +1657,27 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M98"/>
+  <dimension ref="B1:M101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="4" width="1.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="3" width="11.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="6" width="12.77734375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="6" width="16.77734375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="8" width="13.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="8" width="12.33203125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="8" width="11.44140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="8" width="15.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="8" width="11.88671875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="8" width="14.77734375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="6" width="12.77734375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.5546875" collapsed="true"/>
-    <col min="14" max="16384" style="4" width="8.77734375" collapsed="true"/>
+    <col min="1" max="1" width="1.77734375" style="4" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.5546875" style="3" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="16.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.109375" style="8" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.33203125" style="8" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.44140625" style="8" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" style="8" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.88671875" style="8" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.77734375" style="8" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.77734375" style="6" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12.5546875" style="4" customWidth="1" collapsed="1"/>
+    <col min="14" max="16384" width="8.77734375" style="4" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1662,7 +1689,7 @@
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1671,48 +1698,48 @@
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="2:13" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="9" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1721,29 +1748,30 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
       <c r="F4" s="12">
         <v>1</v>
       </c>
+      <c r="G4" s="18"/>
       <c r="H4" s="12">
         <f>(InventoryList!F4:F4*InventoryList!G4:G4)</f>
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="24">
         <v>1</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1752,22 +1780,23 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="12">
         <v>1</v>
       </c>
+      <c r="G5" s="18"/>
       <c r="H5" s="12">
         <f>(InventoryList!F5:F5*InventoryList!G5:G5)</f>
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="24">
         <v>1</v>
       </c>
       <c r="J5">
@@ -1775,7 +1804,7 @@
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1783,33 +1812,33 @@
         <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G6:G6)&lt;=_xlfn.SINGLE(InventoryList!I6:I6))*(_xlfn.SINGLE(InventoryList!L6:L6)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>1</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>20</v>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F6" s="15">
         <v>1</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
       <c r="H6" s="15">
         <f>(InventoryList!F6:F6*InventoryList!G6:G6)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="24">
         <v>1</v>
       </c>
       <c r="J6" s="16">
         <v>1</v>
       </c>
       <c r="K6" s="16"/>
-      <c r="L6" s="14"/>
+      <c r="L6" s="8"/>
       <c r="M6" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1817,26 +1846,26 @@
         <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G7:G7)&lt;=_xlfn.SINGLE(InventoryList!I7:I7))*(_xlfn.SINGLE(InventoryList!L7:L7)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>0</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="15">
         <v>1</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="18">
         <v>45</v>
       </c>
       <c r="H7" s="15">
         <f>(InventoryList!F7:F7*InventoryList!G7:G7)</f>
         <v>45</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="24">
         <v>1</v>
       </c>
       <c r="J7" s="16">
@@ -1845,9 +1874,9 @@
       <c r="K7" s="16">
         <v>12</v>
       </c>
-      <c r="L7" s="14"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1855,27 +1884,27 @@
         <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G8:G8)&lt;=_xlfn.SINGLE(InventoryList!I8:I8))*(_xlfn.SINGLE(InventoryList!L8:L8)="")*_xlfn.SINGLE(valHighlight),0))</f>
         <v>0</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>25</v>
       </c>
       <c r="F8" s="15">
         <v>3</v>
       </c>
-      <c r="G8" s="16" t="n">
-        <v>130.0</v>
+      <c r="G8" s="18">
+        <v>130</v>
       </c>
       <c r="H8" s="15">
         <f>(InventoryList!F8:F8*InventoryList!G8:G8)</f>
-        <v>471</v>
-      </c>
-      <c r="I8" s="16">
-        <v>3</v>
+        <v>390</v>
+      </c>
+      <c r="I8" s="24">
+        <v>1</v>
       </c>
       <c r="J8" s="16">
         <v>3</v>
@@ -1883,9 +1912,9 @@
       <c r="K8" s="16">
         <v>1</v>
       </c>
-      <c r="L8" s="14"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1897,15 +1926,15 @@
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="15">
         <f>(InventoryList!F9:F9*InventoryList!G9:G9)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="16"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
-      <c r="L9" s="14"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="17"/>
     </row>
     <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1917,15 +1946,15 @@
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="F10" s="15"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="15">
         <f>(InventoryList!F10:F10*InventoryList!G10:G10)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="16"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="14"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="17"/>
     </row>
     <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1937,15 +1966,15 @@
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="16"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="15">
         <f>(InventoryList!F11:F11*InventoryList!G11:G11)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="16"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="14"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="17"/>
     </row>
     <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1957,15 +1986,15 @@
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
       <c r="F12" s="15"/>
-      <c r="G12" s="16"/>
+      <c r="G12" s="18"/>
       <c r="H12" s="15">
         <f>(InventoryList!F12:F12*InventoryList!G12:G12)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="16"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="14"/>
+      <c r="L12" s="8"/>
       <c r="M12" s="17"/>
     </row>
     <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1977,15 +2006,15 @@
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
+      <c r="G13" s="18"/>
       <c r="H13" s="15">
         <f>(InventoryList!F13:F13*InventoryList!G13:G13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="16"/>
+      <c r="I13" s="24"/>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
-      <c r="L13" s="14"/>
+      <c r="L13" s="8"/>
       <c r="M13" s="17"/>
     </row>
     <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1997,15 +2026,15 @@
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
       <c r="F14" s="15"/>
-      <c r="G14" s="16"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="15">
         <f>(InventoryList!F14:F14*InventoryList!G14:G14)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="16"/>
+      <c r="I14" s="24"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
-      <c r="L14" s="14"/>
+      <c r="L14" s="8"/>
       <c r="M14" s="17"/>
     </row>
     <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2017,15 +2046,15 @@
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
       <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="15">
         <f>(InventoryList!F15:F15*InventoryList!G15:G15)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="16"/>
+      <c r="I15" s="24"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="14"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="17"/>
     </row>
     <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2037,15 +2066,15 @@
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="16"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="15">
         <f>(InventoryList!F16:F16*InventoryList!G16:G16)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="16"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
-      <c r="L16" s="14"/>
+      <c r="L16" s="8"/>
       <c r="M16" s="17"/>
     </row>
     <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2057,15 +2086,15 @@
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
       <c r="F17" s="15"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="18"/>
       <c r="H17" s="15">
         <f>(InventoryList!F17:F17*InventoryList!G17:G17)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="16"/>
+      <c r="I17" s="24"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="14"/>
+      <c r="L17" s="8"/>
       <c r="M17" s="17"/>
     </row>
     <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2077,15 +2106,15 @@
       <c r="D18" s="14"/>
       <c r="E18" s="14"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="16"/>
+      <c r="G18" s="18"/>
       <c r="H18" s="15">
         <f>(InventoryList!F18:F18*InventoryList!G18:G18)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="16"/>
+      <c r="I18" s="24"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="14"/>
+      <c r="L18" s="8"/>
       <c r="M18" s="17"/>
     </row>
     <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2097,15 +2126,15 @@
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="16"/>
+      <c r="G19" s="18"/>
       <c r="H19" s="15">
         <f>(InventoryList!F19:F19*InventoryList!G19:G19)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="16"/>
+      <c r="I19" s="24"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
-      <c r="L19" s="14"/>
+      <c r="L19" s="8"/>
       <c r="M19" s="17"/>
     </row>
     <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2117,15 +2146,15 @@
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
+      <c r="G20" s="18"/>
       <c r="H20" s="15">
         <f>(InventoryList!F20:F20*InventoryList!G20:G20)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="16"/>
+      <c r="I20" s="24"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
-      <c r="L20" s="14"/>
+      <c r="L20" s="8"/>
       <c r="M20" s="17"/>
     </row>
     <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2137,15 +2166,15 @@
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="15">
         <f>(InventoryList!F21:F21*InventoryList!G21:G21)</f>
         <v>0</v>
       </c>
-      <c r="I21" s="16"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
-      <c r="L21" s="14"/>
+      <c r="L21" s="8"/>
       <c r="M21" s="17"/>
     </row>
     <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2157,15 +2186,15 @@
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
+      <c r="G22" s="18"/>
       <c r="H22" s="15">
         <f>(InventoryList!F22:F22*InventoryList!G22:G22)</f>
         <v>0</v>
       </c>
-      <c r="I22" s="16"/>
+      <c r="I22" s="24"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="14"/>
+      <c r="L22" s="8"/>
       <c r="M22" s="17"/>
     </row>
     <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2177,15 +2206,15 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
+      <c r="G23" s="18"/>
       <c r="H23" s="15">
         <f>(InventoryList!F23:F23*InventoryList!G23:G23)</f>
         <v>0</v>
       </c>
-      <c r="I23" s="16"/>
+      <c r="I23" s="24"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
-      <c r="L23" s="14"/>
+      <c r="L23" s="8"/>
       <c r="M23" s="17"/>
     </row>
     <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2197,15 +2226,15 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="15">
         <f>(InventoryList!F24:F24*InventoryList!G24:G24)</f>
         <v>0</v>
       </c>
-      <c r="I24" s="16"/>
+      <c r="I24" s="24"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="14"/>
+      <c r="L24" s="8"/>
       <c r="M24" s="17"/>
     </row>
     <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2217,15 +2246,15 @@
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
+      <c r="G25" s="18"/>
       <c r="H25" s="15">
         <f>(InventoryList!F25:F25*InventoryList!G25:G25)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="16"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
-      <c r="L25" s="14"/>
+      <c r="L25" s="8"/>
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2237,15 +2266,15 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="16"/>
+      <c r="G26" s="18"/>
       <c r="H26" s="15">
         <f>(InventoryList!F26:F26*InventoryList!G26:G26)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="16"/>
+      <c r="I26" s="24"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="14"/>
+      <c r="L26" s="8"/>
       <c r="M26" s="17"/>
     </row>
     <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2257,15 +2286,15 @@
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="16"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="15">
         <f>(InventoryList!F27:F27*InventoryList!G27:G27)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="16"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
-      <c r="L27" s="14"/>
+      <c r="L27" s="8"/>
       <c r="M27" s="17"/>
     </row>
     <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2277,15 +2306,15 @@
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="16"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="15">
         <f>(InventoryList!F28:F28*InventoryList!G28:G28)</f>
         <v>0</v>
       </c>
-      <c r="I28" s="16"/>
+      <c r="I28" s="24"/>
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
-      <c r="L28" s="14"/>
+      <c r="L28" s="8"/>
       <c r="M28" s="17"/>
     </row>
     <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2297,15 +2326,15 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="16"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="15">
         <f>(InventoryList!F29:F29*InventoryList!G29:G29)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="16"/>
+      <c r="I29" s="24"/>
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
-      <c r="L29" s="14"/>
+      <c r="L29" s="8"/>
       <c r="M29" s="17"/>
     </row>
     <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2317,15 +2346,15 @@
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="16"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="15">
         <f>(InventoryList!F30:F30*InventoryList!G30:G30)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="16"/>
+      <c r="I30" s="24"/>
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
-      <c r="L30" s="14"/>
+      <c r="L30" s="8"/>
       <c r="M30" s="17"/>
     </row>
     <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2337,15 +2366,15 @@
       <c r="D31" s="14"/>
       <c r="E31" s="14"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="16"/>
+      <c r="G31" s="18"/>
       <c r="H31" s="15">
         <f>(InventoryList!F31:F31*InventoryList!G31:G31)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="16"/>
+      <c r="I31" s="24"/>
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
-      <c r="L31" s="14"/>
+      <c r="L31" s="8"/>
       <c r="M31" s="17"/>
     </row>
     <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2357,15 +2386,15 @@
       <c r="D32" s="14"/>
       <c r="E32" s="14"/>
       <c r="F32" s="15"/>
-      <c r="G32" s="16"/>
+      <c r="G32" s="18"/>
       <c r="H32" s="15">
         <f>(InventoryList!F32:F32*InventoryList!G32:G32)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="16"/>
+      <c r="I32" s="24"/>
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
-      <c r="L32" s="14"/>
+      <c r="L32" s="8"/>
       <c r="M32" s="17"/>
     </row>
     <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2377,15 +2406,15 @@
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
       <c r="F33" s="15"/>
-      <c r="G33" s="16"/>
+      <c r="G33" s="18"/>
       <c r="H33" s="15">
         <f>(InventoryList!F33:F33*InventoryList!G33:G33)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="16"/>
+      <c r="I33" s="24"/>
       <c r="J33" s="16"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="14"/>
+      <c r="L33" s="8"/>
       <c r="M33" s="17"/>
     </row>
     <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2397,15 +2426,15 @@
       <c r="D34" s="14"/>
       <c r="E34" s="14"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
+      <c r="G34" s="18"/>
       <c r="H34" s="15">
         <f>(InventoryList!F34:F34*InventoryList!G34:G34)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="16"/>
+      <c r="I34" s="24"/>
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
-      <c r="L34" s="14"/>
+      <c r="L34" s="8"/>
       <c r="M34" s="17"/>
     </row>
     <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2417,15 +2446,15 @@
       <c r="D35" s="14"/>
       <c r="E35" s="14"/>
       <c r="F35" s="15"/>
-      <c r="G35" s="16"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="15">
         <f>(InventoryList!F35:F35*InventoryList!G35:G35)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="16"/>
+      <c r="I35" s="24"/>
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
-      <c r="L35" s="14"/>
+      <c r="L35" s="8"/>
       <c r="M35" s="17"/>
     </row>
     <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2437,15 +2466,15 @@
       <c r="D36" s="14"/>
       <c r="E36" s="14"/>
       <c r="F36" s="15"/>
-      <c r="G36" s="16"/>
+      <c r="G36" s="18"/>
       <c r="H36" s="15">
         <f>(InventoryList!F36:F36*InventoryList!G36:G36)</f>
         <v>0</v>
       </c>
-      <c r="I36" s="16"/>
+      <c r="I36" s="24"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="14"/>
+      <c r="L36" s="8"/>
       <c r="M36" s="17"/>
     </row>
     <row r="37" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2457,15 +2486,15 @@
       <c r="D37" s="14"/>
       <c r="E37" s="14"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="16"/>
+      <c r="G37" s="18"/>
       <c r="H37" s="15">
         <f>(InventoryList!F37:F37*InventoryList!G37:G37)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="16"/>
+      <c r="I37" s="24"/>
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
-      <c r="L37" s="14"/>
+      <c r="L37" s="8"/>
       <c r="M37" s="17"/>
     </row>
     <row r="38" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2477,15 +2506,15 @@
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
+      <c r="G38" s="18"/>
       <c r="H38" s="15">
         <f>(InventoryList!F38:F38*InventoryList!G38:G38)</f>
         <v>0</v>
       </c>
-      <c r="I38" s="16"/>
+      <c r="I38" s="24"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
-      <c r="L38" s="14"/>
+      <c r="L38" s="8"/>
       <c r="M38" s="17"/>
     </row>
     <row r="39" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2497,15 +2526,15 @@
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="15"/>
-      <c r="G39" s="16"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="15">
         <f>(InventoryList!F39:F39*InventoryList!G39:G39)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="16"/>
+      <c r="I39" s="24"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
-      <c r="L39" s="14"/>
+      <c r="L39" s="8"/>
       <c r="M39" s="17"/>
     </row>
     <row r="40" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2517,15 +2546,15 @@
       <c r="D40" s="14"/>
       <c r="E40" s="14"/>
       <c r="F40" s="15"/>
-      <c r="G40" s="16"/>
+      <c r="G40" s="18"/>
       <c r="H40" s="15">
         <f>(InventoryList!F40:F40*InventoryList!G40:G40)</f>
         <v>0</v>
       </c>
-      <c r="I40" s="16"/>
+      <c r="I40" s="24"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
-      <c r="L40" s="14"/>
+      <c r="L40" s="8"/>
       <c r="M40" s="17"/>
     </row>
     <row r="41" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2537,15 +2566,15 @@
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="15"/>
-      <c r="G41" s="16"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="15">
         <f>(InventoryList!F41:F41*InventoryList!G41:G41)</f>
         <v>0</v>
       </c>
-      <c r="I41" s="16"/>
+      <c r="I41" s="24"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
-      <c r="L41" s="14"/>
+      <c r="L41" s="8"/>
       <c r="M41" s="17"/>
     </row>
     <row r="42" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2557,15 +2586,15 @@
       <c r="D42" s="14"/>
       <c r="E42" s="14"/>
       <c r="F42" s="15"/>
-      <c r="G42" s="16"/>
+      <c r="G42" s="18"/>
       <c r="H42" s="15">
         <f>(InventoryList!F42:F42*InventoryList!G42:G42)</f>
         <v>0</v>
       </c>
-      <c r="I42" s="16"/>
+      <c r="I42" s="24"/>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
-      <c r="L42" s="14"/>
+      <c r="L42" s="8"/>
       <c r="M42" s="17"/>
     </row>
     <row r="43" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2577,15 +2606,15 @@
       <c r="D43" s="14"/>
       <c r="E43" s="14"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="16"/>
+      <c r="G43" s="18"/>
       <c r="H43" s="15">
         <f>(InventoryList!F43:F43*InventoryList!G43:G43)</f>
         <v>0</v>
       </c>
-      <c r="I43" s="16"/>
+      <c r="I43" s="24"/>
       <c r="J43" s="16"/>
       <c r="K43" s="16"/>
-      <c r="L43" s="14"/>
+      <c r="L43" s="8"/>
       <c r="M43" s="17"/>
     </row>
     <row r="44" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2597,15 +2626,15 @@
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
       <c r="F44" s="15"/>
-      <c r="G44" s="16"/>
+      <c r="G44" s="18"/>
       <c r="H44" s="15">
         <f>(InventoryList!F44:F44*InventoryList!G44:G44)</f>
         <v>0</v>
       </c>
-      <c r="I44" s="16"/>
+      <c r="I44" s="24"/>
       <c r="J44" s="16"/>
       <c r="K44" s="16"/>
-      <c r="L44" s="14"/>
+      <c r="L44" s="8"/>
       <c r="M44" s="17"/>
     </row>
     <row r="45" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2617,15 +2646,15 @@
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
       <c r="F45" s="15"/>
-      <c r="G45" s="16"/>
+      <c r="G45" s="18"/>
       <c r="H45" s="15">
         <f>(InventoryList!F45:F45*InventoryList!G45:G45)</f>
         <v>0</v>
       </c>
-      <c r="I45" s="16"/>
+      <c r="I45" s="24"/>
       <c r="J45" s="16"/>
       <c r="K45" s="16"/>
-      <c r="L45" s="14"/>
+      <c r="L45" s="8"/>
       <c r="M45" s="17"/>
     </row>
     <row r="46" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2637,15 +2666,15 @@
       <c r="D46" s="14"/>
       <c r="E46" s="14"/>
       <c r="F46" s="15"/>
-      <c r="G46" s="16"/>
+      <c r="G46" s="18"/>
       <c r="H46" s="15">
         <f>(InventoryList!F46:F46*InventoryList!G46:G46)</f>
         <v>0</v>
       </c>
-      <c r="I46" s="16"/>
+      <c r="I46" s="24"/>
       <c r="J46" s="16"/>
       <c r="K46" s="16"/>
-      <c r="L46" s="14"/>
+      <c r="L46" s="8"/>
       <c r="M46" s="17"/>
     </row>
     <row r="47" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2657,15 +2686,15 @@
       <c r="D47" s="14"/>
       <c r="E47" s="14"/>
       <c r="F47" s="15"/>
-      <c r="G47" s="16"/>
+      <c r="G47" s="18"/>
       <c r="H47" s="15">
         <f>(InventoryList!F47:F47*InventoryList!G47:G47)</f>
         <v>0</v>
       </c>
-      <c r="I47" s="16"/>
+      <c r="I47" s="24"/>
       <c r="J47" s="16"/>
       <c r="K47" s="16"/>
-      <c r="L47" s="14"/>
+      <c r="L47" s="8"/>
       <c r="M47" s="17"/>
     </row>
     <row r="48" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2677,15 +2706,15 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="15"/>
-      <c r="G48" s="16"/>
+      <c r="G48" s="18"/>
       <c r="H48" s="15">
         <f>(InventoryList!F48:F48*InventoryList!G48:G48)</f>
         <v>0</v>
       </c>
-      <c r="I48" s="16"/>
+      <c r="I48" s="24"/>
       <c r="J48" s="16"/>
       <c r="K48" s="16"/>
-      <c r="L48" s="14"/>
+      <c r="L48" s="8"/>
       <c r="M48" s="17"/>
     </row>
     <row r="49" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2697,15 +2726,15 @@
       <c r="D49" s="14"/>
       <c r="E49" s="14"/>
       <c r="F49" s="15"/>
-      <c r="G49" s="16"/>
+      <c r="G49" s="18"/>
       <c r="H49" s="15">
         <f>(InventoryList!F49:F49*InventoryList!G49:G49)</f>
         <v>0</v>
       </c>
-      <c r="I49" s="16"/>
+      <c r="I49" s="24"/>
       <c r="J49" s="16"/>
       <c r="K49" s="16"/>
-      <c r="L49" s="14"/>
+      <c r="L49" s="8"/>
       <c r="M49" s="17"/>
     </row>
     <row r="50" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2717,15 +2746,15 @@
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="15"/>
-      <c r="G50" s="16"/>
+      <c r="G50" s="18"/>
       <c r="H50" s="15">
         <f>(InventoryList!F50:F50*InventoryList!G50:G50)</f>
         <v>0</v>
       </c>
-      <c r="I50" s="16"/>
+      <c r="I50" s="24"/>
       <c r="J50" s="16"/>
       <c r="K50" s="16"/>
-      <c r="L50" s="14"/>
+      <c r="L50" s="8"/>
       <c r="M50" s="17"/>
     </row>
     <row r="51" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2737,15 +2766,15 @@
       <c r="D51" s="14"/>
       <c r="E51" s="14"/>
       <c r="F51" s="15"/>
-      <c r="G51" s="16"/>
+      <c r="G51" s="18"/>
       <c r="H51" s="15">
         <f>(InventoryList!F51:F51*InventoryList!G51:G51)</f>
         <v>0</v>
       </c>
-      <c r="I51" s="16"/>
+      <c r="I51" s="24"/>
       <c r="J51" s="16"/>
       <c r="K51" s="16"/>
-      <c r="L51" s="14"/>
+      <c r="L51" s="8"/>
       <c r="M51" s="17"/>
     </row>
     <row r="52" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2757,15 +2786,15 @@
       <c r="D52" s="14"/>
       <c r="E52" s="14"/>
       <c r="F52" s="15"/>
-      <c r="G52" s="16"/>
+      <c r="G52" s="18"/>
       <c r="H52" s="15">
         <f>(InventoryList!F52:F52*InventoryList!G52:G52)</f>
         <v>0</v>
       </c>
-      <c r="I52" s="16"/>
+      <c r="I52" s="24"/>
       <c r="J52" s="16"/>
       <c r="K52" s="16"/>
-      <c r="L52" s="14"/>
+      <c r="L52" s="8"/>
       <c r="M52" s="17"/>
     </row>
     <row r="53" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2777,15 +2806,15 @@
       <c r="D53" s="14"/>
       <c r="E53" s="14"/>
       <c r="F53" s="15"/>
-      <c r="G53" s="16"/>
+      <c r="G53" s="18"/>
       <c r="H53" s="15">
         <f>(InventoryList!F53:F53*InventoryList!G53:G53)</f>
         <v>0</v>
       </c>
-      <c r="I53" s="16"/>
+      <c r="I53" s="24"/>
       <c r="J53" s="16"/>
       <c r="K53" s="16"/>
-      <c r="L53" s="14"/>
+      <c r="L53" s="8"/>
       <c r="M53" s="17"/>
     </row>
     <row r="54" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2797,15 +2826,15 @@
       <c r="D54" s="14"/>
       <c r="E54" s="14"/>
       <c r="F54" s="15"/>
-      <c r="G54" s="16"/>
+      <c r="G54" s="18"/>
       <c r="H54" s="15">
         <f>(InventoryList!F54:F54*InventoryList!G54:G54)</f>
         <v>0</v>
       </c>
-      <c r="I54" s="16"/>
+      <c r="I54" s="24"/>
       <c r="J54" s="16"/>
       <c r="K54" s="16"/>
-      <c r="L54" s="14"/>
+      <c r="L54" s="8"/>
       <c r="M54" s="17"/>
     </row>
     <row r="55" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2817,15 +2846,15 @@
       <c r="D55" s="14"/>
       <c r="E55" s="14"/>
       <c r="F55" s="15"/>
-      <c r="G55" s="16"/>
+      <c r="G55" s="18"/>
       <c r="H55" s="15">
         <f>(InventoryList!F55:F55*InventoryList!G55:G55)</f>
         <v>0</v>
       </c>
-      <c r="I55" s="16"/>
+      <c r="I55" s="24"/>
       <c r="J55" s="16"/>
       <c r="K55" s="16"/>
-      <c r="L55" s="14"/>
+      <c r="L55" s="8"/>
       <c r="M55" s="17"/>
     </row>
     <row r="56" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2837,15 +2866,15 @@
       <c r="D56" s="14"/>
       <c r="E56" s="14"/>
       <c r="F56" s="15"/>
-      <c r="G56" s="16"/>
+      <c r="G56" s="18"/>
       <c r="H56" s="15">
         <f>(InventoryList!F56:F56*InventoryList!G56:G56)</f>
         <v>0</v>
       </c>
-      <c r="I56" s="16"/>
+      <c r="I56" s="24"/>
       <c r="J56" s="16"/>
       <c r="K56" s="16"/>
-      <c r="L56" s="14"/>
+      <c r="L56" s="8"/>
       <c r="M56" s="17"/>
     </row>
     <row r="57" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2857,15 +2886,15 @@
       <c r="D57" s="14"/>
       <c r="E57" s="14"/>
       <c r="F57" s="15"/>
-      <c r="G57" s="16"/>
+      <c r="G57" s="18"/>
       <c r="H57" s="15">
         <f>(InventoryList!F57:F57*InventoryList!G57:G57)</f>
         <v>0</v>
       </c>
-      <c r="I57" s="16"/>
+      <c r="I57" s="24"/>
       <c r="J57" s="16"/>
       <c r="K57" s="16"/>
-      <c r="L57" s="14"/>
+      <c r="L57" s="8"/>
       <c r="M57" s="17"/>
     </row>
     <row r="58" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2877,15 +2906,15 @@
       <c r="D58" s="14"/>
       <c r="E58" s="14"/>
       <c r="F58" s="15"/>
-      <c r="G58" s="16"/>
+      <c r="G58" s="18"/>
       <c r="H58" s="15">
         <f>(InventoryList!F58:F58*InventoryList!G58:G58)</f>
         <v>0</v>
       </c>
-      <c r="I58" s="16"/>
+      <c r="I58" s="24"/>
       <c r="J58" s="16"/>
       <c r="K58" s="16"/>
-      <c r="L58" s="14"/>
+      <c r="L58" s="8"/>
       <c r="M58" s="17"/>
     </row>
     <row r="59" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2897,15 +2926,15 @@
       <c r="D59" s="14"/>
       <c r="E59" s="14"/>
       <c r="F59" s="15"/>
-      <c r="G59" s="16"/>
+      <c r="G59" s="18"/>
       <c r="H59" s="15">
         <f>(InventoryList!F59:F59*InventoryList!G59:G59)</f>
         <v>0</v>
       </c>
-      <c r="I59" s="16"/>
+      <c r="I59" s="24"/>
       <c r="J59" s="16"/>
       <c r="K59" s="16"/>
-      <c r="L59" s="14"/>
+      <c r="L59" s="8"/>
       <c r="M59" s="17"/>
     </row>
     <row r="60" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2917,15 +2946,15 @@
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
       <c r="F60" s="15"/>
-      <c r="G60" s="16"/>
+      <c r="G60" s="18"/>
       <c r="H60" s="15">
         <f>(InventoryList!F60:F60*InventoryList!G60:G60)</f>
         <v>0</v>
       </c>
-      <c r="I60" s="16"/>
+      <c r="I60" s="24"/>
       <c r="J60" s="16"/>
       <c r="K60" s="16"/>
-      <c r="L60" s="14"/>
+      <c r="L60" s="8"/>
       <c r="M60" s="17"/>
     </row>
     <row r="61" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2937,15 +2966,15 @@
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
       <c r="F61" s="15"/>
-      <c r="G61" s="16"/>
+      <c r="G61" s="18"/>
       <c r="H61" s="15">
         <f>(InventoryList!F61:F61*InventoryList!G61:G61)</f>
         <v>0</v>
       </c>
-      <c r="I61" s="16"/>
+      <c r="I61" s="24"/>
       <c r="J61" s="16"/>
       <c r="K61" s="16"/>
-      <c r="L61" s="14"/>
+      <c r="L61" s="8"/>
       <c r="M61" s="17"/>
     </row>
     <row r="62" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2957,15 +2986,15 @@
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
       <c r="F62" s="15"/>
-      <c r="G62" s="16"/>
+      <c r="G62" s="18"/>
       <c r="H62" s="15">
         <f>(InventoryList!F62:F62*InventoryList!G62:G62)</f>
         <v>0</v>
       </c>
-      <c r="I62" s="16"/>
+      <c r="I62" s="24"/>
       <c r="J62" s="16"/>
       <c r="K62" s="16"/>
-      <c r="L62" s="14"/>
+      <c r="L62" s="8"/>
       <c r="M62" s="17"/>
     </row>
     <row r="63" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2977,15 +3006,15 @@
       <c r="D63" s="14"/>
       <c r="E63" s="14"/>
       <c r="F63" s="15"/>
-      <c r="G63" s="16"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="15">
         <f>(InventoryList!F63:F63*InventoryList!G63:G63)</f>
         <v>0</v>
       </c>
-      <c r="I63" s="16"/>
+      <c r="I63" s="24"/>
       <c r="J63" s="16"/>
       <c r="K63" s="16"/>
-      <c r="L63" s="14"/>
+      <c r="L63" s="8"/>
       <c r="M63" s="17"/>
     </row>
     <row r="64" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2997,15 +3026,15 @@
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
       <c r="F64" s="15"/>
-      <c r="G64" s="16"/>
+      <c r="G64" s="18"/>
       <c r="H64" s="15">
         <f>(InventoryList!F64:F64*InventoryList!G64:G64)</f>
         <v>0</v>
       </c>
-      <c r="I64" s="16"/>
+      <c r="I64" s="24"/>
       <c r="J64" s="16"/>
       <c r="K64" s="16"/>
-      <c r="L64" s="14"/>
+      <c r="L64" s="8"/>
       <c r="M64" s="17"/>
     </row>
     <row r="65" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3017,15 +3046,15 @@
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
       <c r="F65" s="15"/>
-      <c r="G65" s="16"/>
+      <c r="G65" s="18"/>
       <c r="H65" s="15">
         <f>(InventoryList!F65:F65*InventoryList!G65:G65)</f>
         <v>0</v>
       </c>
-      <c r="I65" s="16"/>
+      <c r="I65" s="24"/>
       <c r="J65" s="16"/>
       <c r="K65" s="16"/>
-      <c r="L65" s="14"/>
+      <c r="L65" s="8"/>
       <c r="M65" s="17"/>
     </row>
     <row r="66" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3037,15 +3066,15 @@
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
       <c r="F66" s="15"/>
-      <c r="G66" s="16"/>
+      <c r="G66" s="18"/>
       <c r="H66" s="15">
         <f>(InventoryList!F66:F66*InventoryList!G66:G66)</f>
         <v>0</v>
       </c>
-      <c r="I66" s="16"/>
+      <c r="I66" s="24"/>
       <c r="J66" s="16"/>
       <c r="K66" s="16"/>
-      <c r="L66" s="14"/>
+      <c r="L66" s="8"/>
       <c r="M66" s="17"/>
     </row>
     <row r="67" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3057,15 +3086,15 @@
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
       <c r="F67" s="15"/>
-      <c r="G67" s="16"/>
+      <c r="G67" s="18"/>
       <c r="H67" s="15">
         <f>(InventoryList!F67:F67*InventoryList!G67:G67)</f>
         <v>0</v>
       </c>
-      <c r="I67" s="16"/>
+      <c r="I67" s="24"/>
       <c r="J67" s="16"/>
       <c r="K67" s="16"/>
-      <c r="L67" s="14"/>
+      <c r="L67" s="8"/>
       <c r="M67" s="17"/>
     </row>
     <row r="68" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3077,15 +3106,15 @@
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
       <c r="F68" s="15"/>
-      <c r="G68" s="16"/>
+      <c r="G68" s="18"/>
       <c r="H68" s="15">
         <f>(InventoryList!F68:F68*InventoryList!G68:G68)</f>
         <v>0</v>
       </c>
-      <c r="I68" s="16"/>
+      <c r="I68" s="24"/>
       <c r="J68" s="16"/>
       <c r="K68" s="16"/>
-      <c r="L68" s="14"/>
+      <c r="L68" s="8"/>
       <c r="M68" s="17"/>
     </row>
     <row r="69" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3097,15 +3126,15 @@
       <c r="D69" s="14"/>
       <c r="E69" s="14"/>
       <c r="F69" s="15"/>
-      <c r="G69" s="16"/>
+      <c r="G69" s="18"/>
       <c r="H69" s="15">
         <f>(InventoryList!F69:F69*InventoryList!G69:G69)</f>
         <v>0</v>
       </c>
-      <c r="I69" s="16"/>
+      <c r="I69" s="24"/>
       <c r="J69" s="16"/>
       <c r="K69" s="16"/>
-      <c r="L69" s="14"/>
+      <c r="L69" s="8"/>
       <c r="M69" s="17"/>
     </row>
     <row r="70" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3117,15 +3146,15 @@
       <c r="D70" s="14"/>
       <c r="E70" s="14"/>
       <c r="F70" s="15"/>
-      <c r="G70" s="16"/>
+      <c r="G70" s="18"/>
       <c r="H70" s="15">
         <f>(InventoryList!F70:F70*InventoryList!G70:G70)</f>
         <v>0</v>
       </c>
-      <c r="I70" s="16"/>
+      <c r="I70" s="24"/>
       <c r="J70" s="16"/>
       <c r="K70" s="16"/>
-      <c r="L70" s="14"/>
+      <c r="L70" s="8"/>
       <c r="M70" s="17"/>
     </row>
     <row r="71" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3137,15 +3166,15 @@
       <c r="D71" s="14"/>
       <c r="E71" s="14"/>
       <c r="F71" s="15"/>
-      <c r="G71" s="16"/>
+      <c r="G71" s="18"/>
       <c r="H71" s="15">
         <f>(InventoryList!F71:F71*InventoryList!G71:G71)</f>
         <v>0</v>
       </c>
-      <c r="I71" s="16"/>
+      <c r="I71" s="24"/>
       <c r="J71" s="16"/>
       <c r="K71" s="16"/>
-      <c r="L71" s="14"/>
+      <c r="L71" s="8"/>
       <c r="M71" s="17"/>
     </row>
     <row r="72" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3157,15 +3186,15 @@
       <c r="D72" s="14"/>
       <c r="E72" s="14"/>
       <c r="F72" s="15"/>
-      <c r="G72" s="16"/>
+      <c r="G72" s="18"/>
       <c r="H72" s="15">
         <f>(InventoryList!F72:F72*InventoryList!G72:G72)</f>
         <v>0</v>
       </c>
-      <c r="I72" s="16"/>
+      <c r="I72" s="24"/>
       <c r="J72" s="16"/>
       <c r="K72" s="16"/>
-      <c r="L72" s="14"/>
+      <c r="L72" s="8"/>
       <c r="M72" s="17"/>
     </row>
     <row r="73" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3177,15 +3206,15 @@
       <c r="D73" s="14"/>
       <c r="E73" s="14"/>
       <c r="F73" s="15"/>
-      <c r="G73" s="16"/>
+      <c r="G73" s="18"/>
       <c r="H73" s="15">
         <f>(InventoryList!F73:F73*InventoryList!G73:G73)</f>
         <v>0</v>
       </c>
-      <c r="I73" s="16"/>
+      <c r="I73" s="24"/>
       <c r="J73" s="16"/>
       <c r="K73" s="16"/>
-      <c r="L73" s="14"/>
+      <c r="L73" s="8"/>
       <c r="M73" s="17"/>
     </row>
     <row r="74" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3197,15 +3226,15 @@
       <c r="D74" s="14"/>
       <c r="E74" s="14"/>
       <c r="F74" s="15"/>
-      <c r="G74" s="16"/>
+      <c r="G74" s="18"/>
       <c r="H74" s="15">
         <f>(InventoryList!F74:F74*InventoryList!G74:G74)</f>
         <v>0</v>
       </c>
-      <c r="I74" s="16"/>
+      <c r="I74" s="24"/>
       <c r="J74" s="16"/>
       <c r="K74" s="16"/>
-      <c r="L74" s="14"/>
+      <c r="L74" s="8"/>
       <c r="M74" s="17"/>
     </row>
     <row r="75" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3217,15 +3246,15 @@
       <c r="D75" s="14"/>
       <c r="E75" s="14"/>
       <c r="F75" s="15"/>
-      <c r="G75" s="16"/>
+      <c r="G75" s="18"/>
       <c r="H75" s="15">
         <f>(InventoryList!F75:F75*InventoryList!G75:G75)</f>
         <v>0</v>
       </c>
-      <c r="I75" s="16"/>
+      <c r="I75" s="24"/>
       <c r="J75" s="16"/>
       <c r="K75" s="16"/>
-      <c r="L75" s="14"/>
+      <c r="L75" s="8"/>
       <c r="M75" s="17"/>
     </row>
     <row r="76" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3237,15 +3266,15 @@
       <c r="D76" s="14"/>
       <c r="E76" s="14"/>
       <c r="F76" s="15"/>
-      <c r="G76" s="16"/>
+      <c r="G76" s="18"/>
       <c r="H76" s="15">
         <f>(InventoryList!F76:F76*InventoryList!G76:G76)</f>
         <v>0</v>
       </c>
-      <c r="I76" s="16"/>
+      <c r="I76" s="24"/>
       <c r="J76" s="16"/>
       <c r="K76" s="16"/>
-      <c r="L76" s="14"/>
+      <c r="L76" s="8"/>
       <c r="M76" s="17"/>
     </row>
     <row r="77" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3257,15 +3286,15 @@
       <c r="D77" s="14"/>
       <c r="E77" s="14"/>
       <c r="F77" s="15"/>
-      <c r="G77" s="16"/>
+      <c r="G77" s="18"/>
       <c r="H77" s="15">
         <f>(InventoryList!F77:F77*InventoryList!G77:G77)</f>
         <v>0</v>
       </c>
-      <c r="I77" s="16"/>
+      <c r="I77" s="24"/>
       <c r="J77" s="16"/>
       <c r="K77" s="16"/>
-      <c r="L77" s="14"/>
+      <c r="L77" s="8"/>
       <c r="M77" s="17"/>
     </row>
     <row r="78" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3277,15 +3306,15 @@
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
       <c r="F78" s="15"/>
-      <c r="G78" s="16"/>
+      <c r="G78" s="18"/>
       <c r="H78" s="15">
         <f>(InventoryList!F78:F78*InventoryList!G78:G78)</f>
         <v>0</v>
       </c>
-      <c r="I78" s="16"/>
+      <c r="I78" s="24"/>
       <c r="J78" s="16"/>
       <c r="K78" s="16"/>
-      <c r="L78" s="14"/>
+      <c r="L78" s="8"/>
       <c r="M78" s="17"/>
     </row>
     <row r="79" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3297,15 +3326,15 @@
       <c r="D79" s="14"/>
       <c r="E79" s="14"/>
       <c r="F79" s="15"/>
-      <c r="G79" s="16"/>
+      <c r="G79" s="18"/>
       <c r="H79" s="15">
         <f>(InventoryList!F79:F79*InventoryList!G79:G79)</f>
         <v>0</v>
       </c>
-      <c r="I79" s="16"/>
+      <c r="I79" s="24"/>
       <c r="J79" s="16"/>
       <c r="K79" s="16"/>
-      <c r="L79" s="14"/>
+      <c r="L79" s="8"/>
       <c r="M79" s="17"/>
     </row>
     <row r="80" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3317,15 +3346,15 @@
       <c r="D80" s="14"/>
       <c r="E80" s="14"/>
       <c r="F80" s="15"/>
-      <c r="G80" s="16"/>
+      <c r="G80" s="18"/>
       <c r="H80" s="15">
         <f>(InventoryList!F80:F80*InventoryList!G80:G80)</f>
         <v>0</v>
       </c>
-      <c r="I80" s="16"/>
+      <c r="I80" s="24"/>
       <c r="J80" s="16"/>
       <c r="K80" s="16"/>
-      <c r="L80" s="14"/>
+      <c r="L80" s="8"/>
       <c r="M80" s="17"/>
     </row>
     <row r="81" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3337,15 +3366,15 @@
       <c r="D81" s="14"/>
       <c r="E81" s="14"/>
       <c r="F81" s="15"/>
-      <c r="G81" s="16"/>
+      <c r="G81" s="18"/>
       <c r="H81" s="15">
         <f>(InventoryList!F81:F81*InventoryList!G81:G81)</f>
         <v>0</v>
       </c>
-      <c r="I81" s="16"/>
+      <c r="I81" s="24"/>
       <c r="J81" s="16"/>
       <c r="K81" s="16"/>
-      <c r="L81" s="14"/>
+      <c r="L81" s="8"/>
       <c r="M81" s="17"/>
     </row>
     <row r="82" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3357,15 +3386,15 @@
       <c r="D82" s="14"/>
       <c r="E82" s="14"/>
       <c r="F82" s="15"/>
-      <c r="G82" s="16"/>
+      <c r="G82" s="18"/>
       <c r="H82" s="15">
         <f>(InventoryList!F82:F82*InventoryList!G82:G82)</f>
         <v>0</v>
       </c>
-      <c r="I82" s="16"/>
+      <c r="I82" s="24"/>
       <c r="J82" s="16"/>
       <c r="K82" s="16"/>
-      <c r="L82" s="14"/>
+      <c r="L82" s="8"/>
       <c r="M82" s="17"/>
     </row>
     <row r="83" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3377,15 +3406,15 @@
       <c r="D83" s="14"/>
       <c r="E83" s="14"/>
       <c r="F83" s="15"/>
-      <c r="G83" s="16"/>
+      <c r="G83" s="18"/>
       <c r="H83" s="15">
         <f>(InventoryList!F83:F83*InventoryList!G83:G83)</f>
         <v>0</v>
       </c>
-      <c r="I83" s="16"/>
+      <c r="I83" s="24"/>
       <c r="J83" s="16"/>
       <c r="K83" s="16"/>
-      <c r="L83" s="14"/>
+      <c r="L83" s="8"/>
       <c r="M83" s="17"/>
     </row>
     <row r="84" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3397,15 +3426,15 @@
       <c r="D84" s="14"/>
       <c r="E84" s="14"/>
       <c r="F84" s="15"/>
-      <c r="G84" s="16"/>
+      <c r="G84" s="18"/>
       <c r="H84" s="15">
         <f>(InventoryList!F84:F84*InventoryList!G84:G84)</f>
         <v>0</v>
       </c>
-      <c r="I84" s="16"/>
+      <c r="I84" s="24"/>
       <c r="J84" s="16"/>
       <c r="K84" s="16"/>
-      <c r="L84" s="14"/>
+      <c r="L84" s="8"/>
       <c r="M84" s="17"/>
     </row>
     <row r="85" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3417,15 +3446,15 @@
       <c r="D85" s="14"/>
       <c r="E85" s="14"/>
       <c r="F85" s="15"/>
-      <c r="G85" s="16"/>
+      <c r="G85" s="18"/>
       <c r="H85" s="15">
         <f>(InventoryList!F85:F85*InventoryList!G85:G85)</f>
         <v>0</v>
       </c>
-      <c r="I85" s="16"/>
+      <c r="I85" s="24"/>
       <c r="J85" s="16"/>
       <c r="K85" s="16"/>
-      <c r="L85" s="14"/>
+      <c r="L85" s="8"/>
       <c r="M85" s="17"/>
     </row>
     <row r="86" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3437,15 +3466,15 @@
       <c r="D86" s="14"/>
       <c r="E86" s="14"/>
       <c r="F86" s="15"/>
-      <c r="G86" s="16"/>
+      <c r="G86" s="18"/>
       <c r="H86" s="15">
         <f>(InventoryList!F86:F86*InventoryList!G86:G86)</f>
         <v>0</v>
       </c>
-      <c r="I86" s="16"/>
+      <c r="I86" s="24"/>
       <c r="J86" s="16"/>
       <c r="K86" s="16"/>
-      <c r="L86" s="14"/>
+      <c r="L86" s="8"/>
       <c r="M86" s="17"/>
     </row>
     <row r="87" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3457,15 +3486,15 @@
       <c r="D87" s="14"/>
       <c r="E87" s="14"/>
       <c r="F87" s="15"/>
-      <c r="G87" s="16"/>
+      <c r="G87" s="18"/>
       <c r="H87" s="15">
         <f>(InventoryList!F87:F87*InventoryList!G87:G87)</f>
         <v>0</v>
       </c>
-      <c r="I87" s="16"/>
+      <c r="I87" s="24"/>
       <c r="J87" s="16"/>
       <c r="K87" s="16"/>
-      <c r="L87" s="14"/>
+      <c r="L87" s="8"/>
       <c r="M87" s="17"/>
     </row>
     <row r="88" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3477,15 +3506,15 @@
       <c r="D88" s="14"/>
       <c r="E88" s="14"/>
       <c r="F88" s="15"/>
-      <c r="G88" s="16"/>
+      <c r="G88" s="18"/>
       <c r="H88" s="15">
         <f>(InventoryList!F88:F88*InventoryList!G88:G88)</f>
         <v>0</v>
       </c>
-      <c r="I88" s="16"/>
+      <c r="I88" s="24"/>
       <c r="J88" s="16"/>
       <c r="K88" s="16"/>
-      <c r="L88" s="14"/>
+      <c r="L88" s="8"/>
       <c r="M88" s="17"/>
     </row>
     <row r="89" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3497,15 +3526,15 @@
       <c r="D89" s="14"/>
       <c r="E89" s="14"/>
       <c r="F89" s="15"/>
-      <c r="G89" s="16"/>
+      <c r="G89" s="18"/>
       <c r="H89" s="15">
         <f>(InventoryList!F89:F89*InventoryList!G89:G89)</f>
         <v>0</v>
       </c>
-      <c r="I89" s="16"/>
+      <c r="I89" s="24"/>
       <c r="J89" s="16"/>
       <c r="K89" s="16"/>
-      <c r="L89" s="14"/>
+      <c r="L89" s="8"/>
       <c r="M89" s="17"/>
     </row>
     <row r="90" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3517,15 +3546,15 @@
       <c r="D90" s="14"/>
       <c r="E90" s="14"/>
       <c r="F90" s="15"/>
-      <c r="G90" s="16"/>
+      <c r="G90" s="18"/>
       <c r="H90" s="15">
         <f>(InventoryList!F90:F90*InventoryList!G90:G90)</f>
         <v>0</v>
       </c>
-      <c r="I90" s="16"/>
+      <c r="I90" s="24"/>
       <c r="J90" s="16"/>
       <c r="K90" s="16"/>
-      <c r="L90" s="14"/>
+      <c r="L90" s="8"/>
       <c r="M90" s="17"/>
     </row>
     <row r="91" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3537,15 +3566,15 @@
       <c r="D91" s="14"/>
       <c r="E91" s="14"/>
       <c r="F91" s="15"/>
-      <c r="G91" s="16"/>
+      <c r="G91" s="18"/>
       <c r="H91" s="15">
         <f>(InventoryList!F91:F91*InventoryList!G91:G91)</f>
         <v>0</v>
       </c>
-      <c r="I91" s="16"/>
+      <c r="I91" s="24"/>
       <c r="J91" s="16"/>
       <c r="K91" s="16"/>
-      <c r="L91" s="14"/>
+      <c r="L91" s="8"/>
       <c r="M91" s="17"/>
     </row>
     <row r="92" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3557,15 +3586,15 @@
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
       <c r="F92" s="15"/>
-      <c r="G92" s="16"/>
+      <c r="G92" s="18"/>
       <c r="H92" s="15">
         <f>(InventoryList!F92:F92*InventoryList!G92:G92)</f>
         <v>0</v>
       </c>
-      <c r="I92" s="16"/>
+      <c r="I92" s="24"/>
       <c r="J92" s="16"/>
       <c r="K92" s="16"/>
-      <c r="L92" s="14"/>
+      <c r="L92" s="8"/>
       <c r="M92" s="17"/>
     </row>
     <row r="93" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3577,15 +3606,15 @@
       <c r="D93" s="14"/>
       <c r="E93" s="14"/>
       <c r="F93" s="15"/>
-      <c r="G93" s="16"/>
+      <c r="G93" s="18"/>
       <c r="H93" s="15">
         <f>(InventoryList!F93:F93*InventoryList!G93:G93)</f>
         <v>0</v>
       </c>
-      <c r="I93" s="16"/>
+      <c r="I93" s="24"/>
       <c r="J93" s="16"/>
       <c r="K93" s="16"/>
-      <c r="L93" s="14"/>
+      <c r="L93" s="8"/>
       <c r="M93" s="17"/>
     </row>
     <row r="94" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3597,15 +3626,15 @@
       <c r="D94" s="14"/>
       <c r="E94" s="14"/>
       <c r="F94" s="15"/>
-      <c r="G94" s="16"/>
+      <c r="G94" s="18"/>
       <c r="H94" s="15">
         <f>(InventoryList!F94:F94*InventoryList!G94:G94)</f>
         <v>0</v>
       </c>
-      <c r="I94" s="16"/>
+      <c r="I94" s="24"/>
       <c r="J94" s="16"/>
       <c r="K94" s="16"/>
-      <c r="L94" s="14"/>
+      <c r="L94" s="8"/>
       <c r="M94" s="17"/>
     </row>
     <row r="95" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3617,15 +3646,15 @@
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
       <c r="F95" s="15"/>
-      <c r="G95" s="16"/>
+      <c r="G95" s="18"/>
       <c r="H95" s="15">
         <f>(InventoryList!F95:F95*InventoryList!G95:G95)</f>
         <v>0</v>
       </c>
-      <c r="I95" s="16"/>
+      <c r="I95" s="24"/>
       <c r="J95" s="16"/>
       <c r="K95" s="16"/>
-      <c r="L95" s="14"/>
+      <c r="L95" s="8"/>
       <c r="M95" s="17"/>
     </row>
     <row r="96" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3637,15 +3666,15 @@
       <c r="D96" s="14"/>
       <c r="E96" s="14"/>
       <c r="F96" s="15"/>
-      <c r="G96" s="16"/>
+      <c r="G96" s="18"/>
       <c r="H96" s="15">
         <f>(InventoryList!F96:F96*InventoryList!G96:G96)</f>
         <v>0</v>
       </c>
-      <c r="I96" s="16"/>
+      <c r="I96" s="24"/>
       <c r="J96" s="16"/>
       <c r="K96" s="16"/>
-      <c r="L96" s="14"/>
+      <c r="L96" s="8"/>
       <c r="M96" s="17"/>
     </row>
     <row r="97" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3657,15 +3686,15 @@
       <c r="D97" s="14"/>
       <c r="E97" s="14"/>
       <c r="F97" s="15"/>
-      <c r="G97" s="16"/>
+      <c r="G97" s="18"/>
       <c r="H97" s="15">
         <f>(InventoryList!F97:F97*InventoryList!G97:G97)</f>
         <v>0</v>
       </c>
-      <c r="I97" s="16"/>
+      <c r="I97" s="24"/>
       <c r="J97" s="16"/>
       <c r="K97" s="16"/>
-      <c r="L97" s="14"/>
+      <c r="L97" s="8"/>
       <c r="M97" s="17"/>
     </row>
     <row r="98" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3677,20 +3706,42 @@
       <c r="D98" s="14"/>
       <c r="E98" s="14"/>
       <c r="F98" s="15"/>
-      <c r="G98" s="16"/>
+      <c r="G98" s="18"/>
       <c r="H98" s="15">
         <f>(InventoryList!F98:F98*InventoryList!G98:G98)</f>
         <v>0</v>
       </c>
-      <c r="I98" s="16"/>
+      <c r="I98" s="24"/>
       <c r="J98" s="16"/>
       <c r="K98" s="16"/>
-      <c r="L98" s="14"/>
+      <c r="L98" s="8"/>
       <c r="M98" s="17"/>
+    </row>
+    <row r="99" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G99" s="18"/>
+      <c r="L99" s="8"/>
+    </row>
+    <row r="100" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G100" s="18"/>
+      <c r="L100" s="8"/>
+    </row>
+    <row r="101" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="19"/>
+      <c r="C101" s="20"/>
+      <c r="D101" s="20"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="21"/>
+      <c r="G101" s="22"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="22"/>
+      <c r="J101" s="22"/>
+      <c r="K101" s="22"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="23"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B4:M98">
+  <conditionalFormatting sqref="B4:M4 G5:G100 M6:M98 L6:L101 J6:K98 J5:M5 B5:F98 H5:I98">
     <cfRule type="expression" dxfId="27" priority="1">
       <formula>#REF!="Так"</formula>
     </cfRule>
@@ -3710,7 +3761,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці кількість кожного товару на складі" sqref="G3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці ціну за одиницю кожного товару" sqref="F3" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Введіть у цьому стовпці опис товару" sqref="E3" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L5" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L98" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>"Так"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Щоб почати виділення елементів перевпорядкування, виберіть «Так». Після цього в стовпці B з’являтиметься позначка, а весь відповідний рядок виділятиметься кольором у таблиці «Список запасів». Якщо вибрати «Ні», позначки та виділення повністю прибираються." sqref="L2" xr:uid="{00000000-0002-0000-0000-00000D000000}">
@@ -3744,7 +3795,7 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B4:B100</xm:sqref>
+          <xm:sqref>B4:B98</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3753,12 +3804,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3970,18 +4021,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4007,11 +4060,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
some fix + InventoryStatistics.java add async mathematical calculations
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -1759,8 +1759,8 @@
       <c r="F4" s="24">
         <v>1</v>
       </c>
-      <c r="G4" s="16">
-        <v>0</v>
+      <c r="G4" s="16" t="n">
+        <v>40.0</v>
       </c>
       <c r="H4" s="14">
         <f>(InventoryList!F4:F4*InventoryList!G4:G4)</f>
@@ -1772,7 +1772,9 @@
       <c r="J4" s="22">
         <v>3</v>
       </c>
-      <c r="K4" s="16"/>
+      <c r="K4" s="16" t="n">
+        <v>40.0</v>
+      </c>
       <c r="L4" s="23"/>
       <c r="M4" s="15" t="s">
         <v>17</v>
@@ -1833,8 +1835,8 @@
       <c r="F6" s="24">
         <v>1</v>
       </c>
-      <c r="G6" s="16">
-        <v>0</v>
+      <c r="G6" s="16" t="n">
+        <v>25.0</v>
       </c>
       <c r="H6" s="14">
         <f>(InventoryList!F6:F6*InventoryList!G6:G6)</f>
@@ -1846,7 +1848,9 @@
       <c r="J6" s="22">
         <v>1</v>
       </c>
-      <c r="K6" s="16"/>
+      <c r="K6" s="16" t="n">
+        <v>25.0</v>
+      </c>
       <c r="L6" s="23"/>
       <c r="M6" s="15" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
done mb need fix
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB356DD-B6A7-44F1-AE93-6CB0FD97A67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE44A4A5-40B3-40D0-8FB0-C7CDD96AB463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InventoryList" sheetId="1" r:id="rId1"/>
@@ -15,17 +15,28 @@
     <definedName name="valHighlight">IFERROR(IF(InventoryList!$L$2="Так", TRUE, FALSE),FALSE)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">InventoryList!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>Ідентифікатор товару</t>
   </si>
@@ -103,6 +114,84 @@
   </si>
   <si>
     <t>Gr3</t>
+  </si>
+  <si>
+    <t>Id0</t>
+  </si>
+  <si>
+    <t>item0</t>
+  </si>
+  <si>
+    <t>id1</t>
+  </si>
+  <si>
+    <t>item1</t>
+  </si>
+  <si>
+    <t>id2</t>
+  </si>
+  <si>
+    <t>item2</t>
+  </si>
+  <si>
+    <t>Sup3</t>
+  </si>
+  <si>
+    <t>id3</t>
+  </si>
+  <si>
+    <t>item3</t>
+  </si>
+  <si>
+    <t>Gr2</t>
+  </si>
+  <si>
+    <t>id4</t>
+  </si>
+  <si>
+    <t>item4</t>
+  </si>
+  <si>
+    <t>id5</t>
+  </si>
+  <si>
+    <t>item5</t>
+  </si>
+  <si>
+    <t>id6</t>
+  </si>
+  <si>
+    <t>item6</t>
+  </si>
+  <si>
+    <t>id7</t>
+  </si>
+  <si>
+    <t>item7</t>
+  </si>
+  <si>
+    <t>id8</t>
+  </si>
+  <si>
+    <t>item8</t>
+  </si>
+  <si>
+    <t>Gr11</t>
+  </si>
+  <si>
+    <t>Gr33</t>
+  </si>
+  <si>
+    <t>Supik1</t>
+  </si>
+  <si>
+    <t>Supik2</t>
+  </si>
+  <si>
+    <t>Gr11!</t>
+  </si>
+  <si>
+    <t>q1!</t>
   </si>
 </sst>
 </file>
@@ -704,53 +793,53 @@
     </xf>
   </cellXfs>
   <cellStyles count="47">
-    <cellStyle name="20% – колірна тема 1" xfId="24" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 2" xfId="28" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 3" xfId="32" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 4" xfId="36" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 5" xfId="40" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% – колірна тема 6" xfId="44" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 1" xfId="25" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 2" xfId="29" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 3" xfId="33" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 4" xfId="37" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 5" xfId="41" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% – колірна тема 6" xfId="45" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 1" xfId="26" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 2" xfId="30" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 3" xfId="34" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 4" xfId="38" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 5" xfId="42" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% – колірна тема 6" xfId="46" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Ввід" xfId="14" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Відсотковий" xfId="5" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Гарний" xfId="11" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Грошовий" xfId="3" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Грошовий [0]" xfId="4" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="20% — акцент1" xfId="24" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% — акцент2" xfId="28" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% — акцент3" xfId="32" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% — акцент4" xfId="36" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% — акцент5" xfId="40" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% — акцент6" xfId="44" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% — акцент1" xfId="25" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% — акцент2" xfId="29" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% — акцент3" xfId="33" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% — акцент4" xfId="37" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% — акцент5" xfId="41" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% — акцент6" xfId="45" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% — акцент1" xfId="26" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% — акцент2" xfId="30" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% — акцент3" xfId="34" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% — акцент4" xfId="38" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% — акцент5" xfId="42" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% — акцент6" xfId="46" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Акцент1" xfId="23" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Акцент2" xfId="27" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Акцент3" xfId="31" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Акцент4" xfId="35" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Акцент5" xfId="39" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Акцент6" xfId="43" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ввод " xfId="14" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Вывод" xfId="15" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Вычисление" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Денежный" xfId="3" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Денежный [0]" xfId="4" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Заголовок 1" xfId="7" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Заголовок 2" xfId="8" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Заголовок 3" xfId="9" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Заголовок 4" xfId="10" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Звичайний" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Зв'язана клітинка" xfId="17" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 1" xfId="23" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 2" xfId="27" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 3" xfId="31" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 4" xfId="35" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 5" xfId="39" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Колірна тема 6" xfId="43" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Контрольна клітинка" xfId="18" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Назва" xfId="6" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Нейтральний" xfId="13" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Обчислення" xfId="16" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Підсумок" xfId="22" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Поганий" xfId="12" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Примітка" xfId="20" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Результат" xfId="15" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Текст попередження" xfId="19" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Текст пояснення" xfId="21" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Фінансовий" xfId="1" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Фінансовий [0]" xfId="2" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Итог" xfId="22" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Контрольная ячейка" xfId="18" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Название" xfId="6" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Нейтральный" xfId="13" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Плохой" xfId="12" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Пояснение" xfId="21" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Примечание" xfId="20" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Процентный" xfId="5" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Связанная ячейка" xfId="17" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Текст предупреждения" xfId="19" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Финансовый" xfId="1" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Финансовый [0]" xfId="2" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Хороший" xfId="11" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="31">
     <dxf>
@@ -1646,30 +1735,30 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:M92"/>
+  <dimension ref="B1:M88"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.765625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.765625" style="4" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.53515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.765625" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="16.765625" style="6" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.07421875" style="8" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.3046875" style="8" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.4609375" style="8" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" style="8" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.84375" style="8" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.765625" style="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.765625" style="6" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.53515625" style="4" customWidth="1" collapsed="1"/>
-    <col min="14" max="16384" width="8.765625" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="1.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="11.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="6" width="12.77734375" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="6" width="16.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="8" width="13.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="8" width="12.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="8" width="11.44140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="8" width="15.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="8" width="11.88671875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="8" width="14.77734375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="6" width="12.77734375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="4" width="12.5546875" collapsed="true"/>
+    <col min="14" max="16384" style="4" width="8.77734375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" s="1" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
@@ -1681,7 +1770,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F2" s="4"/>
       <c r="G2" s="10"/>
       <c r="I2" s="10"/>
@@ -1693,7 +1782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:13" s="3" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:13" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>14</v>
       </c>
@@ -1731,105 +1820,103 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G4:G4)&lt;=_xlfn.SINGLE(InventoryList!I4:I4))*(_xlfn.SINGLE(InventoryList!L4:L4)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
+    <row r="4" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G4:G4)&lt;=_xlfn.SINGLE(InventoryList!I4:I4))*(_xlfn.SINGLE(InventoryList!L4:L4)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="F4" s="24">
         <v>1</v>
       </c>
       <c r="G4" s="16">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="H4" s="14">
         <f>(InventoryList!F4:F4*InventoryList!G4:G4)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I4" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4" s="16">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="L4" s="23"/>
-      <c r="M4" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G5:G5)&lt;=_xlfn.SINGLE(InventoryList!I5:I5))*(_xlfn.SINGLE(InventoryList!L5:L5)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
+      <c r="M4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G5:G5)&lt;=_xlfn.SINGLE(InventoryList!I5:I5))*(_xlfn.SINGLE(InventoryList!L5:L5)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="F5" s="24">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G5" s="16">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H5" s="14">
         <f>(InventoryList!F5:F5*InventoryList!G5:G5)</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="I5" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="22">
-        <v>3</v>
-      </c>
-      <c r="K5" s="16">
-        <v>222</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K5" s="16"/>
       <c r="L5" s="23"/>
-      <c r="M5" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G6:G6)&lt;=_xlfn.SINGLE(InventoryList!I6:I6))*(_xlfn.SINGLE(InventoryList!L6:L6)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+      <c r="M5" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G6:G6)&lt;=_xlfn.SINGLE(InventoryList!I6:I6))*(_xlfn.SINGLE(InventoryList!L6:L6)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F6" s="24">
         <v>1</v>
       </c>
       <c r="G6" s="16">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="H6" s="14">
         <f>(InventoryList!F6:F6*InventoryList!G6:G6)</f>
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I6" s="22">
         <v>1</v>
@@ -1837,24 +1924,22 @@
       <c r="J6" s="22">
         <v>1</v>
       </c>
-      <c r="K6" s="16">
-        <v>10</v>
-      </c>
+      <c r="K6" s="16"/>
       <c r="L6" s="23"/>
       <c r="M6" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G7:G7)&lt;=_xlfn.SINGLE(InventoryList!I7:I7))*(_xlfn.SINGLE(InventoryList!L7:L7)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G7:G7)&lt;=_xlfn.SINGLE(InventoryList!I7:I7))*(_xlfn.SINGLE(InventoryList!L7:L7)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>20</v>
@@ -1863,42 +1948,40 @@
         <v>1</v>
       </c>
       <c r="G7" s="16">
-        <v>182</v>
+        <v>0</v>
       </c>
       <c r="H7" s="14">
         <f>(InventoryList!F7:F7*InventoryList!G7:G7)</f>
-        <v>182</v>
+        <v>0</v>
       </c>
       <c r="I7" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="22">
-        <v>3</v>
-      </c>
-      <c r="K7" s="16">
-        <v>222</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K7" s="16"/>
       <c r="L7" s="23"/>
       <c r="M7" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G8:G8)&lt;=_xlfn.SINGLE(InventoryList!I8:I8))*(_xlfn.SINGLE(InventoryList!L8:L8)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G8:G8)&lt;=_xlfn.SINGLE(InventoryList!I8:I8))*(_xlfn.SINGLE(InventoryList!L8:L8)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F8" s="24">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G8" s="16">
         <v>0</v>
@@ -1908,7 +1991,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="22">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J8" s="22">
         <v>1</v>
@@ -1919,19 +2002,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G9:G9)&lt;=_xlfn.SINGLE(InventoryList!I9:I9))*(_xlfn.SINGLE(InventoryList!L9:L9)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G9:G9)&lt;=_xlfn.SINGLE(InventoryList!I9:I9))*(_xlfn.SINGLE(InventoryList!L9:L9)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="F9" s="24">
         <v>1</v>
@@ -1944,26 +2027,34 @@
         <v>0</v>
       </c>
       <c r="I9" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K9" s="16"/>
       <c r="L9" s="23"/>
       <c r="M9" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G10:G10)&lt;=_xlfn.SINGLE(InventoryList!I10:I10))*(_xlfn.SINGLE(InventoryList!L10:L10)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="24"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G10:G10)&lt;=_xlfn.SINGLE(InventoryList!I10:I10))*(_xlfn.SINGLE(InventoryList!L10:L10)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="24">
+        <v>1</v>
+      </c>
       <c r="G10" s="16">
         <v>0</v>
       </c>
@@ -1971,21 +2062,35 @@
         <f>(InventoryList!F10:F10*InventoryList!G10:G10)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
+      <c r="I10" s="22">
+        <v>1</v>
+      </c>
+      <c r="J10" s="22">
+        <v>1</v>
+      </c>
       <c r="K10" s="16"/>
       <c r="L10" s="23"/>
-      <c r="M10" s="15"/>
-    </row>
-    <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G11:G11)&lt;=_xlfn.SINGLE(InventoryList!I11:I11))*(_xlfn.SINGLE(InventoryList!L11:L11)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="24"/>
+      <c r="M10" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G11:G11)&lt;=_xlfn.SINGLE(InventoryList!I11:I11))*(_xlfn.SINGLE(InventoryList!L11:L11)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="24">
+        <v>1</v>
+      </c>
       <c r="G11" s="16">
         <v>0</v>
       </c>
@@ -1993,21 +2098,35 @@
         <f>(InventoryList!F11:F11*InventoryList!G11:G11)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="I11" s="22">
+        <v>1</v>
+      </c>
+      <c r="J11" s="22">
+        <v>1</v>
+      </c>
       <c r="K11" s="16"/>
       <c r="L11" s="23"/>
-      <c r="M11" s="15"/>
-    </row>
-    <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G12:G12)&lt;=_xlfn.SINGLE(InventoryList!I12:I12))*(_xlfn.SINGLE(InventoryList!L12:L12)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="24"/>
+      <c r="M11" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G12:G12)&lt;=_xlfn.SINGLE(InventoryList!I12:I12))*(_xlfn.SINGLE(InventoryList!L12:L12)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="24">
+        <v>1</v>
+      </c>
       <c r="G12" s="16">
         <v>0</v>
       </c>
@@ -2015,21 +2134,35 @@
         <f>(InventoryList!F12:F12*InventoryList!G12:G12)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
+      <c r="I12" s="22">
+        <v>1</v>
+      </c>
+      <c r="J12" s="22">
+        <v>1</v>
+      </c>
       <c r="K12" s="16"/>
       <c r="L12" s="23"/>
-      <c r="M12" s="15"/>
-    </row>
-    <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G13:G13)&lt;=_xlfn.SINGLE(InventoryList!I13:I13))*(_xlfn.SINGLE(InventoryList!L13:L13)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="24"/>
+      <c r="M12" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G13:G13)&lt;=_xlfn.SINGLE(InventoryList!I13:I13))*(_xlfn.SINGLE(InventoryList!L13:L13)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="24">
+        <v>1</v>
+      </c>
       <c r="G13" s="16">
         <v>0</v>
       </c>
@@ -2037,21 +2170,35 @@
         <f>(InventoryList!F13:F13*InventoryList!G13:G13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
+      <c r="I13" s="22">
+        <v>1</v>
+      </c>
+      <c r="J13" s="22">
+        <v>1</v>
+      </c>
       <c r="K13" s="16"/>
       <c r="L13" s="23"/>
-      <c r="M13" s="15"/>
-    </row>
-    <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G14:G14)&lt;=_xlfn.SINGLE(InventoryList!I14:I14))*(_xlfn.SINGLE(InventoryList!L14:L14)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="24"/>
+      <c r="M13" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G14:G14)&lt;=_xlfn.SINGLE(InventoryList!I14:I14))*(_xlfn.SINGLE(InventoryList!L14:L14)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="24">
+        <v>1</v>
+      </c>
       <c r="G14" s="16">
         <v>0</v>
       </c>
@@ -2059,16 +2206,22 @@
         <f>(InventoryList!F14:F14*InventoryList!G14:G14)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
+      <c r="I14" s="22">
+        <v>1</v>
+      </c>
+      <c r="J14" s="22">
+        <v>1</v>
+      </c>
       <c r="K14" s="16"/>
       <c r="L14" s="23"/>
-      <c r="M14" s="15"/>
-    </row>
-    <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G15:G15)&lt;=_xlfn.SINGLE(InventoryList!I15:I15))*(_xlfn.SINGLE(InventoryList!L15:L15)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+      <c r="M14" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G15:G15)&lt;=_xlfn.SINGLE(InventoryList!I15:I15))*(_xlfn.SINGLE(InventoryList!L15:L15)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -2087,10 +2240,10 @@
       <c r="L15" s="23"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G16:G16)&lt;=_xlfn.SINGLE(InventoryList!I16:I16))*(_xlfn.SINGLE(InventoryList!L16:L16)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G16:G16)&lt;=_xlfn.SINGLE(InventoryList!I16:I16))*(_xlfn.SINGLE(InventoryList!L16:L16)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="13"/>
@@ -2109,10 +2262,10 @@
       <c r="L16" s="23"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G17:G17)&lt;=_xlfn.SINGLE(InventoryList!I17:I17))*(_xlfn.SINGLE(InventoryList!L17:L17)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="17" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G17:G17)&lt;=_xlfn.SINGLE(InventoryList!I17:I17))*(_xlfn.SINGLE(InventoryList!L17:L17)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
@@ -2131,10 +2284,10 @@
       <c r="L17" s="23"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G18:G18)&lt;=_xlfn.SINGLE(InventoryList!I18:I18))*(_xlfn.SINGLE(InventoryList!L18:L18)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="18" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G18:G18)&lt;=_xlfn.SINGLE(InventoryList!I18:I18))*(_xlfn.SINGLE(InventoryList!L18:L18)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="13"/>
@@ -2153,10 +2306,10 @@
       <c r="L18" s="23"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G19:G19)&lt;=_xlfn.SINGLE(InventoryList!I19:I19))*(_xlfn.SINGLE(InventoryList!L19:L19)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="19" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G19:G19)&lt;=_xlfn.SINGLE(InventoryList!I19:I19))*(_xlfn.SINGLE(InventoryList!L19:L19)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -2175,10 +2328,10 @@
       <c r="L19" s="23"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G20:G20)&lt;=_xlfn.SINGLE(InventoryList!I20:I20))*(_xlfn.SINGLE(InventoryList!L20:L20)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="20" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G20:G20)&lt;=_xlfn.SINGLE(InventoryList!I20:I20))*(_xlfn.SINGLE(InventoryList!L20:L20)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2197,10 +2350,10 @@
       <c r="L20" s="23"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G21:G21)&lt;=_xlfn.SINGLE(InventoryList!I21:I21))*(_xlfn.SINGLE(InventoryList!L21:L21)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="21" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G21:G21)&lt;=_xlfn.SINGLE(InventoryList!I21:I21))*(_xlfn.SINGLE(InventoryList!L21:L21)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -2219,10 +2372,10 @@
       <c r="L21" s="23"/>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G22:G22)&lt;=_xlfn.SINGLE(InventoryList!I22:I22))*(_xlfn.SINGLE(InventoryList!L22:L22)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="22" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G22:G22)&lt;=_xlfn.SINGLE(InventoryList!I22:I22))*(_xlfn.SINGLE(InventoryList!L22:L22)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
@@ -2241,10 +2394,10 @@
       <c r="L22" s="23"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G23:G23)&lt;=_xlfn.SINGLE(InventoryList!I23:I23))*(_xlfn.SINGLE(InventoryList!L23:L23)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="23" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G23:G23)&lt;=_xlfn.SINGLE(InventoryList!I23:I23))*(_xlfn.SINGLE(InventoryList!L23:L23)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C23" s="13"/>
       <c r="D23" s="13"/>
@@ -2263,10 +2416,10 @@
       <c r="L23" s="23"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G24:G24)&lt;=_xlfn.SINGLE(InventoryList!I24:I24))*(_xlfn.SINGLE(InventoryList!L24:L24)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="24" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G24:G24)&lt;=_xlfn.SINGLE(InventoryList!I24:I24))*(_xlfn.SINGLE(InventoryList!L24:L24)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
@@ -2285,10 +2438,10 @@
       <c r="L24" s="23"/>
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G25:G25)&lt;=_xlfn.SINGLE(InventoryList!I25:I25))*(_xlfn.SINGLE(InventoryList!L25:L25)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="25" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G25:G25)&lt;=_xlfn.SINGLE(InventoryList!I25:I25))*(_xlfn.SINGLE(InventoryList!L25:L25)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="13"/>
@@ -2307,10 +2460,10 @@
       <c r="L25" s="23"/>
       <c r="M25" s="15"/>
     </row>
-    <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G26:G26)&lt;=_xlfn.SINGLE(InventoryList!I26:I26))*(_xlfn.SINGLE(InventoryList!L26:L26)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="26" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G26:G26)&lt;=_xlfn.SINGLE(InventoryList!I26:I26))*(_xlfn.SINGLE(InventoryList!L26:L26)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="13"/>
@@ -2329,10 +2482,10 @@
       <c r="L26" s="23"/>
       <c r="M26" s="15"/>
     </row>
-    <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G27:G27)&lt;=_xlfn.SINGLE(InventoryList!I27:I27))*(_xlfn.SINGLE(InventoryList!L27:L27)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="27" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G27:G27)&lt;=_xlfn.SINGLE(InventoryList!I27:I27))*(_xlfn.SINGLE(InventoryList!L27:L27)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="13"/>
@@ -2351,10 +2504,10 @@
       <c r="L27" s="23"/>
       <c r="M27" s="15"/>
     </row>
-    <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G28:G28)&lt;=_xlfn.SINGLE(InventoryList!I28:I28))*(_xlfn.SINGLE(InventoryList!L28:L28)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="28" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G28:G28)&lt;=_xlfn.SINGLE(InventoryList!I28:I28))*(_xlfn.SINGLE(InventoryList!L28:L28)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -2373,10 +2526,10 @@
       <c r="L28" s="23"/>
       <c r="M28" s="15"/>
     </row>
-    <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G29:G29)&lt;=_xlfn.SINGLE(InventoryList!I29:I29))*(_xlfn.SINGLE(InventoryList!L29:L29)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="29" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G29:G29)&lt;=_xlfn.SINGLE(InventoryList!I29:I29))*(_xlfn.SINGLE(InventoryList!L29:L29)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
@@ -2395,10 +2548,10 @@
       <c r="L29" s="23"/>
       <c r="M29" s="15"/>
     </row>
-    <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G30:G30)&lt;=_xlfn.SINGLE(InventoryList!I30:I30))*(_xlfn.SINGLE(InventoryList!L30:L30)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="30" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G30:G30)&lt;=_xlfn.SINGLE(InventoryList!I30:I30))*(_xlfn.SINGLE(InventoryList!L30:L30)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="13"/>
@@ -2417,10 +2570,10 @@
       <c r="L30" s="23"/>
       <c r="M30" s="15"/>
     </row>
-    <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G31:G31)&lt;=_xlfn.SINGLE(InventoryList!I31:I31))*(_xlfn.SINGLE(InventoryList!L31:L31)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="31" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G31:G31)&lt;=_xlfn.SINGLE(InventoryList!I31:I31))*(_xlfn.SINGLE(InventoryList!L31:L31)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
@@ -2439,10 +2592,10 @@
       <c r="L31" s="23"/>
       <c r="M31" s="15"/>
     </row>
-    <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G32:G32)&lt;=_xlfn.SINGLE(InventoryList!I32:I32))*(_xlfn.SINGLE(InventoryList!L32:L32)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="32" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G32:G32)&lt;=_xlfn.SINGLE(InventoryList!I32:I32))*(_xlfn.SINGLE(InventoryList!L32:L32)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -2461,10 +2614,10 @@
       <c r="L32" s="23"/>
       <c r="M32" s="15"/>
     </row>
-    <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G33:G33)&lt;=_xlfn.SINGLE(InventoryList!I33:I33))*(_xlfn.SINGLE(InventoryList!L33:L33)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="33" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G33:G33)&lt;=_xlfn.SINGLE(InventoryList!I33:I33))*(_xlfn.SINGLE(InventoryList!L33:L33)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
@@ -2483,10 +2636,10 @@
       <c r="L33" s="23"/>
       <c r="M33" s="15"/>
     </row>
-    <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G34:G34)&lt;=_xlfn.SINGLE(InventoryList!I34:I34))*(_xlfn.SINGLE(InventoryList!L34:L34)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="34" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G34:G34)&lt;=_xlfn.SINGLE(InventoryList!I34:I34))*(_xlfn.SINGLE(InventoryList!L34:L34)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2505,10 +2658,10 @@
       <c r="L34" s="23"/>
       <c r="M34" s="15"/>
     </row>
-    <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G35:G35)&lt;=_xlfn.SINGLE(InventoryList!I35:I35))*(_xlfn.SINGLE(InventoryList!L35:L35)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="35" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G35:G35)&lt;=_xlfn.SINGLE(InventoryList!I35:I35))*(_xlfn.SINGLE(InventoryList!L35:L35)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="13"/>
@@ -2527,10 +2680,10 @@
       <c r="L35" s="23"/>
       <c r="M35" s="15"/>
     </row>
-    <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G36:G36)&lt;=_xlfn.SINGLE(InventoryList!I36:I36))*(_xlfn.SINGLE(InventoryList!L36:L36)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="36" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G36:G36)&lt;=_xlfn.SINGLE(InventoryList!I36:I36))*(_xlfn.SINGLE(InventoryList!L36:L36)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
@@ -2549,10 +2702,10 @@
       <c r="L36" s="23"/>
       <c r="M36" s="15"/>
     </row>
-    <row r="37" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G37:G37)&lt;=_xlfn.SINGLE(InventoryList!I37:I37))*(_xlfn.SINGLE(InventoryList!L37:L37)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="37" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G37:G37)&lt;=_xlfn.SINGLE(InventoryList!I37:I37))*(_xlfn.SINGLE(InventoryList!L37:L37)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
@@ -2571,10 +2724,10 @@
       <c r="L37" s="23"/>
       <c r="M37" s="15"/>
     </row>
-    <row r="38" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G38:G38)&lt;=_xlfn.SINGLE(InventoryList!I38:I38))*(_xlfn.SINGLE(InventoryList!L38:L38)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="38" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G38:G38)&lt;=_xlfn.SINGLE(InventoryList!I38:I38))*(_xlfn.SINGLE(InventoryList!L38:L38)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -2593,10 +2746,10 @@
       <c r="L38" s="23"/>
       <c r="M38" s="15"/>
     </row>
-    <row r="39" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G39:G39)&lt;=_xlfn.SINGLE(InventoryList!I39:I39))*(_xlfn.SINGLE(InventoryList!L39:L39)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="39" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G39:G39)&lt;=_xlfn.SINGLE(InventoryList!I39:I39))*(_xlfn.SINGLE(InventoryList!L39:L39)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="13"/>
@@ -2615,10 +2768,10 @@
       <c r="L39" s="23"/>
       <c r="M39" s="15"/>
     </row>
-    <row r="40" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G40:G40)&lt;=_xlfn.SINGLE(InventoryList!I40:I40))*(_xlfn.SINGLE(InventoryList!L40:L40)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="40" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G40:G40)&lt;=_xlfn.SINGLE(InventoryList!I40:I40))*(_xlfn.SINGLE(InventoryList!L40:L40)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C40" s="13"/>
       <c r="D40" s="13"/>
@@ -2637,10 +2790,10 @@
       <c r="L40" s="23"/>
       <c r="M40" s="15"/>
     </row>
-    <row r="41" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G41:G41)&lt;=_xlfn.SINGLE(InventoryList!I41:I41))*(_xlfn.SINGLE(InventoryList!L41:L41)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="41" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G41:G41)&lt;=_xlfn.SINGLE(InventoryList!I41:I41))*(_xlfn.SINGLE(InventoryList!L41:L41)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C41" s="13"/>
       <c r="D41" s="13"/>
@@ -2659,10 +2812,10 @@
       <c r="L41" s="23"/>
       <c r="M41" s="15"/>
     </row>
-    <row r="42" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G42:G42)&lt;=_xlfn.SINGLE(InventoryList!I42:I42))*(_xlfn.SINGLE(InventoryList!L42:L42)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="42" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G42:G42)&lt;=_xlfn.SINGLE(InventoryList!I42:I42))*(_xlfn.SINGLE(InventoryList!L42:L42)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
@@ -2681,10 +2834,10 @@
       <c r="L42" s="23"/>
       <c r="M42" s="15"/>
     </row>
-    <row r="43" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G43:G43)&lt;=_xlfn.SINGLE(InventoryList!I43:I43))*(_xlfn.SINGLE(InventoryList!L43:L43)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="43" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G43:G43)&lt;=_xlfn.SINGLE(InventoryList!I43:I43))*(_xlfn.SINGLE(InventoryList!L43:L43)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -2703,10 +2856,10 @@
       <c r="L43" s="23"/>
       <c r="M43" s="15"/>
     </row>
-    <row r="44" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G44:G44)&lt;=_xlfn.SINGLE(InventoryList!I44:I44))*(_xlfn.SINGLE(InventoryList!L44:L44)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="44" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G44:G44)&lt;=_xlfn.SINGLE(InventoryList!I44:I44))*(_xlfn.SINGLE(InventoryList!L44:L44)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
@@ -2725,10 +2878,10 @@
       <c r="L44" s="23"/>
       <c r="M44" s="15"/>
     </row>
-    <row r="45" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G45:G45)&lt;=_xlfn.SINGLE(InventoryList!I45:I45))*(_xlfn.SINGLE(InventoryList!L45:L45)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="45" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G45:G45)&lt;=_xlfn.SINGLE(InventoryList!I45:I45))*(_xlfn.SINGLE(InventoryList!L45:L45)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
@@ -2747,10 +2900,10 @@
       <c r="L45" s="23"/>
       <c r="M45" s="15"/>
     </row>
-    <row r="46" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G46:G46)&lt;=_xlfn.SINGLE(InventoryList!I46:I46))*(_xlfn.SINGLE(InventoryList!L46:L46)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="46" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G46:G46)&lt;=_xlfn.SINGLE(InventoryList!I46:I46))*(_xlfn.SINGLE(InventoryList!L46:L46)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C46" s="13"/>
       <c r="D46" s="13"/>
@@ -2769,10 +2922,10 @@
       <c r="L46" s="23"/>
       <c r="M46" s="15"/>
     </row>
-    <row r="47" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G47:G47)&lt;=_xlfn.SINGLE(InventoryList!I47:I47))*(_xlfn.SINGLE(InventoryList!L47:L47)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="47" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G47:G47)&lt;=_xlfn.SINGLE(InventoryList!I47:I47))*(_xlfn.SINGLE(InventoryList!L47:L47)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
@@ -2791,10 +2944,10 @@
       <c r="L47" s="23"/>
       <c r="M47" s="15"/>
     </row>
-    <row r="48" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G48:G48)&lt;=_xlfn.SINGLE(InventoryList!I48:I48))*(_xlfn.SINGLE(InventoryList!L48:L48)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="48" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G48:G48)&lt;=_xlfn.SINGLE(InventoryList!I48:I48))*(_xlfn.SINGLE(InventoryList!L48:L48)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C48" s="13"/>
       <c r="D48" s="13"/>
@@ -2813,10 +2966,10 @@
       <c r="L48" s="23"/>
       <c r="M48" s="15"/>
     </row>
-    <row r="49" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G49:G49)&lt;=_xlfn.SINGLE(InventoryList!I49:I49))*(_xlfn.SINGLE(InventoryList!L49:L49)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="49" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G49:G49)&lt;=_xlfn.SINGLE(InventoryList!I49:I49))*(_xlfn.SINGLE(InventoryList!L49:L49)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C49" s="13"/>
       <c r="D49" s="13"/>
@@ -2835,10 +2988,10 @@
       <c r="L49" s="23"/>
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G50:G50)&lt;=_xlfn.SINGLE(InventoryList!I50:I50))*(_xlfn.SINGLE(InventoryList!L50:L50)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="50" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G50:G50)&lt;=_xlfn.SINGLE(InventoryList!I50:I50))*(_xlfn.SINGLE(InventoryList!L50:L50)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C50" s="13"/>
       <c r="D50" s="13"/>
@@ -2857,10 +3010,10 @@
       <c r="L50" s="23"/>
       <c r="M50" s="15"/>
     </row>
-    <row r="51" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G51:G51)&lt;=_xlfn.SINGLE(InventoryList!I51:I51))*(_xlfn.SINGLE(InventoryList!L51:L51)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="51" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G51:G51)&lt;=_xlfn.SINGLE(InventoryList!I51:I51))*(_xlfn.SINGLE(InventoryList!L51:L51)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="13"/>
@@ -2879,10 +3032,10 @@
       <c r="L51" s="23"/>
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G52:G52)&lt;=_xlfn.SINGLE(InventoryList!I52:I52))*(_xlfn.SINGLE(InventoryList!L52:L52)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="52" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G52:G52)&lt;=_xlfn.SINGLE(InventoryList!I52:I52))*(_xlfn.SINGLE(InventoryList!L52:L52)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C52" s="13"/>
       <c r="D52" s="13"/>
@@ -2901,10 +3054,10 @@
       <c r="L52" s="23"/>
       <c r="M52" s="15"/>
     </row>
-    <row r="53" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G53:G53)&lt;=_xlfn.SINGLE(InventoryList!I53:I53))*(_xlfn.SINGLE(InventoryList!L53:L53)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="53" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G53:G53)&lt;=_xlfn.SINGLE(InventoryList!I53:I53))*(_xlfn.SINGLE(InventoryList!L53:L53)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
@@ -2923,10 +3076,10 @@
       <c r="L53" s="23"/>
       <c r="M53" s="15"/>
     </row>
-    <row r="54" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G54:G54)&lt;=_xlfn.SINGLE(InventoryList!I54:I54))*(_xlfn.SINGLE(InventoryList!L54:L54)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="54" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G54:G54)&lt;=_xlfn.SINGLE(InventoryList!I54:I54))*(_xlfn.SINGLE(InventoryList!L54:L54)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
@@ -2945,10 +3098,10 @@
       <c r="L54" s="23"/>
       <c r="M54" s="15"/>
     </row>
-    <row r="55" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G55:G55)&lt;=_xlfn.SINGLE(InventoryList!I55:I55))*(_xlfn.SINGLE(InventoryList!L55:L55)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="55" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G55:G55)&lt;=_xlfn.SINGLE(InventoryList!I55:I55))*(_xlfn.SINGLE(InventoryList!L55:L55)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
@@ -2967,10 +3120,10 @@
       <c r="L55" s="23"/>
       <c r="M55" s="15"/>
     </row>
-    <row r="56" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G56:G56)&lt;=_xlfn.SINGLE(InventoryList!I56:I56))*(_xlfn.SINGLE(InventoryList!L56:L56)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="56" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G56:G56)&lt;=_xlfn.SINGLE(InventoryList!I56:I56))*(_xlfn.SINGLE(InventoryList!L56:L56)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="13"/>
@@ -2989,10 +3142,10 @@
       <c r="L56" s="23"/>
       <c r="M56" s="15"/>
     </row>
-    <row r="57" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G57:G57)&lt;=_xlfn.SINGLE(InventoryList!I57:I57))*(_xlfn.SINGLE(InventoryList!L57:L57)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="57" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G57:G57)&lt;=_xlfn.SINGLE(InventoryList!I57:I57))*(_xlfn.SINGLE(InventoryList!L57:L57)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="13"/>
@@ -3011,10 +3164,10 @@
       <c r="L57" s="23"/>
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G58:G58)&lt;=_xlfn.SINGLE(InventoryList!I58:I58))*(_xlfn.SINGLE(InventoryList!L58:L58)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="58" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G58:G58)&lt;=_xlfn.SINGLE(InventoryList!I58:I58))*(_xlfn.SINGLE(InventoryList!L58:L58)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="13"/>
@@ -3033,10 +3186,10 @@
       <c r="L58" s="23"/>
       <c r="M58" s="15"/>
     </row>
-    <row r="59" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G59:G59)&lt;=_xlfn.SINGLE(InventoryList!I59:I59))*(_xlfn.SINGLE(InventoryList!L59:L59)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="59" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G59:G59)&lt;=_xlfn.SINGLE(InventoryList!I59:I59))*(_xlfn.SINGLE(InventoryList!L59:L59)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C59" s="13"/>
       <c r="D59" s="13"/>
@@ -3055,10 +3208,10 @@
       <c r="L59" s="23"/>
       <c r="M59" s="15"/>
     </row>
-    <row r="60" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B60" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G60:G60)&lt;=_xlfn.SINGLE(InventoryList!I60:I60))*(_xlfn.SINGLE(InventoryList!L60:L60)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="60" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G60:G60)&lt;=_xlfn.SINGLE(InventoryList!I60:I60))*(_xlfn.SINGLE(InventoryList!L60:L60)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
@@ -3077,10 +3230,10 @@
       <c r="L60" s="23"/>
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G61:G61)&lt;=_xlfn.SINGLE(InventoryList!I61:I61))*(_xlfn.SINGLE(InventoryList!L61:L61)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="61" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G61:G61)&lt;=_xlfn.SINGLE(InventoryList!I61:I61))*(_xlfn.SINGLE(InventoryList!L61:L61)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="13"/>
@@ -3099,10 +3252,10 @@
       <c r="L61" s="23"/>
       <c r="M61" s="15"/>
     </row>
-    <row r="62" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G62:G62)&lt;=_xlfn.SINGLE(InventoryList!I62:I62))*(_xlfn.SINGLE(InventoryList!L62:L62)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="62" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G62:G62)&lt;=_xlfn.SINGLE(InventoryList!I62:I62))*(_xlfn.SINGLE(InventoryList!L62:L62)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C62" s="13"/>
       <c r="D62" s="13"/>
@@ -3121,10 +3274,10 @@
       <c r="L62" s="23"/>
       <c r="M62" s="15"/>
     </row>
-    <row r="63" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G63:G63)&lt;=_xlfn.SINGLE(InventoryList!I63:I63))*(_xlfn.SINGLE(InventoryList!L63:L63)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="63" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G63:G63)&lt;=_xlfn.SINGLE(InventoryList!I63:I63))*(_xlfn.SINGLE(InventoryList!L63:L63)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C63" s="13"/>
       <c r="D63" s="13"/>
@@ -3143,10 +3296,10 @@
       <c r="L63" s="23"/>
       <c r="M63" s="15"/>
     </row>
-    <row r="64" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G64:G64)&lt;=_xlfn.SINGLE(InventoryList!I64:I64))*(_xlfn.SINGLE(InventoryList!L64:L64)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="64" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G64:G64)&lt;=_xlfn.SINGLE(InventoryList!I64:I64))*(_xlfn.SINGLE(InventoryList!L64:L64)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C64" s="13"/>
       <c r="D64" s="13"/>
@@ -3165,10 +3318,10 @@
       <c r="L64" s="23"/>
       <c r="M64" s="15"/>
     </row>
-    <row r="65" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B65" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G65:G65)&lt;=_xlfn.SINGLE(InventoryList!I65:I65))*(_xlfn.SINGLE(InventoryList!L65:L65)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="65" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G65:G65)&lt;=_xlfn.SINGLE(InventoryList!I65:I65))*(_xlfn.SINGLE(InventoryList!L65:L65)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C65" s="13"/>
       <c r="D65" s="13"/>
@@ -3187,10 +3340,10 @@
       <c r="L65" s="23"/>
       <c r="M65" s="15"/>
     </row>
-    <row r="66" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G66:G66)&lt;=_xlfn.SINGLE(InventoryList!I66:I66))*(_xlfn.SINGLE(InventoryList!L66:L66)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="66" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G66:G66)&lt;=_xlfn.SINGLE(InventoryList!I66:I66))*(_xlfn.SINGLE(InventoryList!L66:L66)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C66" s="13"/>
       <c r="D66" s="13"/>
@@ -3209,10 +3362,10 @@
       <c r="L66" s="23"/>
       <c r="M66" s="15"/>
     </row>
-    <row r="67" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G67:G67)&lt;=_xlfn.SINGLE(InventoryList!I67:I67))*(_xlfn.SINGLE(InventoryList!L67:L67)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="67" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G67:G67)&lt;=_xlfn.SINGLE(InventoryList!I67:I67))*(_xlfn.SINGLE(InventoryList!L67:L67)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="13"/>
@@ -3231,10 +3384,10 @@
       <c r="L67" s="23"/>
       <c r="M67" s="15"/>
     </row>
-    <row r="68" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G68:G68)&lt;=_xlfn.SINGLE(InventoryList!I68:I68))*(_xlfn.SINGLE(InventoryList!L68:L68)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="68" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G68:G68)&lt;=_xlfn.SINGLE(InventoryList!I68:I68))*(_xlfn.SINGLE(InventoryList!L68:L68)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="13"/>
@@ -3253,10 +3406,10 @@
       <c r="L68" s="23"/>
       <c r="M68" s="15"/>
     </row>
-    <row r="69" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B69" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G69:G69)&lt;=_xlfn.SINGLE(InventoryList!I69:I69))*(_xlfn.SINGLE(InventoryList!L69:L69)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="69" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G69:G69)&lt;=_xlfn.SINGLE(InventoryList!I69:I69))*(_xlfn.SINGLE(InventoryList!L69:L69)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="13"/>
@@ -3275,10 +3428,10 @@
       <c r="L69" s="23"/>
       <c r="M69" s="15"/>
     </row>
-    <row r="70" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B70" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G70:G70)&lt;=_xlfn.SINGLE(InventoryList!I70:I70))*(_xlfn.SINGLE(InventoryList!L70:L70)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="70" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G70:G70)&lt;=_xlfn.SINGLE(InventoryList!I70:I70))*(_xlfn.SINGLE(InventoryList!L70:L70)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C70" s="13"/>
       <c r="D70" s="13"/>
@@ -3297,10 +3450,10 @@
       <c r="L70" s="23"/>
       <c r="M70" s="15"/>
     </row>
-    <row r="71" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G71:G71)&lt;=_xlfn.SINGLE(InventoryList!I71:I71))*(_xlfn.SINGLE(InventoryList!L71:L71)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="71" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G71:G71)&lt;=_xlfn.SINGLE(InventoryList!I71:I71))*(_xlfn.SINGLE(InventoryList!L71:L71)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13"/>
@@ -3319,10 +3472,10 @@
       <c r="L71" s="23"/>
       <c r="M71" s="15"/>
     </row>
-    <row r="72" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G72:G72)&lt;=_xlfn.SINGLE(InventoryList!I72:I72))*(_xlfn.SINGLE(InventoryList!L72:L72)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="72" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G72:G72)&lt;=_xlfn.SINGLE(InventoryList!I72:I72))*(_xlfn.SINGLE(InventoryList!L72:L72)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C72" s="13"/>
       <c r="D72" s="13"/>
@@ -3341,10 +3494,10 @@
       <c r="L72" s="23"/>
       <c r="M72" s="15"/>
     </row>
-    <row r="73" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B73" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G73:G73)&lt;=_xlfn.SINGLE(InventoryList!I73:I73))*(_xlfn.SINGLE(InventoryList!L73:L73)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="73" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G73:G73)&lt;=_xlfn.SINGLE(InventoryList!I73:I73))*(_xlfn.SINGLE(InventoryList!L73:L73)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C73" s="13"/>
       <c r="D73" s="13"/>
@@ -3363,10 +3516,10 @@
       <c r="L73" s="23"/>
       <c r="M73" s="15"/>
     </row>
-    <row r="74" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G74:G74)&lt;=_xlfn.SINGLE(InventoryList!I74:I74))*(_xlfn.SINGLE(InventoryList!L74:L74)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="74" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G74:G74)&lt;=_xlfn.SINGLE(InventoryList!I74:I74))*(_xlfn.SINGLE(InventoryList!L74:L74)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C74" s="13"/>
       <c r="D74" s="13"/>
@@ -3385,10 +3538,10 @@
       <c r="L74" s="23"/>
       <c r="M74" s="15"/>
     </row>
-    <row r="75" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B75" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G75:G75)&lt;=_xlfn.SINGLE(InventoryList!I75:I75))*(_xlfn.SINGLE(InventoryList!L75:L75)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="75" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G75:G75)&lt;=_xlfn.SINGLE(InventoryList!I75:I75))*(_xlfn.SINGLE(InventoryList!L75:L75)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C75" s="13"/>
       <c r="D75" s="13"/>
@@ -3407,10 +3560,10 @@
       <c r="L75" s="23"/>
       <c r="M75" s="15"/>
     </row>
-    <row r="76" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B76" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G76:G76)&lt;=_xlfn.SINGLE(InventoryList!I76:I76))*(_xlfn.SINGLE(InventoryList!L76:L76)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="76" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G76:G76)&lt;=_xlfn.SINGLE(InventoryList!I76:I76))*(_xlfn.SINGLE(InventoryList!L76:L76)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C76" s="13"/>
       <c r="D76" s="13"/>
@@ -3429,10 +3582,10 @@
       <c r="L76" s="23"/>
       <c r="M76" s="15"/>
     </row>
-    <row r="77" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B77" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G77:G77)&lt;=_xlfn.SINGLE(InventoryList!I77:I77))*(_xlfn.SINGLE(InventoryList!L77:L77)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="77" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G77:G77)&lt;=_xlfn.SINGLE(InventoryList!I77:I77))*(_xlfn.SINGLE(InventoryList!L77:L77)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
@@ -3451,10 +3604,10 @@
       <c r="L77" s="23"/>
       <c r="M77" s="15"/>
     </row>
-    <row r="78" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B78" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G78:G78)&lt;=_xlfn.SINGLE(InventoryList!I78:I78))*(_xlfn.SINGLE(InventoryList!L78:L78)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="78" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G78:G78)&lt;=_xlfn.SINGLE(InventoryList!I78:I78))*(_xlfn.SINGLE(InventoryList!L78:L78)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C78" s="13"/>
       <c r="D78" s="13"/>
@@ -3473,10 +3626,10 @@
       <c r="L78" s="23"/>
       <c r="M78" s="15"/>
     </row>
-    <row r="79" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B79" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G79:G79)&lt;=_xlfn.SINGLE(InventoryList!I79:I79))*(_xlfn.SINGLE(InventoryList!L79:L79)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="79" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G79:G79)&lt;=_xlfn.SINGLE(InventoryList!I79:I79))*(_xlfn.SINGLE(InventoryList!L79:L79)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C79" s="13"/>
       <c r="D79" s="13"/>
@@ -3495,10 +3648,10 @@
       <c r="L79" s="23"/>
       <c r="M79" s="15"/>
     </row>
-    <row r="80" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B80" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G80:G80)&lt;=_xlfn.SINGLE(InventoryList!I80:I80))*(_xlfn.SINGLE(InventoryList!L80:L80)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="80" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G80:G80)&lt;=_xlfn.SINGLE(InventoryList!I80:I80))*(_xlfn.SINGLE(InventoryList!L80:L80)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C80" s="13"/>
       <c r="D80" s="13"/>
@@ -3517,10 +3670,10 @@
       <c r="L80" s="23"/>
       <c r="M80" s="15"/>
     </row>
-    <row r="81" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B81" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G81:G81)&lt;=_xlfn.SINGLE(InventoryList!I81:I81))*(_xlfn.SINGLE(InventoryList!L81:L81)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="81" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G81:G81)&lt;=_xlfn.SINGLE(InventoryList!I81:I81))*(_xlfn.SINGLE(InventoryList!L81:L81)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C81" s="13"/>
       <c r="D81" s="13"/>
@@ -3539,10 +3692,10 @@
       <c r="L81" s="23"/>
       <c r="M81" s="15"/>
     </row>
-    <row r="82" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B82" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G82:G82)&lt;=_xlfn.SINGLE(InventoryList!I82:I82))*(_xlfn.SINGLE(InventoryList!L82:L82)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="82" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B82" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G82:G82)&lt;=_xlfn.SINGLE(InventoryList!I82:I82))*(_xlfn.SINGLE(InventoryList!L82:L82)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>
@@ -3561,10 +3714,10 @@
       <c r="L82" s="23"/>
       <c r="M82" s="15"/>
     </row>
-    <row r="83" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B83" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G83:G83)&lt;=_xlfn.SINGLE(InventoryList!I83:I83))*(_xlfn.SINGLE(InventoryList!L83:L83)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="83" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G83:G83)&lt;=_xlfn.SINGLE(InventoryList!I83:I83))*(_xlfn.SINGLE(InventoryList!L83:L83)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C83" s="13"/>
       <c r="D83" s="13"/>
@@ -3583,10 +3736,10 @@
       <c r="L83" s="23"/>
       <c r="M83" s="15"/>
     </row>
-    <row r="84" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B84" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G84:G84)&lt;=_xlfn.SINGLE(InventoryList!I84:I84))*(_xlfn.SINGLE(InventoryList!L84:L84)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="84" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G84:G84)&lt;=_xlfn.SINGLE(InventoryList!I84:I84))*(_xlfn.SINGLE(InventoryList!L84:L84)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C84" s="13"/>
       <c r="D84" s="13"/>
@@ -3605,10 +3758,10 @@
       <c r="L84" s="23"/>
       <c r="M84" s="15"/>
     </row>
-    <row r="85" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B85" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G85:G85)&lt;=_xlfn.SINGLE(InventoryList!I85:I85))*(_xlfn.SINGLE(InventoryList!L85:L85)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
+    <row r="85" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G85:G85)&lt;=_xlfn.SINGLE(InventoryList!I85:I85))*(_xlfn.SINGLE(InventoryList!L85:L85)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
       </c>
       <c r="C85" s="13"/>
       <c r="D85" s="13"/>
@@ -3627,15 +3780,11 @@
       <c r="L85" s="23"/>
       <c r="M85" s="15"/>
     </row>
-    <row r="86" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B86" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G86:G86)&lt;=_xlfn.SINGLE(InventoryList!I86:I86))*(_xlfn.SINGLE(InventoryList!L86:L86)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="24"/>
+    <row r="86" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G86:G86)&lt;=_xlfn.SINGLE(InventoryList!I86:I86))*(_xlfn.SINGLE(InventoryList!L86:L86)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
       <c r="G86" s="16">
         <v>0</v>
       </c>
@@ -3643,21 +3792,13 @@
         <f>(InventoryList!F86:F86*InventoryList!G86:G86)</f>
         <v>0</v>
       </c>
-      <c r="I86" s="22"/>
-      <c r="J86" s="22"/>
-      <c r="K86" s="16"/>
-      <c r="L86" s="23"/>
-      <c r="M86" s="15"/>
-    </row>
-    <row r="87" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B87" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G87:G87)&lt;=_xlfn.SINGLE(InventoryList!I87:I87))*(_xlfn.SINGLE(InventoryList!L87:L87)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="24"/>
+      <c r="L86" s="8"/>
+    </row>
+    <row r="87" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="12">
+        <f>_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G87:G87)&lt;=_xlfn.SINGLE(InventoryList!I87:I87))*(_xlfn.SINGLE(InventoryList!L87:L87)="")*_xlfn.SINGLE(valHighlight),0))</f>
+        <v>1</v>
+      </c>
       <c r="G87" s="16">
         <v>0</v>
       </c>
@@ -3665,101 +3806,25 @@
         <f>(InventoryList!F87:F87*InventoryList!G87:G87)</f>
         <v>0</v>
       </c>
-      <c r="I87" s="22"/>
-      <c r="J87" s="22"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="23"/>
-      <c r="M87" s="15"/>
-    </row>
-    <row r="88" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B88" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G88:G88)&lt;=_xlfn.SINGLE(InventoryList!I88:I88))*(_xlfn.SINGLE(InventoryList!L88:L88)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="16">
-        <v>0</v>
-      </c>
-      <c r="H88" s="14">
-        <f>(InventoryList!F88:F88*InventoryList!G88:G88)</f>
-        <v>0</v>
-      </c>
-      <c r="I88" s="22"/>
-      <c r="J88" s="22"/>
-      <c r="K88" s="16"/>
-      <c r="L88" s="23"/>
-      <c r="M88" s="15"/>
-    </row>
-    <row r="89" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B89" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G89:G89)&lt;=_xlfn.SINGLE(InventoryList!I89:I89))*(_xlfn.SINGLE(InventoryList!L89:L89)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="24"/>
-      <c r="G89" s="16">
-        <v>0</v>
-      </c>
-      <c r="H89" s="14">
-        <f>(InventoryList!F89:F89*InventoryList!G89:G89)</f>
-        <v>0</v>
-      </c>
-      <c r="I89" s="22"/>
-      <c r="J89" s="22"/>
-      <c r="K89" s="16"/>
-      <c r="L89" s="23"/>
-      <c r="M89" s="15"/>
-    </row>
-    <row r="90" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B90" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G90:G90)&lt;=_xlfn.SINGLE(InventoryList!I90:I90))*(_xlfn.SINGLE(InventoryList!L90:L90)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G90" s="16">
-        <v>0</v>
-      </c>
-      <c r="H90" s="14">
-        <f>(InventoryList!F90:F90*InventoryList!G90:G90)</f>
-        <v>0</v>
-      </c>
-      <c r="L90" s="8"/>
-    </row>
-    <row r="91" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B91" s="12" t="e">
-        <f ca="1">_xlfn.SINGLE(IFERROR((_xlfn.SINGLE(InventoryList!G91:G91)&lt;=_xlfn.SINGLE(InventoryList!I91:I91))*(_xlfn.SINGLE(InventoryList!L91:L91)="")*_xlfn.SINGLE(valHighlight),0))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G91" s="16">
-        <v>0</v>
-      </c>
-      <c r="H91" s="14">
-        <f>(InventoryList!F91:F91*InventoryList!G91:G91)</f>
-        <v>0</v>
-      </c>
-      <c r="L91" s="8"/>
-    </row>
-    <row r="92" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B92" s="17"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="19"/>
-      <c r="G92" s="20"/>
-      <c r="H92" s="19"/>
-      <c r="I92" s="20"/>
-      <c r="J92" s="20"/>
-      <c r="K92" s="20"/>
-      <c r="L92" s="8"/>
-      <c r="M92" s="21"/>
+      <c r="L87" s="8"/>
+    </row>
+    <row r="88" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="17"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="18"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="19"/>
+      <c r="I88" s="20"/>
+      <c r="J88" s="20"/>
+      <c r="K88" s="20"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
-  <conditionalFormatting sqref="B4:F89 H4:M89 G4:G91 B90:B91 H90:H91 L90:L92">
+  <conditionalFormatting sqref="B4:F85 G4:G87 B86:B87 H86:H87 L86:L88 H4:M85">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>#REF!="Так"</formula>
     </cfRule>
@@ -3822,12 +3887,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4039,20 +4104,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4078,9 +4141,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
bug fix + javadocs + NumericFilter into a separate class
</commit_message>
<xml_diff>
--- a/src/com/automatedworkspace/files/Inventory.xlsx
+++ b/src/com/automatedworkspace/files/Inventory.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>Ідентифікатор товару</t>
   </si>
@@ -1906,7 +1906,7 @@
         <v>27</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F6" s="24">
         <v>1</v>
@@ -2014,7 +2014,7 @@
         <v>34</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F9" s="24">
         <v>1</v>
@@ -2122,7 +2122,7 @@
         <v>41</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="F12" s="24">
         <v>1</v>

</xml_diff>